<commit_message>
switched the region_id and site_group_name columns for convention
</commit_message>
<xml_diff>
--- a/backend/internal/seed/seed_data/mst_dummy_data.xlsx
+++ b/backend/internal/seed/seed_data/mst_dummy_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Uni\Intern SM\Stock Opname App [SOSMIT]\SOSMIT\backend\internal\seed\seed_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC88D971-8270-41E7-BF2F-CC8A44485B5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E6003C4-6164-4968-9583-0FEA4F9215E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10540" activeTab="5" xr2:uid="{AF28B77B-5B1D-47C2-ADE5-ADF50DA09BCF}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10540" activeTab="1" xr2:uid="{AF28B77B-5B1D-47C2-ADE5-ADF50DA09BCF}"/>
   </bookViews>
   <sheets>
     <sheet name="Region" sheetId="1" r:id="rId1"/>
@@ -1835,13 +1835,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F51990CE-FF2C-48E9-82E1-2E87B3A6C16A}">
   <dimension ref="A1:C82"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="3" max="3" width="24.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -1849,901 +1849,901 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>54</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="4">
         <v>1</v>
       </c>
-      <c r="B2" s="4">
+      <c r="B2" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C2" s="4">
         <v>1</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="4">
         <v>2</v>
       </c>
-      <c r="B3" s="4">
+      <c r="B3" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C3" s="4">
         <v>2</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="4">
         <v>3</v>
       </c>
-      <c r="B4" s="4">
+      <c r="B4" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C4" s="4">
         <v>2</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="4">
         <v>4</v>
       </c>
-      <c r="B5" s="4">
+      <c r="B5" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="C5" s="4">
         <v>3</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="4">
         <v>5</v>
       </c>
-      <c r="B6" s="4">
+      <c r="B6" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="C6" s="4">
         <v>4</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="4">
         <v>6</v>
       </c>
-      <c r="B7" s="4">
+      <c r="B7" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="C7" s="4">
         <v>5</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="4">
         <v>7</v>
       </c>
-      <c r="B8" s="4">
+      <c r="B8" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="C8" s="4">
         <v>6</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="4">
         <v>8</v>
       </c>
-      <c r="B9" s="4">
+      <c r="B9" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C9" s="4">
         <v>6</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="4">
         <v>9</v>
       </c>
-      <c r="B10" s="4">
+      <c r="B10" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="C10" s="4">
         <v>8</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="4">
         <v>10</v>
       </c>
-      <c r="B11" s="4">
+      <c r="B11" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C11" s="4">
         <v>10</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" s="4">
         <v>11</v>
       </c>
-      <c r="B12" s="4">
+      <c r="B12" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="C12" s="4">
         <v>10</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="4">
         <v>12</v>
       </c>
-      <c r="B13" s="4">
+      <c r="B13" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="C13" s="4">
         <v>11</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="4">
         <v>13</v>
       </c>
-      <c r="B14" s="4">
+      <c r="B14" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C14" s="4">
         <v>11</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" s="4">
         <v>14</v>
       </c>
-      <c r="B15" s="4">
+      <c r="B15" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C15" s="4">
         <v>11</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" s="4">
         <v>15</v>
       </c>
-      <c r="B16" s="4">
+      <c r="B16" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="C16" s="4">
         <v>12</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" s="4">
         <v>16</v>
       </c>
-      <c r="B17" s="4">
+      <c r="B17" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="C17" s="4">
         <v>12</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" s="4">
         <v>17</v>
       </c>
-      <c r="B18" s="4">
+      <c r="B18" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="C18" s="4">
         <v>12</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" s="4">
         <v>18</v>
       </c>
-      <c r="B19" s="4">
+      <c r="B19" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C19" s="4">
         <v>12</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" s="4">
         <v>19</v>
       </c>
-      <c r="B20" s="4">
+      <c r="B20" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="C20" s="4">
         <v>13</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" s="4">
         <v>20</v>
       </c>
-      <c r="B21" s="4">
+      <c r="B21" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="C21" s="4">
         <v>13</v>
-      </c>
-      <c r="C21" s="5" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" s="4">
         <v>21</v>
       </c>
-      <c r="B22" s="4">
+      <c r="B22" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="C22" s="4">
         <v>13</v>
-      </c>
-      <c r="C22" s="5" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" s="4">
         <v>22</v>
       </c>
-      <c r="B23" s="4">
+      <c r="B23" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="C23" s="4">
         <v>13</v>
-      </c>
-      <c r="C23" s="5" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" s="4">
         <v>23</v>
       </c>
-      <c r="B24" s="4">
+      <c r="B24" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C24" s="4">
         <v>13</v>
-      </c>
-      <c r="C24" s="5" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" s="4">
         <v>24</v>
       </c>
-      <c r="B25" s="4">
+      <c r="B25" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="C25" s="4">
         <v>13</v>
-      </c>
-      <c r="C25" s="5" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" s="4">
         <v>25</v>
       </c>
-      <c r="B26" s="4">
+      <c r="B26" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C26" s="4">
         <v>14</v>
-      </c>
-      <c r="C26" s="5" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="27" spans="1:3">
       <c r="A27" s="4">
         <v>26</v>
       </c>
-      <c r="B27" s="4">
+      <c r="B27" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="C27" s="4">
         <v>14</v>
-      </c>
-      <c r="C27" s="5" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="28" spans="1:3">
       <c r="A28" s="4">
         <v>27</v>
       </c>
-      <c r="B28" s="4">
+      <c r="B28" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="C28" s="4">
         <v>15</v>
-      </c>
-      <c r="C28" s="5" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="29" spans="1:3">
       <c r="A29" s="4">
         <v>28</v>
       </c>
-      <c r="B29" s="4">
+      <c r="B29" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="C29" s="4">
         <v>15</v>
-      </c>
-      <c r="C29" s="5" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="30" spans="1:3">
       <c r="A30" s="4">
         <v>29</v>
       </c>
-      <c r="B30" s="4">
+      <c r="B30" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="C30" s="4">
         <v>16</v>
-      </c>
-      <c r="C30" s="5" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="31" spans="1:3">
       <c r="A31" s="4">
         <v>30</v>
       </c>
-      <c r="B31" s="4">
+      <c r="B31" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="C31" s="4">
         <v>17</v>
-      </c>
-      <c r="C31" s="5" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="32" spans="1:3">
       <c r="A32" s="4">
         <v>31</v>
       </c>
-      <c r="B32" s="4">
+      <c r="B32" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="C32" s="4">
         <v>18</v>
-      </c>
-      <c r="C32" s="5" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="33" spans="1:3">
       <c r="A33" s="4">
         <v>32</v>
       </c>
-      <c r="B33" s="4">
+      <c r="B33" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C33" s="4">
         <v>19</v>
-      </c>
-      <c r="C33" s="5" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="34" spans="1:3">
       <c r="A34" s="4">
         <v>33</v>
       </c>
-      <c r="B34" s="4">
+      <c r="B34" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="C34" s="4">
         <v>20</v>
-      </c>
-      <c r="C34" s="5" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="35" spans="1:3">
       <c r="A35" s="4">
         <v>34</v>
       </c>
-      <c r="B35" s="4">
+      <c r="B35" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="C35" s="4">
         <v>21</v>
-      </c>
-      <c r="C35" s="5" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="36" spans="1:3">
       <c r="A36" s="4">
         <v>35</v>
       </c>
-      <c r="B36" s="4">
+      <c r="B36" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="C36" s="4">
         <v>21</v>
-      </c>
-      <c r="C36" s="5" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="37" spans="1:3">
       <c r="A37" s="4">
         <v>36</v>
       </c>
-      <c r="B37" s="4">
+      <c r="B37" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="C37" s="4">
         <v>22</v>
-      </c>
-      <c r="C37" s="5" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="38" spans="1:3">
       <c r="A38" s="4">
         <v>37</v>
       </c>
-      <c r="B38" s="4">
+      <c r="B38" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="C38" s="4">
         <v>22</v>
-      </c>
-      <c r="C38" s="5" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="39" spans="1:3">
       <c r="A39" s="4">
         <v>38</v>
       </c>
-      <c r="B39" s="4">
+      <c r="B39" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="C39" s="4">
         <v>24</v>
-      </c>
-      <c r="C39" s="5" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="40" spans="1:3">
       <c r="A40" s="4">
         <v>39</v>
       </c>
-      <c r="B40" s="4">
+      <c r="B40" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="C40" s="4">
         <v>25</v>
-      </c>
-      <c r="C40" s="5" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="41" spans="1:3">
       <c r="A41" s="4">
         <v>40</v>
       </c>
-      <c r="B41" s="4">
+      <c r="B41" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="C41" s="4">
         <v>25</v>
-      </c>
-      <c r="C41" s="5" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="42" spans="1:3">
       <c r="A42" s="4">
         <v>41</v>
       </c>
-      <c r="B42" s="4">
+      <c r="B42" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C42" s="4">
         <v>26</v>
-      </c>
-      <c r="C42" s="5" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="43" spans="1:3">
       <c r="A43" s="4">
         <v>42</v>
       </c>
-      <c r="B43" s="4">
+      <c r="B43" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C43" s="4">
         <v>27</v>
-      </c>
-      <c r="C43" s="5" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="44" spans="1:3">
       <c r="A44" s="4">
         <v>43</v>
       </c>
-      <c r="B44" s="4">
+      <c r="B44" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="C44" s="4">
         <v>28</v>
-      </c>
-      <c r="C44" s="5" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="45" spans="1:3">
       <c r="A45" s="4">
         <v>44</v>
       </c>
-      <c r="B45" s="4">
+      <c r="B45" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="C45" s="4">
         <v>28</v>
-      </c>
-      <c r="C45" s="5" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="46" spans="1:3">
       <c r="A46" s="4">
         <v>45</v>
       </c>
-      <c r="B46" s="4">
+      <c r="B46" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="C46" s="4">
         <v>29</v>
-      </c>
-      <c r="C46" s="5" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="47" spans="1:3">
       <c r="A47" s="4">
         <v>46</v>
       </c>
-      <c r="B47" s="4">
+      <c r="B47" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="C47" s="4">
         <v>29</v>
-      </c>
-      <c r="C47" s="5" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="48" spans="1:3">
       <c r="A48" s="4">
         <v>47</v>
       </c>
-      <c r="B48" s="4">
+      <c r="B48" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="C48" s="4">
         <v>30</v>
-      </c>
-      <c r="C48" s="5" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="49" spans="1:3">
       <c r="A49" s="4">
         <v>48</v>
       </c>
-      <c r="B49" s="4">
+      <c r="B49" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="C49" s="4">
         <v>30</v>
-      </c>
-      <c r="C49" s="5" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="50" spans="1:3">
       <c r="A50" s="4">
         <v>49</v>
       </c>
-      <c r="B50" s="4">
+      <c r="B50" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="C50" s="4">
         <v>31</v>
-      </c>
-      <c r="C50" s="5" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="51" spans="1:3">
       <c r="A51" s="4">
         <v>50</v>
       </c>
-      <c r="B51" s="4">
+      <c r="B51" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="C51" s="4">
         <v>32</v>
-      </c>
-      <c r="C51" s="5" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="52" spans="1:3">
       <c r="A52" s="4">
         <v>51</v>
       </c>
-      <c r="B52" s="4">
+      <c r="B52" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="C52" s="4">
         <v>32</v>
-      </c>
-      <c r="C52" s="5" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="53" spans="1:3">
       <c r="A53" s="4">
         <v>52</v>
       </c>
-      <c r="B53" s="4">
+      <c r="B53" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="C53" s="4">
         <v>33</v>
-      </c>
-      <c r="C53" s="5" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="54" spans="1:3">
       <c r="A54" s="4">
         <v>53</v>
       </c>
-      <c r="B54" s="4">
+      <c r="B54" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="C54" s="4">
         <v>33</v>
-      </c>
-      <c r="C54" s="5" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="55" spans="1:3">
       <c r="A55" s="4">
         <v>54</v>
       </c>
-      <c r="B55" s="4">
+      <c r="B55" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="C55" s="4">
         <v>34</v>
-      </c>
-      <c r="C55" s="5" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="56" spans="1:3">
       <c r="A56" s="4">
         <v>55</v>
       </c>
-      <c r="B56" s="4">
+      <c r="B56" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="C56" s="4">
         <v>35</v>
-      </c>
-      <c r="C56" s="5" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="57" spans="1:3">
       <c r="A57" s="4">
         <v>56</v>
       </c>
-      <c r="B57" s="4">
+      <c r="B57" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="C57" s="4">
         <v>35</v>
-      </c>
-      <c r="C57" s="5" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="58" spans="1:3">
       <c r="A58" s="4">
         <v>57</v>
       </c>
-      <c r="B58" s="4">
+      <c r="B58" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="C58" s="4">
         <v>36</v>
-      </c>
-      <c r="C58" s="5" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="59" spans="1:3">
       <c r="A59" s="4">
         <v>58</v>
       </c>
-      <c r="B59" s="4">
+      <c r="B59" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="C59" s="4">
         <v>37</v>
-      </c>
-      <c r="C59" s="5" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="60" spans="1:3">
       <c r="A60" s="4">
         <v>59</v>
       </c>
-      <c r="B60" s="4">
+      <c r="B60" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="C60" s="4">
         <v>37</v>
-      </c>
-      <c r="C60" s="5" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="61" spans="1:3">
       <c r="A61" s="4">
         <v>60</v>
       </c>
-      <c r="B61" s="4">
+      <c r="B61" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C61" s="4">
         <v>37</v>
-      </c>
-      <c r="C61" s="5" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="62" spans="1:3">
       <c r="A62" s="4">
         <v>61</v>
       </c>
-      <c r="B62" s="4">
+      <c r="B62" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="C62" s="4">
         <v>38</v>
-      </c>
-      <c r="C62" s="5" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="63" spans="1:3">
       <c r="A63" s="4">
         <v>62</v>
       </c>
-      <c r="B63" s="4">
+      <c r="B63" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="C63" s="4">
         <v>38</v>
-      </c>
-      <c r="C63" s="5" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="64" spans="1:3">
       <c r="A64" s="4">
         <v>63</v>
       </c>
-      <c r="B64" s="4">
+      <c r="B64" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="C64" s="4">
         <v>39</v>
-      </c>
-      <c r="C64" s="5" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="65" spans="1:3">
       <c r="A65" s="4">
         <v>64</v>
       </c>
-      <c r="B65" s="4">
+      <c r="B65" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="C65" s="4">
         <v>44</v>
-      </c>
-      <c r="C65" s="5" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="66" spans="1:3">
       <c r="A66" s="4">
         <v>65</v>
       </c>
-      <c r="B66" s="4">
+      <c r="B66" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C66" s="4">
         <v>48</v>
-      </c>
-      <c r="C66" s="5" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="67" spans="1:3">
       <c r="A67" s="4">
         <v>66</v>
       </c>
-      <c r="B67" s="4">
+      <c r="B67" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="C67" s="4">
         <v>49</v>
-      </c>
-      <c r="C67" s="5" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="68" spans="1:3">
       <c r="A68" s="4">
         <v>67</v>
       </c>
-      <c r="B68" s="4">
+      <c r="B68" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="C68" s="4">
         <v>52</v>
-      </c>
-      <c r="C68" s="5" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="69" spans="1:3">
       <c r="A69" s="4">
         <v>68</v>
       </c>
-      <c r="B69" s="4">
+      <c r="B69" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="C69" s="4">
         <v>52</v>
-      </c>
-      <c r="C69" s="5" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="70" spans="1:3">
       <c r="A70" s="4">
         <v>69</v>
       </c>
-      <c r="B70" s="4">
+      <c r="B70" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="C70" s="4">
         <v>52</v>
-      </c>
-      <c r="C70" s="5" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="71" spans="1:3">
       <c r="A71" s="4">
         <v>70</v>
       </c>
-      <c r="B71" s="4">
+      <c r="B71" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="C71" s="4">
         <v>52</v>
-      </c>
-      <c r="C71" s="5" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="72" spans="1:3">
       <c r="A72" s="4">
         <v>71</v>
       </c>
-      <c r="B72" s="4">
+      <c r="B72" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="C72" s="4">
         <v>58</v>
-      </c>
-      <c r="C72" s="5" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="73" spans="1:3">
       <c r="A73" s="4">
         <v>72</v>
       </c>
-      <c r="B73" s="4">
+      <c r="B73" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="C73" s="4">
         <v>61</v>
-      </c>
-      <c r="C73" s="5" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="74" spans="1:3">
       <c r="A74" s="4">
         <v>73</v>
       </c>
-      <c r="B74" s="4">
+      <c r="B74" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="C74" s="4">
         <v>62</v>
-      </c>
-      <c r="C74" s="5" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="75" spans="1:3">
       <c r="A75" s="4">
         <v>74</v>
       </c>
-      <c r="B75" s="4">
+      <c r="B75" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="C75" s="4">
         <v>65</v>
-      </c>
-      <c r="C75" s="5" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="76" spans="1:3">
       <c r="A76" s="4">
         <v>75</v>
       </c>
-      <c r="B76" s="4">
+      <c r="B76" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="C76" s="4">
         <v>66</v>
-      </c>
-      <c r="C76" s="5" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="77" spans="1:3">
       <c r="A77" s="4">
         <v>76</v>
       </c>
-      <c r="B77" s="4">
+      <c r="B77" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="C77" s="4">
         <v>67</v>
-      </c>
-      <c r="C77" s="5" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="78" spans="1:3">
       <c r="A78" s="4">
         <v>77</v>
       </c>
-      <c r="B78" s="4">
+      <c r="B78" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="C78" s="4">
         <v>68</v>
-      </c>
-      <c r="C78" s="5" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="79" spans="1:3">
       <c r="A79" s="4">
         <v>78</v>
       </c>
-      <c r="B79" s="4">
+      <c r="B79" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="C79" s="4">
         <v>70</v>
-      </c>
-      <c r="C79" s="5" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="80" spans="1:3">
       <c r="A80" s="4">
         <v>79</v>
       </c>
-      <c r="B80" s="4">
+      <c r="B80" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="C80" s="4">
         <v>71</v>
-      </c>
-      <c r="C80" s="5" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="81" spans="1:3">
       <c r="A81" s="4">
         <v>80</v>
       </c>
-      <c r="B81" s="4">
+      <c r="B81" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="C81" s="4">
         <v>71</v>
-      </c>
-      <c r="C81" s="5" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="82" spans="1:3">
       <c r="A82" s="4">
         <v>81</v>
       </c>
-      <c r="B82" s="4">
+      <c r="B82" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="C82" s="4">
         <v>78</v>
-      </c>
-      <c r="C82" s="5" t="s">
-        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -3724,7 +3724,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{491D14EC-1CB1-4681-930A-4B9B4015FC83}">
   <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
added columns to asset data
</commit_message>
<xml_diff>
--- a/backend/internal/seed/seed_data/mst_dummy_data.xlsx
+++ b/backend/internal/seed/seed_data/mst_dummy_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Uni\Intern SM\Stock Opname App [SOSMIT]\SOSMIT\backend\internal\seed\seed_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E6003C4-6164-4968-9583-0FEA4F9215E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EB1D521-431D-4551-B751-FE0FA7876217}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10540" activeTab="1" xr2:uid="{AF28B77B-5B1D-47C2-ADE5-ADF50DA09BCF}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10540" activeTab="5" xr2:uid="{AF28B77B-5B1D-47C2-ADE5-ADF50DA09BCF}"/>
   </bookViews>
   <sheets>
     <sheet name="Region" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="241">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="246">
   <si>
     <t>id</t>
   </si>
@@ -764,6 +764,21 @@
   </si>
   <si>
     <t>XXZHJ231947513</t>
+  </si>
+  <si>
+    <t>status_reason</t>
+  </si>
+  <si>
+    <t>Disposed</t>
+  </si>
+  <si>
+    <t>Obsolete</t>
+  </si>
+  <si>
+    <t>condition</t>
+  </si>
+  <si>
+    <t>condition_photo_url</t>
   </si>
 </sst>
 </file>
@@ -1835,7 +1850,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F51990CE-FF2C-48E9-82E1-2E87B3A6C16A}">
   <dimension ref="A1:C82"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
@@ -3722,25 +3737,28 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{491D14EC-1CB1-4681-930A-4B9B4015FC83}">
-  <dimension ref="A1:J13"/>
+  <dimension ref="A1:M13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="14.08984375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.90625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.08984375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.54296875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.36328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.26953125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="31.453125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.26953125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.08984375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.54296875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.36328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.26953125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="31.453125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.453125" customWidth="1"/>
+    <col min="11" max="11" width="21" customWidth="1"/>
+    <col min="12" max="12" width="9.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:13">
       <c r="A1" s="1" t="s">
         <v>211</v>
       </c>
@@ -3751,28 +3769,37 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>215</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:13">
       <c r="A2" s="1" t="s">
         <v>175</v>
       </c>
@@ -3782,29 +3809,34 @@
       <c r="C2" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="1"/>
+      <c r="E2" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="I2" s="2">
+      <c r="J2" s="1">
+        <v>1</v>
+      </c>
+      <c r="K2" s="1"/>
+      <c r="L2" s="2">
         <v>1223</v>
       </c>
-      <c r="J2" s="1">
+      <c r="M2" s="1">
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:13">
       <c r="A3" s="1" t="s">
         <v>182</v>
       </c>
@@ -3814,29 +3846,34 @@
       <c r="C3" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="1"/>
+      <c r="E3" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="H3" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="I3" s="1" t="s">
         <v>184</v>
-      </c>
-      <c r="I3" s="1">
-        <v>1224</v>
       </c>
       <c r="J3" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:10">
+      <c r="K3" s="1"/>
+      <c r="L3" s="1">
+        <v>1224</v>
+      </c>
+      <c r="M3" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13">
       <c r="A4" s="1" t="s">
         <v>185</v>
       </c>
@@ -3846,29 +3883,34 @@
       <c r="C4" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="1"/>
+      <c r="E4" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="F4" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="G4" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="H4" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="I4" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="I4" s="2">
+      <c r="J4" s="1">
+        <v>1</v>
+      </c>
+      <c r="K4" s="1"/>
+      <c r="L4" s="2">
         <v>1225</v>
       </c>
-      <c r="J4" s="1">
+      <c r="M4" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:13">
       <c r="A5" s="1" t="s">
         <v>188</v>
       </c>
@@ -3878,29 +3920,34 @@
       <c r="C5" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" s="1"/>
+      <c r="E5" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="F5" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="G5" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="H5" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="H5" s="1" t="s">
+      <c r="I5" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="I5" s="1">
+      <c r="J5" s="1">
+        <v>1</v>
+      </c>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1">
         <v>1226</v>
       </c>
-      <c r="J5" s="1">
+      <c r="M5" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:13">
       <c r="A6" s="1" t="s">
         <v>189</v>
       </c>
@@ -3910,29 +3957,34 @@
       <c r="C6" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" s="1"/>
+      <c r="E6" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="F6" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="G6" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="H6" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="H6" s="1" t="s">
+      <c r="I6" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="I6" s="2">
+      <c r="J6" s="1">
+        <v>1</v>
+      </c>
+      <c r="K6" s="1"/>
+      <c r="L6" s="2">
         <v>1223</v>
       </c>
-      <c r="J6" s="1">
+      <c r="M6" s="1">
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:13">
       <c r="A7" s="1" t="s">
         <v>193</v>
       </c>
@@ -3942,29 +3994,34 @@
       <c r="C7" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D7" s="1"/>
+      <c r="E7" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="F7" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="G7" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="G7" s="1" t="s">
+      <c r="H7" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="H7" s="1" t="s">
+      <c r="I7" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="I7" s="1">
+      <c r="J7" s="1">
+        <v>1</v>
+      </c>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1">
         <v>1223</v>
       </c>
-      <c r="J7" s="1">
+      <c r="M7" s="1">
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:13">
       <c r="A8" s="1" t="s">
         <v>198</v>
       </c>
@@ -3974,29 +4031,34 @@
       <c r="C8" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D8" s="1"/>
+      <c r="E8" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="F8" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="G8" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="G8" s="1" t="s">
+      <c r="H8" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="H8" s="1" t="s">
+      <c r="I8" s="1" t="s">
         <v>201</v>
-      </c>
-      <c r="I8" s="2">
-        <v>1229</v>
       </c>
       <c r="J8" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:10">
+      <c r="K8" s="1"/>
+      <c r="L8" s="2">
+        <v>1229</v>
+      </c>
+      <c r="M8" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13">
       <c r="A9" s="1" t="s">
         <v>202</v>
       </c>
@@ -4006,29 +4068,34 @@
       <c r="C9" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D9" s="1"/>
+      <c r="E9" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="F9" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="G9" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="G9" s="1" t="s">
+      <c r="H9" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="H9" s="1" t="s">
+      <c r="I9" s="1" t="s">
         <v>201</v>
-      </c>
-      <c r="I9" s="1">
-        <v>1230</v>
       </c>
       <c r="J9" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:10">
+      <c r="K9" s="1"/>
+      <c r="L9" s="1">
+        <v>1230</v>
+      </c>
+      <c r="M9" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13">
       <c r="A10" s="1" t="s">
         <v>203</v>
       </c>
@@ -4038,29 +4105,34 @@
       <c r="C10" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="D10" s="1"/>
+      <c r="E10" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="F10" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="G10" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="G10" s="1" t="s">
+      <c r="H10" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="H10" s="1" t="s">
+      <c r="I10" s="1" t="s">
         <v>204</v>
-      </c>
-      <c r="I10" s="2">
-        <v>1231</v>
       </c>
       <c r="J10" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:10">
+      <c r="K10" s="1"/>
+      <c r="L10" s="2">
+        <v>1231</v>
+      </c>
+      <c r="M10" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13">
       <c r="A11" s="1" t="s">
         <v>205</v>
       </c>
@@ -4070,29 +4142,34 @@
       <c r="C11" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="D11" s="1"/>
+      <c r="E11" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="F11" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="F11" s="1" t="s">
+      <c r="G11" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="G11" s="1" t="s">
+      <c r="H11" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="H11" s="1" t="s">
+      <c r="I11" s="1" t="s">
         <v>207</v>
-      </c>
-      <c r="I11" s="1">
-        <v>1231</v>
       </c>
       <c r="J11" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:10">
+      <c r="K11" s="1"/>
+      <c r="L11" s="1">
+        <v>1231</v>
+      </c>
+      <c r="M11" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13">
       <c r="A12" s="1" t="s">
         <v>208</v>
       </c>
@@ -4102,29 +4179,34 @@
       <c r="C12" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="D12" s="1"/>
+      <c r="E12" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="F12" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="F12" s="1" t="s">
+      <c r="G12" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="G12" s="1" t="s">
+      <c r="H12" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="H12" s="1" t="s">
+      <c r="I12" s="1" t="s">
         <v>207</v>
-      </c>
-      <c r="I12" s="2">
-        <v>1224</v>
       </c>
       <c r="J12" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:10">
+      <c r="K12" s="1"/>
+      <c r="L12" s="2">
+        <v>1224</v>
+      </c>
+      <c r="M12" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13">
       <c r="A13" s="1" t="s">
         <v>209</v>
       </c>
@@ -4132,27 +4214,34 @@
         <v>240</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>176</v>
+        <v>242</v>
       </c>
       <c r="D13" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="E13" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="F13" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="F13" s="1" t="s">
+      <c r="G13" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="G13" s="1" t="s">
+      <c r="H13" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="H13" s="1" t="s">
+      <c r="I13" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="I13" s="1">
+      <c r="J13" s="1">
+        <v>1</v>
+      </c>
+      <c r="K13" s="1"/>
+      <c r="L13" s="1">
         <v>1225</v>
       </c>
-      <c r="J13" s="1">
+      <c r="M13" s="1">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added new column 'site_ga_id' in 'Site' table
</commit_message>
<xml_diff>
--- a/backend/internal/seed/seed_data/mst_dummy_data.xlsx
+++ b/backend/internal/seed/seed_data/mst_dummy_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Uni\Intern SM\Stock Opname App [SOSMIT]\SOSMIT\backend\internal\seed\seed_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EB1D521-431D-4551-B751-FE0FA7876217}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{396F4910-0844-4D1E-B4BB-3F25CEB45D79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10540" activeTab="5" xr2:uid="{AF28B77B-5B1D-47C2-ADE5-ADF50DA09BCF}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10540" firstSheet="1" activeTab="2" xr2:uid="{AF28B77B-5B1D-47C2-ADE5-ADF50DA09BCF}"/>
   </bookViews>
   <sheets>
     <sheet name="Region" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="246">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="247">
   <si>
     <t>id</t>
   </si>
@@ -779,6 +779,9 @@
   </si>
   <si>
     <t>condition_photo_url</t>
+  </si>
+  <si>
+    <t>site_ga_id</t>
   </si>
 </sst>
 </file>
@@ -1851,7 +1854,7 @@
   <dimension ref="A1:C82"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -2768,19 +2771,20 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E6AD482-693C-4526-A8EF-051504D339CF}">
-  <dimension ref="A1:C51"/>
+  <dimension ref="A1:D51"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="2" max="2" width="47.08984375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -2790,8 +2794,11 @@
       <c r="C1" s="5" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
+      <c r="D1" s="5" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -2801,8 +2808,11 @@
       <c r="C2" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:3">
+      <c r="D2" s="1">
+        <v>1233</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -2812,8 +2822,11 @@
       <c r="C3" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:3">
+      <c r="D3" s="1">
+        <v>1233</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" s="4">
         <v>3</v>
       </c>
@@ -2823,8 +2836,11 @@
       <c r="C4" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:3">
+      <c r="D4" s="1">
+        <v>1233</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5" s="4">
         <v>4</v>
       </c>
@@ -2834,8 +2850,11 @@
       <c r="C5" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:3">
+      <c r="D5" s="1">
+        <v>1233</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
       <c r="A6" s="4">
         <v>5</v>
       </c>
@@ -2845,8 +2864,11 @@
       <c r="C6" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:3">
+      <c r="D6" s="1">
+        <v>1222</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
       <c r="A7" s="4">
         <v>6</v>
       </c>
@@ -2856,8 +2878,11 @@
       <c r="C7" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:3">
+      <c r="D7" s="1">
+        <v>1222</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
       <c r="A8" s="4">
         <v>7</v>
       </c>
@@ -2867,8 +2892,11 @@
       <c r="C8" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:3">
+      <c r="D8" s="1">
+        <v>1222</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
       <c r="A9" s="4">
         <v>8</v>
       </c>
@@ -2878,8 +2906,11 @@
       <c r="C9" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:3">
+      <c r="D9" s="1">
+        <v>1222</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
       <c r="A10" s="4">
         <v>9</v>
       </c>
@@ -2889,8 +2920,12 @@
       <c r="C10" s="4">
         <v>3</v>
       </c>
-    </row>
-    <row r="11" spans="1:3">
+      <c r="D10" s="1">
+        <f ca="1">RANDBETWEEN(1223,1232)</f>
+        <v>1224</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
       <c r="A11" s="4">
         <v>10</v>
       </c>
@@ -2900,8 +2935,12 @@
       <c r="C11" s="4">
         <v>3</v>
       </c>
-    </row>
-    <row r="12" spans="1:3">
+      <c r="D11" s="1">
+        <f t="shared" ref="D11:D51" ca="1" si="0">RANDBETWEEN(1223,1232)</f>
+        <v>1223</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
       <c r="A12" s="4">
         <v>11</v>
       </c>
@@ -2911,8 +2950,12 @@
       <c r="C12" s="4">
         <v>3</v>
       </c>
-    </row>
-    <row r="13" spans="1:3">
+      <c r="D12" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>1225</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
       <c r="A13" s="4">
         <v>12</v>
       </c>
@@ -2922,8 +2965,12 @@
       <c r="C13" s="4">
         <v>3</v>
       </c>
-    </row>
-    <row r="14" spans="1:3">
+      <c r="D13" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>1229</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
       <c r="A14" s="4">
         <v>13</v>
       </c>
@@ -2933,8 +2980,12 @@
       <c r="C14" s="4">
         <v>3</v>
       </c>
-    </row>
-    <row r="15" spans="1:3">
+      <c r="D14" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>1232</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
       <c r="A15" s="4">
         <v>14</v>
       </c>
@@ -2944,8 +2995,12 @@
       <c r="C15" s="4">
         <v>3</v>
       </c>
-    </row>
-    <row r="16" spans="1:3">
+      <c r="D15" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>1231</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
       <c r="A16" s="4">
         <v>15</v>
       </c>
@@ -2955,8 +3010,12 @@
       <c r="C16" s="4">
         <v>3</v>
       </c>
-    </row>
-    <row r="17" spans="1:3">
+      <c r="D16" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>1227</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
       <c r="A17" s="4">
         <v>16</v>
       </c>
@@ -2966,8 +3025,12 @@
       <c r="C17" s="4">
         <v>3</v>
       </c>
-    </row>
-    <row r="18" spans="1:3">
+      <c r="D17" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>1229</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
       <c r="A18" s="4">
         <v>20</v>
       </c>
@@ -2977,8 +3040,12 @@
       <c r="C18" s="4">
         <v>3</v>
       </c>
-    </row>
-    <row r="19" spans="1:3">
+      <c r="D18" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>1228</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
       <c r="A19" s="4">
         <v>21</v>
       </c>
@@ -2988,8 +3055,12 @@
       <c r="C19" s="4">
         <v>3</v>
       </c>
-    </row>
-    <row r="20" spans="1:3">
+      <c r="D19" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>1231</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
       <c r="A20" s="4">
         <v>22</v>
       </c>
@@ -2999,8 +3070,12 @@
       <c r="C20" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="21" spans="1:3">
+      <c r="D20" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>1227</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
       <c r="A21" s="4">
         <v>23</v>
       </c>
@@ -3010,8 +3085,12 @@
       <c r="C21" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="22" spans="1:3">
+      <c r="D21" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>1224</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
       <c r="A22" s="4">
         <v>25</v>
       </c>
@@ -3021,8 +3100,12 @@
       <c r="C22" s="4">
         <v>6</v>
       </c>
-    </row>
-    <row r="23" spans="1:3">
+      <c r="D22" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>1224</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
       <c r="A23" s="4">
         <v>26</v>
       </c>
@@ -3032,8 +3115,12 @@
       <c r="C23" s="4">
         <v>6</v>
       </c>
-    </row>
-    <row r="24" spans="1:3">
+      <c r="D23" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>1230</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
       <c r="A24" s="4">
         <v>27</v>
       </c>
@@ -3043,8 +3130,12 @@
       <c r="C24" s="4">
         <v>6</v>
       </c>
-    </row>
-    <row r="25" spans="1:3">
+      <c r="D24" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>1230</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
       <c r="A25" s="4">
         <v>29</v>
       </c>
@@ -3054,8 +3145,12 @@
       <c r="C25" s="4">
         <v>6</v>
       </c>
-    </row>
-    <row r="26" spans="1:3">
+      <c r="D25" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>1223</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
       <c r="A26" s="4">
         <v>30</v>
       </c>
@@ -3065,8 +3160,12 @@
       <c r="C26" s="4">
         <v>7</v>
       </c>
-    </row>
-    <row r="27" spans="1:3">
+      <c r="D26" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>1223</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
       <c r="A27" s="4">
         <v>32</v>
       </c>
@@ -3076,8 +3175,12 @@
       <c r="C27" s="4">
         <v>8</v>
       </c>
-    </row>
-    <row r="28" spans="1:3">
+      <c r="D27" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>1232</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
       <c r="A28" s="4">
         <v>33</v>
       </c>
@@ -3087,8 +3190,12 @@
       <c r="C28" s="4">
         <v>8</v>
       </c>
-    </row>
-    <row r="29" spans="1:3">
+      <c r="D28" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>1227</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
       <c r="A29" s="4">
         <v>34</v>
       </c>
@@ -3098,8 +3205,12 @@
       <c r="C29" s="4">
         <v>8</v>
       </c>
-    </row>
-    <row r="30" spans="1:3">
+      <c r="D29" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>1229</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
       <c r="A30" s="4">
         <v>35</v>
       </c>
@@ -3109,8 +3220,12 @@
       <c r="C30" s="4">
         <v>8</v>
       </c>
-    </row>
-    <row r="31" spans="1:3">
+      <c r="D30" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>1232</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
       <c r="A31" s="4">
         <v>36</v>
       </c>
@@ -3120,8 +3235,12 @@
       <c r="C31" s="4">
         <v>8</v>
       </c>
-    </row>
-    <row r="32" spans="1:3">
+      <c r="D31" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>1228</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
       <c r="A32" s="4">
         <v>37</v>
       </c>
@@ -3131,8 +3250,12 @@
       <c r="C32" s="4">
         <v>8</v>
       </c>
-    </row>
-    <row r="33" spans="1:3">
+      <c r="D32" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>1227</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
       <c r="A33" s="4">
         <v>38</v>
       </c>
@@ -3142,8 +3265,12 @@
       <c r="C33" s="4">
         <v>8</v>
       </c>
-    </row>
-    <row r="34" spans="1:3">
+      <c r="D33" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>1232</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
       <c r="A34" s="4">
         <v>39</v>
       </c>
@@ -3153,8 +3280,12 @@
       <c r="C34" s="4">
         <v>8</v>
       </c>
-    </row>
-    <row r="35" spans="1:3">
+      <c r="D34" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>1223</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
       <c r="A35" s="4">
         <v>40</v>
       </c>
@@ -3164,8 +3295,12 @@
       <c r="C35" s="4">
         <v>8</v>
       </c>
-    </row>
-    <row r="36" spans="1:3">
+      <c r="D35" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>1228</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
       <c r="A36" s="4">
         <v>41</v>
       </c>
@@ -3175,8 +3310,12 @@
       <c r="C36" s="4">
         <v>8</v>
       </c>
-    </row>
-    <row r="37" spans="1:3">
+      <c r="D36" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>1228</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
       <c r="A37" s="4">
         <v>42</v>
       </c>
@@ -3186,8 +3325,12 @@
       <c r="C37" s="4">
         <v>8</v>
       </c>
-    </row>
-    <row r="38" spans="1:3">
+      <c r="D37" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>1226</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
       <c r="A38" s="4">
         <v>43</v>
       </c>
@@ -3197,8 +3340,12 @@
       <c r="C38" s="4">
         <v>8</v>
       </c>
-    </row>
-    <row r="39" spans="1:3">
+      <c r="D38" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>1230</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
       <c r="A39" s="4">
         <v>44</v>
       </c>
@@ -3208,8 +3355,12 @@
       <c r="C39" s="4">
         <v>8</v>
       </c>
-    </row>
-    <row r="40" spans="1:3">
+      <c r="D39" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>1231</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4">
       <c r="A40" s="4">
         <v>45</v>
       </c>
@@ -3219,8 +3370,12 @@
       <c r="C40" s="4">
         <v>8</v>
       </c>
-    </row>
-    <row r="41" spans="1:3">
+      <c r="D40" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>1231</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4">
       <c r="A41" s="4">
         <v>46</v>
       </c>
@@ -3230,8 +3385,12 @@
       <c r="C41" s="4">
         <v>8</v>
       </c>
-    </row>
-    <row r="42" spans="1:3">
+      <c r="D41" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>1228</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
       <c r="A42" s="4">
         <v>47</v>
       </c>
@@ -3241,8 +3400,12 @@
       <c r="C42" s="4">
         <v>8</v>
       </c>
-    </row>
-    <row r="43" spans="1:3">
+      <c r="D42" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>1227</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4">
       <c r="A43" s="4">
         <v>48</v>
       </c>
@@ -3252,8 +3415,12 @@
       <c r="C43" s="4">
         <v>9</v>
       </c>
-    </row>
-    <row r="44" spans="1:3">
+      <c r="D43" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>1228</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4">
       <c r="A44" s="4">
         <v>49</v>
       </c>
@@ -3263,8 +3430,12 @@
       <c r="C44" s="4">
         <v>9</v>
       </c>
-    </row>
-    <row r="45" spans="1:3">
+      <c r="D44" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>1227</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4">
       <c r="A45" s="4">
         <v>50</v>
       </c>
@@ -3274,8 +3445,12 @@
       <c r="C45" s="4">
         <v>10</v>
       </c>
-    </row>
-    <row r="46" spans="1:3">
+      <c r="D45" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>1229</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4">
       <c r="A46" s="4">
         <v>51</v>
       </c>
@@ -3285,8 +3460,12 @@
       <c r="C46" s="4">
         <v>10</v>
       </c>
-    </row>
-    <row r="47" spans="1:3">
+      <c r="D46" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>1232</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4">
       <c r="A47" s="4">
         <v>52</v>
       </c>
@@ -3296,8 +3475,12 @@
       <c r="C47" s="4">
         <v>10</v>
       </c>
-    </row>
-    <row r="48" spans="1:3">
+      <c r="D47" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>1228</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4">
       <c r="A48" s="4">
         <v>53</v>
       </c>
@@ -3307,8 +3490,12 @@
       <c r="C48" s="4">
         <v>10</v>
       </c>
-    </row>
-    <row r="49" spans="1:3">
+      <c r="D48" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>1230</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4">
       <c r="A49" s="4">
         <v>54</v>
       </c>
@@ -3318,8 +3505,12 @@
       <c r="C49" s="4">
         <v>10</v>
       </c>
-    </row>
-    <row r="50" spans="1:3">
+      <c r="D49" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>1227</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4">
       <c r="A50" s="4">
         <v>55</v>
       </c>
@@ -3329,8 +3520,12 @@
       <c r="C50" s="4">
         <v>13</v>
       </c>
-    </row>
-    <row r="51" spans="1:3">
+      <c r="D50" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>1224</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4">
       <c r="A51" s="4">
         <v>56</v>
       </c>
@@ -3339,6 +3534,10 @@
       </c>
       <c r="C51" s="4">
         <v>13</v>
+      </c>
+      <c r="D51" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>1225</v>
       </c>
     </row>
   </sheetData>
@@ -3351,7 +3550,7 @@
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -3739,7 +3938,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{491D14EC-1CB1-4681-930A-4B9B4015FC83}">
   <dimension ref="A1:M13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+    <sheetView topLeftCell="G1" workbookViewId="0">
       <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
[WORKING] asset page now displays all the necessary info, modified the db as well for this feature to be clean
</commit_message>
<xml_diff>
--- a/backend/internal/seed/seed_data/mst_dummy_data.xlsx
+++ b/backend/internal/seed/seed_data/mst_dummy_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Uni\Intern SM\Stock Opname App [SOSMIT]\SOSMIT\backend\internal\seed\seed_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{396F4910-0844-4D1E-B4BB-3F25CEB45D79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DA5DA70-1B07-4346-AD77-3CA027B1CC16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10540" firstSheet="1" activeTab="2" xr2:uid="{AF28B77B-5B1D-47C2-ADE5-ADF50DA09BCF}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10540" firstSheet="1" activeTab="5" xr2:uid="{AF28B77B-5B1D-47C2-ADE5-ADF50DA09BCF}"/>
   </bookViews>
   <sheets>
     <sheet name="Region" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="247">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="517" uniqueCount="272">
   <si>
     <t>id</t>
   </si>
@@ -782,13 +782,88 @@
   </si>
   <si>
     <t>site_ga_id</t>
+  </si>
+  <si>
+    <t>location</t>
+  </si>
+  <si>
+    <t>room</t>
+  </si>
+  <si>
+    <t>Shelf A.1</t>
+  </si>
+  <si>
+    <t>16th floor storage room</t>
+  </si>
+  <si>
+    <t>SMLT00000002</t>
+  </si>
+  <si>
+    <t>5CD19R0NVT</t>
+  </si>
+  <si>
+    <t>5CD1842KTY</t>
+  </si>
+  <si>
+    <t>SMPR00000004</t>
+  </si>
+  <si>
+    <t>SMPR00000005</t>
+  </si>
+  <si>
+    <t>SMPR00000006</t>
+  </si>
+  <si>
+    <t>SMPR00000007</t>
+  </si>
+  <si>
+    <t>SMPR00000008</t>
+  </si>
+  <si>
+    <t>SMMN00000002</t>
+  </si>
+  <si>
+    <t>SMPU00000002</t>
+  </si>
+  <si>
+    <t>SMPC00000002</t>
+  </si>
+  <si>
+    <t>3CQ9175DFF</t>
+  </si>
+  <si>
+    <t>3B3455X20123</t>
+  </si>
+  <si>
+    <t>SGH7J2L9G7Y</t>
+  </si>
+  <si>
+    <t>SMLT00000004</t>
+  </si>
+  <si>
+    <t>XXZHJ231945357</t>
+  </si>
+  <si>
+    <t>XXZHJ231945846</t>
+  </si>
+  <si>
+    <t>XXZHJ231935678</t>
+  </si>
+  <si>
+    <t>XXZHJ231298358</t>
+  </si>
+  <si>
+    <t>XXZHJ231536587</t>
+  </si>
+  <si>
+    <t>Lost</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -810,6 +885,12 @@
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -2773,7 +2854,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E6AD482-693C-4526-A8EF-051504D339CF}">
   <dimension ref="A1:D51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
@@ -2922,7 +3003,7 @@
       </c>
       <c r="D10" s="1">
         <f ca="1">RANDBETWEEN(1223,1232)</f>
-        <v>1224</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -2937,7 +3018,7 @@
       </c>
       <c r="D11" s="1">
         <f t="shared" ref="D11:D51" ca="1" si="0">RANDBETWEEN(1223,1232)</f>
-        <v>1223</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -2967,7 +3048,7 @@
       </c>
       <c r="D13" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1229</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -2982,7 +3063,7 @@
       </c>
       <c r="D14" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1232</v>
+        <v>1230</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -2997,7 +3078,7 @@
       </c>
       <c r="D15" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1231</v>
+        <v>1226</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -3012,7 +3093,7 @@
       </c>
       <c r="D16" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1227</v>
+        <v>1226</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -3027,7 +3108,7 @@
       </c>
       <c r="D17" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1229</v>
+        <v>1223</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -3042,7 +3123,7 @@
       </c>
       <c r="D18" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1228</v>
+        <v>1226</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -3057,7 +3138,7 @@
       </c>
       <c r="D19" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1231</v>
+        <v>1232</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -3072,7 +3153,7 @@
       </c>
       <c r="D20" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1227</v>
+        <v>1223</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -3102,7 +3183,7 @@
       </c>
       <c r="D22" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1224</v>
+        <v>1225</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -3132,7 +3213,7 @@
       </c>
       <c r="D24" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1230</v>
+        <v>1231</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -3147,7 +3228,7 @@
       </c>
       <c r="D25" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1223</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -3162,7 +3243,7 @@
       </c>
       <c r="D26" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1223</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -3177,7 +3258,7 @@
       </c>
       <c r="D27" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1232</v>
+        <v>1230</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -3192,7 +3273,7 @@
       </c>
       <c r="D28" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1227</v>
+        <v>1230</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -3222,7 +3303,7 @@
       </c>
       <c r="D30" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1232</v>
+        <v>1226</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -3237,7 +3318,7 @@
       </c>
       <c r="D31" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1228</v>
+        <v>1226</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -3252,7 +3333,7 @@
       </c>
       <c r="D32" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1227</v>
+        <v>1224</v>
       </c>
     </row>
     <row r="33" spans="1:4">
@@ -3267,7 +3348,7 @@
       </c>
       <c r="D33" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1232</v>
+        <v>1223</v>
       </c>
     </row>
     <row r="34" spans="1:4">
@@ -3282,7 +3363,7 @@
       </c>
       <c r="D34" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1223</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="35" spans="1:4">
@@ -3312,7 +3393,7 @@
       </c>
       <c r="D36" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1228</v>
+        <v>1224</v>
       </c>
     </row>
     <row r="37" spans="1:4">
@@ -3327,7 +3408,7 @@
       </c>
       <c r="D37" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1226</v>
+        <v>1225</v>
       </c>
     </row>
     <row r="38" spans="1:4">
@@ -3342,7 +3423,7 @@
       </c>
       <c r="D38" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1230</v>
+        <v>1231</v>
       </c>
     </row>
     <row r="39" spans="1:4">
@@ -3372,7 +3453,7 @@
       </c>
       <c r="D40" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1231</v>
+        <v>1229</v>
       </c>
     </row>
     <row r="41" spans="1:4">
@@ -3387,7 +3468,7 @@
       </c>
       <c r="D41" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1228</v>
+        <v>1231</v>
       </c>
     </row>
     <row r="42" spans="1:4">
@@ -3402,7 +3483,7 @@
       </c>
       <c r="D42" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1227</v>
+        <v>1225</v>
       </c>
     </row>
     <row r="43" spans="1:4">
@@ -3417,7 +3498,7 @@
       </c>
       <c r="D43" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1228</v>
+        <v>1223</v>
       </c>
     </row>
     <row r="44" spans="1:4">
@@ -3432,7 +3513,7 @@
       </c>
       <c r="D44" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1227</v>
+        <v>1224</v>
       </c>
     </row>
     <row r="45" spans="1:4">
@@ -3447,7 +3528,7 @@
       </c>
       <c r="D45" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1229</v>
+        <v>1223</v>
       </c>
     </row>
     <row r="46" spans="1:4">
@@ -3462,7 +3543,7 @@
       </c>
       <c r="D46" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1232</v>
+        <v>1225</v>
       </c>
     </row>
     <row r="47" spans="1:4">
@@ -3477,7 +3558,7 @@
       </c>
       <c r="D47" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1228</v>
+        <v>1224</v>
       </c>
     </row>
     <row r="48" spans="1:4">
@@ -3492,7 +3573,7 @@
       </c>
       <c r="D48" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1230</v>
+        <v>1229</v>
       </c>
     </row>
     <row r="49" spans="1:4">
@@ -3522,7 +3603,7 @@
       </c>
       <c r="D50" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1224</v>
+        <v>1226</v>
       </c>
     </row>
     <row r="51" spans="1:4">
@@ -3537,7 +3618,7 @@
       </c>
       <c r="D51" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1225</v>
+        <v>1227</v>
       </c>
     </row>
   </sheetData>
@@ -3936,10 +4017,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{491D14EC-1CB1-4681-930A-4B9B4015FC83}">
-  <dimension ref="A1:M13"/>
+  <dimension ref="A1:O23"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -3954,10 +4035,12 @@
     <col min="9" max="9" width="31.453125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="10.453125" customWidth="1"/>
     <col min="11" max="11" width="21" customWidth="1"/>
-    <col min="12" max="12" width="9.7265625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.54296875" customWidth="1"/>
+    <col min="13" max="13" width="16.54296875" customWidth="1"/>
+    <col min="14" max="14" width="9.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:15">
       <c r="A1" s="1" t="s">
         <v>211</v>
       </c>
@@ -3992,13 +4075,19 @@
         <v>245</v>
       </c>
       <c r="L1" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="2" spans="1:13">
+    <row r="2" spans="1:15">
       <c r="A2" s="1" t="s">
         <v>175</v>
       </c>
@@ -4028,14 +4117,20 @@
         <v>1</v>
       </c>
       <c r="K2" s="1"/>
-      <c r="L2" s="2">
+      <c r="L2" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="N2" s="2">
         <v>1223</v>
       </c>
-      <c r="M2" s="1">
+      <c r="O2" s="1">
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:13">
+    <row r="3" spans="1:15">
       <c r="A3" s="1" t="s">
         <v>182</v>
       </c>
@@ -4065,14 +4160,20 @@
         <v>1</v>
       </c>
       <c r="K3" s="1"/>
-      <c r="L3" s="1">
+      <c r="L3" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="N3" s="1">
         <v>1224</v>
       </c>
-      <c r="M3" s="1">
+      <c r="O3" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:13">
+    <row r="4" spans="1:15">
       <c r="A4" s="1" t="s">
         <v>185</v>
       </c>
@@ -4102,22 +4203,28 @@
         <v>1</v>
       </c>
       <c r="K4" s="1"/>
-      <c r="L4" s="2">
+      <c r="L4" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="N4" s="2">
         <v>1225</v>
       </c>
-      <c r="M4" s="1">
+      <c r="O4" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:13">
+    <row r="5" spans="1:15">
       <c r="A5" s="1" t="s">
-        <v>188</v>
+        <v>251</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>232</v>
+        <v>252</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>186</v>
+        <v>176</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1" t="s">
@@ -4139,19 +4246,25 @@
         <v>1</v>
       </c>
       <c r="K5" s="1"/>
-      <c r="L5" s="1">
-        <v>1226</v>
-      </c>
-      <c r="M5" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13">
+      <c r="L5" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="N5" s="1">
+        <v>1225</v>
+      </c>
+      <c r="O5" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15">
       <c r="A6" s="1" t="s">
-        <v>189</v>
+        <v>265</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>233</v>
+        <v>253</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>176</v>
@@ -4161,71 +4274,83 @@
         <v>177</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>190</v>
+        <v>178</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>191</v>
+        <v>183</v>
       </c>
       <c r="H6" s="1" t="s">
         <v>180</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="J6" s="1">
         <v>1</v>
       </c>
       <c r="K6" s="1"/>
-      <c r="L6" s="2">
-        <v>1223</v>
-      </c>
-      <c r="M6" s="1">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13">
+      <c r="L6" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="N6" s="1">
+        <v>1227</v>
+      </c>
+      <c r="O6" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15">
       <c r="A7" s="1" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>176</v>
+        <v>186</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1" t="s">
         <v>177</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>194</v>
+        <v>178</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>195</v>
+        <v>183</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>196</v>
+        <v>180</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>197</v>
+        <v>187</v>
       </c>
       <c r="J7" s="1">
         <v>1</v>
       </c>
       <c r="K7" s="1"/>
-      <c r="L7" s="1">
-        <v>1223</v>
-      </c>
-      <c r="M7" s="1">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13">
+      <c r="L7" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="N7" s="1">
+        <v>1226</v>
+      </c>
+      <c r="O7" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15">
       <c r="A8" s="1" t="s">
-        <v>198</v>
+        <v>189</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>176</v>
@@ -4235,34 +4360,40 @@
         <v>177</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>178</v>
+        <v>190</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>200</v>
+        <v>180</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
       <c r="J8" s="1">
         <v>1</v>
       </c>
       <c r="K8" s="1"/>
-      <c r="L8" s="2">
-        <v>1229</v>
-      </c>
-      <c r="M8" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13">
+      <c r="L8" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="N8" s="2">
+        <v>1223</v>
+      </c>
+      <c r="O8" s="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15">
       <c r="A9" s="1" t="s">
-        <v>202</v>
+        <v>193</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>176</v>
@@ -4272,34 +4403,40 @@
         <v>177</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>178</v>
+        <v>194</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="J9" s="1">
         <v>1</v>
       </c>
       <c r="K9" s="1"/>
-      <c r="L9" s="1">
-        <v>1230</v>
-      </c>
-      <c r="M9" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13">
+      <c r="L9" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="N9" s="1">
+        <v>1223</v>
+      </c>
+      <c r="O9" s="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15">
       <c r="A10" s="1" t="s">
-        <v>203</v>
+        <v>259</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>237</v>
+        <v>262</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>176</v>
@@ -4309,34 +4446,40 @@
         <v>177</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>178</v>
+        <v>190</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>200</v>
+        <v>180</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>204</v>
+        <v>192</v>
       </c>
       <c r="J10" s="1">
         <v>1</v>
       </c>
       <c r="K10" s="1"/>
-      <c r="L10" s="2">
-        <v>1231</v>
-      </c>
-      <c r="M10" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13">
+      <c r="L10" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="M10" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="N10" s="2">
+        <v>1226</v>
+      </c>
+      <c r="O10" s="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15">
       <c r="A11" s="1" t="s">
-        <v>205</v>
+        <v>260</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>238</v>
+        <v>263</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>176</v>
@@ -4346,34 +4489,40 @@
         <v>177</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>190</v>
+        <v>194</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>206</v>
+        <v>195</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>207</v>
+        <v>197</v>
       </c>
       <c r="J11" s="1">
         <v>1</v>
       </c>
       <c r="K11" s="1"/>
-      <c r="L11" s="1">
-        <v>1231</v>
-      </c>
-      <c r="M11" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13">
+      <c r="L11" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="M11" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="N11" s="1">
+        <v>1226</v>
+      </c>
+      <c r="O11" s="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15">
       <c r="A12" s="1" t="s">
-        <v>208</v>
+        <v>261</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>239</v>
+        <v>264</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>176</v>
@@ -4383,68 +4532,513 @@
         <v>177</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>190</v>
+        <v>178</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>206</v>
+        <v>179</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>200</v>
+        <v>180</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>207</v>
+        <v>181</v>
       </c>
       <c r="J12" s="1">
         <v>1</v>
       </c>
       <c r="K12" s="1"/>
-      <c r="L12" s="2">
-        <v>1224</v>
-      </c>
-      <c r="M12" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13">
+      <c r="L12" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="M12" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="N12" s="2">
+        <v>1226</v>
+      </c>
+      <c r="O12" s="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15">
       <c r="A13" s="1" t="s">
-        <v>209</v>
+        <v>198</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>242</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>243</v>
-      </c>
+        <v>176</v>
+      </c>
+      <c r="D13" s="1"/>
       <c r="E13" s="1" t="s">
         <v>177</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>190</v>
+        <v>178</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
       <c r="H13" s="1" t="s">
         <v>200</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>210</v>
+        <v>201</v>
       </c>
       <c r="J13" s="1">
         <v>1</v>
       </c>
       <c r="K13" s="1"/>
-      <c r="L13" s="1">
+      <c r="L13" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="M13" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="N13" s="2">
+        <v>1229</v>
+      </c>
+      <c r="O13" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15">
+      <c r="A14" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="J14" s="1">
+        <v>1</v>
+      </c>
+      <c r="K14" s="1"/>
+      <c r="L14" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="M14" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="N14" s="1">
+        <v>1230</v>
+      </c>
+      <c r="O14" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15">
+      <c r="A15" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="J15" s="1">
+        <v>1</v>
+      </c>
+      <c r="K15" s="1"/>
+      <c r="L15" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="M15" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="N15" s="2">
+        <v>1231</v>
+      </c>
+      <c r="O15" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15">
+      <c r="A16" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="J16" s="1">
+        <v>1</v>
+      </c>
+      <c r="K16" s="1"/>
+      <c r="L16" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="M16" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="N16" s="1">
+        <v>1231</v>
+      </c>
+      <c r="O16" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15">
+      <c r="A17" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="J17" s="1">
+        <v>1</v>
+      </c>
+      <c r="K17" s="1"/>
+      <c r="L17" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="M17" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="N17" s="2">
+        <v>1224</v>
+      </c>
+      <c r="O17" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15">
+      <c r="A18" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="J18" s="1">
+        <v>1</v>
+      </c>
+      <c r="K18" s="1"/>
+      <c r="L18" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="M18" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="N18" s="1">
         <v>1225</v>
       </c>
-      <c r="M13" s="1">
+      <c r="O18" s="1">
         <v>1</v>
       </c>
     </row>
+    <row r="19" spans="1:15">
+      <c r="A19" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="J19" s="1">
+        <v>1</v>
+      </c>
+      <c r="K19" s="1"/>
+      <c r="L19" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="M19" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="N19" s="1">
+        <v>1226</v>
+      </c>
+      <c r="O19" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15">
+      <c r="A20" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="J20" s="1">
+        <v>1</v>
+      </c>
+      <c r="K20" s="1"/>
+      <c r="L20" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="M20" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="N20" s="1">
+        <v>1223</v>
+      </c>
+      <c r="O20" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15">
+      <c r="A21" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="J21" s="1">
+        <v>1</v>
+      </c>
+      <c r="K21" s="1"/>
+      <c r="L21" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="M21" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="N21" s="1">
+        <v>1229</v>
+      </c>
+      <c r="O21" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15">
+      <c r="A22" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="J22" s="1">
+        <v>1</v>
+      </c>
+      <c r="K22" s="1"/>
+      <c r="L22" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="M22" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="N22" s="1">
+        <v>1228</v>
+      </c>
+      <c r="O22" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15">
+      <c r="A23" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="J23" s="1">
+        <v>1</v>
+      </c>
+      <c r="K23" s="1"/>
+      <c r="L23" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="M23" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="N23" s="1">
+        <v>1227</v>
+      </c>
+      <c r="O23" s="1">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
[WORKING] auto-email when user finishes opname to the L1 support team and to the user themselves. need a report page for L1 support to verify and view opname recap. report page will also be for the site's opname history (can be viewed by other users).
</commit_message>
<xml_diff>
--- a/backend/internal/seed/seed_data/mst_dummy_data.xlsx
+++ b/backend/internal/seed/seed_data/mst_dummy_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Uni\Intern SM\Stock Opname App [SOSMIT]\SOSMIT\backend\internal\seed\seed_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DA5DA70-1B07-4346-AD77-3CA027B1CC16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46463A74-245A-44CC-A4DA-DFDD648689EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10540" firstSheet="1" activeTab="5" xr2:uid="{AF28B77B-5B1D-47C2-ADE5-ADF50DA09BCF}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10540" firstSheet="1" activeTab="3" xr2:uid="{AF28B77B-5B1D-47C2-ADE5-ADF50DA09BCF}"/>
   </bookViews>
   <sheets>
     <sheet name="Region" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="517" uniqueCount="272">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="530" uniqueCount="275">
   <si>
     <t>id</t>
   </si>
@@ -857,13 +857,22 @@
   </si>
   <si>
     <t>Lost</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>samistheguns@gmail.com</t>
+  </si>
+  <si>
+    <t>likarsaaimee@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -888,6 +897,14 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -925,11 +942,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -947,8 +965,10 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="2" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{AFBE5B6D-05B3-4F9B-9E00-733992E0CE0A}"/>
   </cellStyles>
@@ -3003,7 +3023,7 @@
       </c>
       <c r="D10" s="1">
         <f ca="1">RANDBETWEEN(1223,1232)</f>
-        <v>1228</v>
+        <v>1224</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -3018,7 +3038,7 @@
       </c>
       <c r="D11" s="1">
         <f t="shared" ref="D11:D51" ca="1" si="0">RANDBETWEEN(1223,1232)</f>
-        <v>1227</v>
+        <v>1223</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -3033,7 +3053,7 @@
       </c>
       <c r="D12" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1225</v>
+        <v>1229</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -3048,7 +3068,7 @@
       </c>
       <c r="D13" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1228</v>
+        <v>1231</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -3063,7 +3083,7 @@
       </c>
       <c r="D14" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1230</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -3078,7 +3098,7 @@
       </c>
       <c r="D15" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1226</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -3093,7 +3113,7 @@
       </c>
       <c r="D16" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1226</v>
+        <v>1231</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -3108,7 +3128,7 @@
       </c>
       <c r="D17" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1223</v>
+        <v>1230</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -3123,7 +3143,7 @@
       </c>
       <c r="D18" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1226</v>
+        <v>1232</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -3138,7 +3158,7 @@
       </c>
       <c r="D19" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1232</v>
+        <v>1230</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -3153,7 +3173,7 @@
       </c>
       <c r="D20" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1223</v>
+        <v>1229</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -3168,7 +3188,7 @@
       </c>
       <c r="D21" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1224</v>
+        <v>1225</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -3183,7 +3203,7 @@
       </c>
       <c r="D22" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1225</v>
+        <v>1229</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -3198,7 +3218,7 @@
       </c>
       <c r="D23" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1230</v>
+        <v>1224</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -3213,7 +3233,7 @@
       </c>
       <c r="D24" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1231</v>
+        <v>1224</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -3243,7 +3263,7 @@
       </c>
       <c r="D26" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1228</v>
+        <v>1231</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -3258,7 +3278,7 @@
       </c>
       <c r="D27" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1230</v>
+        <v>1231</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -3273,7 +3293,7 @@
       </c>
       <c r="D28" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1230</v>
+        <v>1223</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -3288,7 +3308,7 @@
       </c>
       <c r="D29" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1229</v>
+        <v>1231</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -3303,7 +3323,7 @@
       </c>
       <c r="D30" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1226</v>
+        <v>1225</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -3318,7 +3338,7 @@
       </c>
       <c r="D31" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1226</v>
+        <v>1232</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -3333,7 +3353,7 @@
       </c>
       <c r="D32" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1224</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="33" spans="1:4">
@@ -3348,7 +3368,7 @@
       </c>
       <c r="D33" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1223</v>
+        <v>1231</v>
       </c>
     </row>
     <row r="34" spans="1:4">
@@ -3363,7 +3383,7 @@
       </c>
       <c r="D34" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1228</v>
+        <v>1226</v>
       </c>
     </row>
     <row r="35" spans="1:4">
@@ -3378,7 +3398,7 @@
       </c>
       <c r="D35" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1228</v>
+        <v>1231</v>
       </c>
     </row>
     <row r="36" spans="1:4">
@@ -3393,7 +3413,7 @@
       </c>
       <c r="D36" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1224</v>
+        <v>1226</v>
       </c>
     </row>
     <row r="37" spans="1:4">
@@ -3423,7 +3443,7 @@
       </c>
       <c r="D38" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1231</v>
+        <v>1232</v>
       </c>
     </row>
     <row r="39" spans="1:4">
@@ -3438,7 +3458,7 @@
       </c>
       <c r="D39" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1231</v>
+        <v>1229</v>
       </c>
     </row>
     <row r="40" spans="1:4">
@@ -3453,7 +3473,7 @@
       </c>
       <c r="D40" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1229</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="41" spans="1:4">
@@ -3468,7 +3488,7 @@
       </c>
       <c r="D41" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1231</v>
+        <v>1225</v>
       </c>
     </row>
     <row r="42" spans="1:4">
@@ -3483,7 +3503,7 @@
       </c>
       <c r="D42" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1225</v>
+        <v>1231</v>
       </c>
     </row>
     <row r="43" spans="1:4">
@@ -3498,7 +3518,7 @@
       </c>
       <c r="D43" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1223</v>
+        <v>1229</v>
       </c>
     </row>
     <row r="44" spans="1:4">
@@ -3513,7 +3533,7 @@
       </c>
       <c r="D44" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1224</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="45" spans="1:4">
@@ -3528,7 +3548,7 @@
       </c>
       <c r="D45" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1223</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="46" spans="1:4">
@@ -3543,7 +3563,7 @@
       </c>
       <c r="D46" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1225</v>
+        <v>1229</v>
       </c>
     </row>
     <row r="47" spans="1:4">
@@ -3558,7 +3578,7 @@
       </c>
       <c r="D47" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1224</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="48" spans="1:4">
@@ -3573,7 +3593,7 @@
       </c>
       <c r="D48" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1229</v>
+        <v>1223</v>
       </c>
     </row>
     <row r="49" spans="1:4">
@@ -3588,7 +3608,7 @@
       </c>
       <c r="D49" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1227</v>
+        <v>1232</v>
       </c>
     </row>
     <row r="50" spans="1:4">
@@ -3603,7 +3623,7 @@
       </c>
       <c r="D50" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1226</v>
+        <v>1229</v>
       </c>
     </row>
     <row r="51" spans="1:4">
@@ -3618,7 +3638,7 @@
       </c>
       <c r="D51" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1227</v>
+        <v>1229</v>
       </c>
     </row>
   </sheetData>
@@ -3628,23 +3648,24 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6E05CD4-7C76-4891-A9C7-AB36831BB0B8}">
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="2" max="2" width="9.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.453125" customWidth="1"/>
-    <col min="4" max="4" width="13.7265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="34.7265625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.36328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.453125" customWidth="1"/>
+    <col min="4" max="4" width="13.453125" customWidth="1"/>
+    <col min="5" max="5" width="13.7265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="34.7265625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.36328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:8">
       <c r="A1" s="8" t="s">
         <v>132</v>
       </c>
@@ -3652,298 +3673,342 @@
         <v>226</v>
       </c>
       <c r="C1" s="8" t="s">
+        <v>272</v>
+      </c>
+      <c r="D1" s="8" t="s">
         <v>134</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="E1" s="8" t="s">
         <v>135</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="F1" s="8" t="s">
         <v>227</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="G1" s="8" t="s">
         <v>133</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="H1" s="8" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:8">
       <c r="A2" s="6">
         <v>1223</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>137</v>
+      <c r="C2" s="9" t="s">
+        <v>273</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="F2" s="8" t="s">
         <v>138</v>
       </c>
-      <c r="F2" s="7">
+      <c r="G2" s="7">
         <v>30</v>
       </c>
-      <c r="G2" s="8">
+      <c r="H2" s="8">
         <v>110</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:8">
       <c r="A3" s="8">
         <v>1224</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="9" t="s">
+        <v>273</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="E3" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="F3" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="F3" s="7">
+      <c r="G3" s="7">
         <v>2</v>
       </c>
-      <c r="G3" s="8">
+      <c r="H3" s="8">
         <v>240</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:8">
       <c r="A4" s="6">
         <v>1225</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="9" t="s">
+        <v>273</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="E4" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="F4" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="F4" s="7">
+      <c r="G4" s="7">
         <v>3</v>
       </c>
-      <c r="G4" s="8">
+      <c r="H4" s="8">
         <v>230</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:8">
       <c r="A5" s="8">
         <v>1226</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="9" t="s">
+        <v>273</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="E5" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="F5" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="F5" s="7">
+      <c r="G5" s="7">
         <v>3</v>
       </c>
-      <c r="G5" s="8">
+      <c r="H5" s="8">
         <v>240</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:8">
       <c r="A6" s="6">
         <v>1227</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="9" t="s">
+        <v>273</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="E6" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="F6" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="F6" s="7">
+      <c r="G6" s="7">
         <v>1</v>
       </c>
-      <c r="G6" s="8">
+      <c r="H6" s="8">
         <v>240</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:8">
       <c r="A7" s="8">
         <v>1228</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="9" t="s">
+        <v>273</v>
+      </c>
+      <c r="D7" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="E7" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="F7" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="F7" s="7">
+      <c r="G7" s="7">
         <v>1</v>
       </c>
-      <c r="G7" s="8">
+      <c r="H7" s="8">
         <v>240</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:8">
       <c r="A8" s="6">
         <v>1229</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>156</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="9" t="s">
+        <v>273</v>
+      </c>
+      <c r="D8" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="E8" s="3" t="s">
         <v>159</v>
       </c>
-      <c r="E8" s="8" t="s">
+      <c r="F8" s="8" t="s">
         <v>157</v>
       </c>
-      <c r="F8" s="7">
+      <c r="G8" s="7">
         <v>1</v>
       </c>
-      <c r="G8" s="8">
+      <c r="H8" s="8">
         <v>230</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:8">
       <c r="A9" s="8">
         <v>1230</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>160</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="9" t="s">
+        <v>273</v>
+      </c>
+      <c r="D9" s="3" t="s">
         <v>161</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="E9" s="3" t="s">
         <v>162</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="F9" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="F9" s="7">
+      <c r="G9" s="7">
         <v>1</v>
       </c>
-      <c r="G9" s="8">
+      <c r="H9" s="8">
         <v>230</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:8">
       <c r="A10" s="6">
         <v>1231</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>163</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="9" t="s">
+        <v>273</v>
+      </c>
+      <c r="D10" s="3" t="s">
         <v>164</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="E10" s="3" t="s">
         <v>165</v>
       </c>
-      <c r="E10" s="8" t="s">
+      <c r="F10" s="8" t="s">
         <v>157</v>
       </c>
-      <c r="F10" s="7">
+      <c r="G10" s="7">
         <v>1</v>
       </c>
-      <c r="G10" s="8">
+      <c r="H10" s="8">
         <v>230</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:8">
       <c r="A11" s="8">
         <v>1232</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>166</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="9" t="s">
+        <v>273</v>
+      </c>
+      <c r="D11" s="3" t="s">
         <v>167</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="E11" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="E11" s="8" t="s">
+      <c r="F11" s="8" t="s">
         <v>138</v>
       </c>
-      <c r="F11" s="8">
+      <c r="G11" s="8">
         <v>30</v>
       </c>
-      <c r="G11" s="8">
+      <c r="H11" s="8">
         <v>110</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:8">
       <c r="A12" s="8">
         <v>1233</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>168</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="9" t="s">
+        <v>273</v>
+      </c>
+      <c r="D12" s="3" t="s">
         <v>170</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="E12" s="3" t="s">
         <v>171</v>
       </c>
-      <c r="E12" s="8" t="s">
+      <c r="F12" s="8" t="s">
         <v>169</v>
       </c>
-      <c r="F12" s="8">
+      <c r="G12" s="8">
         <v>4</v>
       </c>
-      <c r="G12" s="8">
+      <c r="H12" s="8">
         <v>350</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:8">
       <c r="A13" s="8">
         <v>1234</v>
       </c>
       <c r="B13" s="8" t="s">
         <v>172</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" s="9" t="s">
+        <v>274</v>
+      </c>
+      <c r="D13" s="3" t="s">
         <v>172</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="E13" s="3" t="s">
         <v>174</v>
       </c>
-      <c r="E13" s="8" t="s">
+      <c r="F13" s="8" t="s">
         <v>173</v>
       </c>
-      <c r="F13" s="8">
+      <c r="G13" s="8">
         <v>30</v>
       </c>
-      <c r="G13" s="8">
+      <c r="H13" s="8">
         <v>110</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{326C7255-3775-42C0-8CED-A0F3BD8EC552}"/>
+    <hyperlink ref="C3:C13" r:id="rId2" display="samistheguns@gmail.com" xr:uid="{3CAD1B5D-2B42-47EB-9EF7-1EF55230C6A8}"/>
+    <hyperlink ref="C13" r:id="rId3" xr:uid="{40AAA3FD-0326-450A-BB81-B7DCF8FF78DD}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -4019,7 +4084,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{491D14EC-1CB1-4681-930A-4B9B4015FC83}">
   <dimension ref="A1:O23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
refactored the code to handle asset equpiments and added business logic for the opname verification process, now area managers should verify first before sending it to L1 support and they have access as well.
</commit_message>
<xml_diff>
--- a/backend/internal/seed/seed_data/mst_dummy_data.xlsx
+++ b/backend/internal/seed/seed_data/mst_dummy_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Uni\Intern SM\Stock Opname App [SOSMIT]\SOSMIT\backend\internal\seed\seed_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46463A74-245A-44CC-A4DA-DFDD648689EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B741DB89-E599-4721-B60B-0ECBCC8C075E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10540" firstSheet="1" activeTab="3" xr2:uid="{AF28B77B-5B1D-47C2-ADE5-ADF50DA09BCF}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10540" firstSheet="1" activeTab="5" xr2:uid="{AF28B77B-5B1D-47C2-ADE5-ADF50DA09BCF}"/>
   </bookViews>
   <sheets>
     <sheet name="Region" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="530" uniqueCount="275">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="558" uniqueCount="285">
   <si>
     <t>id</t>
   </si>
@@ -865,7 +865,37 @@
     <t>samistheguns@gmail.com</t>
   </si>
   <si>
-    <t>likarsaaimee@gmail.com</t>
+    <t>RADITYA</t>
+  </si>
+  <si>
+    <t>DIKA</t>
+  </si>
+  <si>
+    <t>AREA MANAGER</t>
+  </si>
+  <si>
+    <t>equipment</t>
+  </si>
+  <si>
+    <t>Kabel power, Adaptor</t>
+  </si>
+  <si>
+    <t>Tas</t>
+  </si>
+  <si>
+    <t>Kabel power</t>
+  </si>
+  <si>
+    <t>Kabel power, Kabel VGA</t>
+  </si>
+  <si>
+    <t>Simcard, Handstrap, Adaptor, Kabel USB</t>
+  </si>
+  <si>
+    <t>Simcard, Adaptor, Kabel USB</t>
+  </si>
+  <si>
+    <t>Tas, Tali tas, Adaptor, Kabel USB</t>
   </si>
 </sst>
 </file>
@@ -918,7 +948,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -941,13 +971,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -966,6 +1007,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -3023,7 +3067,7 @@
       </c>
       <c r="D10" s="1">
         <f ca="1">RANDBETWEEN(1223,1232)</f>
-        <v>1224</v>
+        <v>1223</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -3038,7 +3082,7 @@
       </c>
       <c r="D11" s="1">
         <f t="shared" ref="D11:D51" ca="1" si="0">RANDBETWEEN(1223,1232)</f>
-        <v>1223</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -3053,7 +3097,7 @@
       </c>
       <c r="D12" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1229</v>
+        <v>1224</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -3068,7 +3112,7 @@
       </c>
       <c r="D13" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1231</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -3083,7 +3127,7 @@
       </c>
       <c r="D14" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1228</v>
+        <v>1225</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -3113,7 +3157,7 @@
       </c>
       <c r="D16" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1231</v>
+        <v>1232</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -3128,7 +3172,7 @@
       </c>
       <c r="D17" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1230</v>
+        <v>1232</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -3143,7 +3187,7 @@
       </c>
       <c r="D18" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1232</v>
+        <v>1226</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -3158,7 +3202,7 @@
       </c>
       <c r="D19" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1230</v>
+        <v>1224</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -3188,7 +3232,7 @@
       </c>
       <c r="D21" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1225</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -3203,7 +3247,7 @@
       </c>
       <c r="D22" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1229</v>
+        <v>1232</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -3218,7 +3262,7 @@
       </c>
       <c r="D23" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1224</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -3233,7 +3277,7 @@
       </c>
       <c r="D24" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1224</v>
+        <v>1231</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -3248,7 +3292,7 @@
       </c>
       <c r="D25" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1228</v>
+        <v>1225</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -3263,7 +3307,7 @@
       </c>
       <c r="D26" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1231</v>
+        <v>1225</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -3278,7 +3322,7 @@
       </c>
       <c r="D27" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1231</v>
+        <v>1226</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -3293,7 +3337,7 @@
       </c>
       <c r="D28" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1223</v>
+        <v>1231</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -3308,7 +3352,7 @@
       </c>
       <c r="D29" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1231</v>
+        <v>1229</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -3323,7 +3367,7 @@
       </c>
       <c r="D30" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1225</v>
+        <v>1223</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -3338,7 +3382,7 @@
       </c>
       <c r="D31" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1232</v>
+        <v>1224</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -3353,7 +3397,7 @@
       </c>
       <c r="D32" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1228</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="33" spans="1:4">
@@ -3368,7 +3412,7 @@
       </c>
       <c r="D33" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1231</v>
+        <v>1232</v>
       </c>
     </row>
     <row r="34" spans="1:4">
@@ -3383,7 +3427,7 @@
       </c>
       <c r="D34" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1226</v>
+        <v>1225</v>
       </c>
     </row>
     <row r="35" spans="1:4">
@@ -3398,7 +3442,7 @@
       </c>
       <c r="D35" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1231</v>
+        <v>1224</v>
       </c>
     </row>
     <row r="36" spans="1:4">
@@ -3428,7 +3472,7 @@
       </c>
       <c r="D37" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1225</v>
+        <v>1226</v>
       </c>
     </row>
     <row r="38" spans="1:4">
@@ -3443,7 +3487,7 @@
       </c>
       <c r="D38" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1232</v>
+        <v>1230</v>
       </c>
     </row>
     <row r="39" spans="1:4">
@@ -3458,7 +3502,7 @@
       </c>
       <c r="D39" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1229</v>
+        <v>1231</v>
       </c>
     </row>
     <row r="40" spans="1:4">
@@ -3473,7 +3517,7 @@
       </c>
       <c r="D40" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1227</v>
+        <v>1232</v>
       </c>
     </row>
     <row r="41" spans="1:4">
@@ -3488,7 +3532,7 @@
       </c>
       <c r="D41" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1225</v>
+        <v>1224</v>
       </c>
     </row>
     <row r="42" spans="1:4">
@@ -3503,7 +3547,7 @@
       </c>
       <c r="D42" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1231</v>
+        <v>1225</v>
       </c>
     </row>
     <row r="43" spans="1:4">
@@ -3518,7 +3562,7 @@
       </c>
       <c r="D43" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1229</v>
+        <v>1232</v>
       </c>
     </row>
     <row r="44" spans="1:4">
@@ -3548,7 +3592,7 @@
       </c>
       <c r="D45" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1227</v>
+        <v>1231</v>
       </c>
     </row>
     <row r="46" spans="1:4">
@@ -3563,7 +3607,7 @@
       </c>
       <c r="D46" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1229</v>
+        <v>1230</v>
       </c>
     </row>
     <row r="47" spans="1:4">
@@ -3578,7 +3622,7 @@
       </c>
       <c r="D47" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1228</v>
+        <v>1223</v>
       </c>
     </row>
     <row r="48" spans="1:4">
@@ -3593,7 +3637,7 @@
       </c>
       <c r="D48" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1223</v>
+        <v>1229</v>
       </c>
     </row>
     <row r="49" spans="1:4">
@@ -3638,7 +3682,7 @@
       </c>
       <c r="D51" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1229</v>
+        <v>1228</v>
       </c>
     </row>
   </sheetData>
@@ -3648,10 +3692,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6E05CD4-7C76-4891-A9C7-AB36831BB0B8}">
-  <dimension ref="A1:H13"/>
+  <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -3740,7 +3784,7 @@
         <v>2</v>
       </c>
       <c r="H3" s="8">
-        <v>240</v>
+        <v>410</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -3766,7 +3810,7 @@
         <v>3</v>
       </c>
       <c r="H4" s="8">
-        <v>230</v>
+        <v>240</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -3818,7 +3862,7 @@
         <v>1</v>
       </c>
       <c r="H6" s="8">
-        <v>240</v>
+        <v>230</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -3844,7 +3888,7 @@
         <v>1</v>
       </c>
       <c r="H7" s="8">
-        <v>240</v>
+        <v>230</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -3985,7 +4029,7 @@
         <v>172</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>172</v>
@@ -4001,13 +4045,38 @@
       </c>
       <c r="H13" s="8">
         <v>110</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" s="10">
+        <v>1235</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>274</v>
+      </c>
+      <c r="C14" s="12" t="s">
+        <v>273</v>
+      </c>
+      <c r="D14" s="11" t="s">
+        <v>274</v>
+      </c>
+      <c r="E14" s="11" t="s">
+        <v>275</v>
+      </c>
+      <c r="F14" s="10" t="s">
+        <v>276</v>
+      </c>
+      <c r="G14" s="10">
+        <v>1</v>
+      </c>
+      <c r="H14" s="10">
+        <v>230</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" xr:uid="{326C7255-3775-42C0-8CED-A0F3BD8EC552}"/>
-    <hyperlink ref="C3:C13" r:id="rId2" display="samistheguns@gmail.com" xr:uid="{3CAD1B5D-2B42-47EB-9EF7-1EF55230C6A8}"/>
-    <hyperlink ref="C13" r:id="rId3" xr:uid="{40AAA3FD-0326-450A-BB81-B7DCF8FF78DD}"/>
+    <hyperlink ref="C14" r:id="rId2" xr:uid="{3075A95B-B014-4146-9A02-CE8105DDA61C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4082,10 +4151,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{491D14EC-1CB1-4681-930A-4B9B4015FC83}">
-  <dimension ref="A1:O23"/>
+  <dimension ref="A1:P23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="N21" sqref="N21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -4101,11 +4170,11 @@
     <col min="10" max="10" width="10.453125" customWidth="1"/>
     <col min="11" max="11" width="21" customWidth="1"/>
     <col min="12" max="12" width="14.54296875" customWidth="1"/>
-    <col min="13" max="13" width="16.54296875" customWidth="1"/>
-    <col min="14" max="14" width="9.7265625" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="16.54296875" customWidth="1"/>
+    <col min="15" max="15" width="9.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:16">
       <c r="A1" s="1" t="s">
         <v>211</v>
       </c>
@@ -4146,13 +4215,16 @@
         <v>248</v>
       </c>
       <c r="N1" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="O1" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="2" spans="1:15">
+    <row r="2" spans="1:16">
       <c r="A2" s="1" t="s">
         <v>175</v>
       </c>
@@ -4188,14 +4260,17 @@
       <c r="M2" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="N2" s="2">
+      <c r="N2" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="O2" s="2">
         <v>1223</v>
       </c>
-      <c r="O2" s="1">
+      <c r="P2" s="1">
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:15">
+    <row r="3" spans="1:16">
       <c r="A3" s="1" t="s">
         <v>182</v>
       </c>
@@ -4231,14 +4306,17 @@
       <c r="M3" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="N3" s="1">
+      <c r="N3" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="O3" s="1">
         <v>1224</v>
       </c>
-      <c r="O3" s="1">
+      <c r="P3" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:15">
+    <row r="4" spans="1:16">
       <c r="A4" s="1" t="s">
         <v>185</v>
       </c>
@@ -4274,14 +4352,17 @@
       <c r="M4" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="N4" s="2">
+      <c r="N4" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="O4" s="2">
         <v>1225</v>
       </c>
-      <c r="O4" s="1">
+      <c r="P4" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:15">
+    <row r="5" spans="1:16">
       <c r="A5" s="1" t="s">
         <v>251</v>
       </c>
@@ -4317,14 +4398,17 @@
       <c r="M5" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="N5" s="1">
+      <c r="N5" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="O5" s="1">
         <v>1225</v>
       </c>
-      <c r="O5" s="1">
+      <c r="P5" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:15">
+    <row r="6" spans="1:16">
       <c r="A6" s="1" t="s">
         <v>265</v>
       </c>
@@ -4360,14 +4444,17 @@
       <c r="M6" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="N6" s="1">
+      <c r="N6" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="O6" s="1">
         <v>1227</v>
       </c>
-      <c r="O6" s="1">
+      <c r="P6" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:15">
+    <row r="7" spans="1:16">
       <c r="A7" s="1" t="s">
         <v>188</v>
       </c>
@@ -4403,14 +4490,17 @@
       <c r="M7" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="N7" s="1">
+      <c r="N7" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="O7" s="1">
         <v>1226</v>
       </c>
-      <c r="O7" s="1">
+      <c r="P7" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:15">
+    <row r="8" spans="1:16">
       <c r="A8" s="1" t="s">
         <v>189</v>
       </c>
@@ -4446,14 +4536,17 @@
       <c r="M8" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="N8" s="2">
+      <c r="N8" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="O8" s="2">
         <v>1223</v>
       </c>
-      <c r="O8" s="1">
+      <c r="P8" s="1">
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:15">
+    <row r="9" spans="1:16">
       <c r="A9" s="1" t="s">
         <v>193</v>
       </c>
@@ -4489,14 +4582,17 @@
       <c r="M9" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="N9" s="1">
+      <c r="N9" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="O9" s="1">
         <v>1223</v>
       </c>
-      <c r="O9" s="1">
+      <c r="P9" s="1">
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:15">
+    <row r="10" spans="1:16">
       <c r="A10" s="1" t="s">
         <v>259</v>
       </c>
@@ -4532,14 +4628,17 @@
       <c r="M10" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="N10" s="2">
+      <c r="N10" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="O10" s="2">
         <v>1226</v>
       </c>
-      <c r="O10" s="1">
+      <c r="P10" s="1">
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:15">
+    <row r="11" spans="1:16">
       <c r="A11" s="1" t="s">
         <v>260</v>
       </c>
@@ -4575,14 +4674,17 @@
       <c r="M11" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="N11" s="1">
+      <c r="N11" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="O11" s="1">
         <v>1226</v>
       </c>
-      <c r="O11" s="1">
+      <c r="P11" s="1">
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:15">
+    <row r="12" spans="1:16">
       <c r="A12" s="1" t="s">
         <v>261</v>
       </c>
@@ -4618,14 +4720,17 @@
       <c r="M12" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="N12" s="2">
+      <c r="N12" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="O12" s="2">
         <v>1226</v>
       </c>
-      <c r="O12" s="1">
+      <c r="P12" s="1">
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:15">
+    <row r="13" spans="1:16">
       <c r="A13" s="1" t="s">
         <v>198</v>
       </c>
@@ -4661,14 +4766,17 @@
       <c r="M13" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="N13" s="2">
+      <c r="N13" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="O13" s="2">
         <v>1229</v>
       </c>
-      <c r="O13" s="1">
+      <c r="P13" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:15">
+    <row r="14" spans="1:16">
       <c r="A14" s="1" t="s">
         <v>202</v>
       </c>
@@ -4704,14 +4812,17 @@
       <c r="M14" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="N14" s="1">
+      <c r="N14" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="O14" s="1">
         <v>1230</v>
       </c>
-      <c r="O14" s="1">
+      <c r="P14" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:15">
+    <row r="15" spans="1:16">
       <c r="A15" s="1" t="s">
         <v>203</v>
       </c>
@@ -4747,14 +4858,17 @@
       <c r="M15" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="N15" s="2">
+      <c r="N15" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="O15" s="2">
         <v>1231</v>
       </c>
-      <c r="O15" s="1">
+      <c r="P15" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:15">
+    <row r="16" spans="1:16">
       <c r="A16" s="1" t="s">
         <v>205</v>
       </c>
@@ -4790,14 +4904,17 @@
       <c r="M16" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="N16" s="1">
+      <c r="N16" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="O16" s="1">
         <v>1231</v>
       </c>
-      <c r="O16" s="1">
+      <c r="P16" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:15">
+    <row r="17" spans="1:16">
       <c r="A17" s="1" t="s">
         <v>208</v>
       </c>
@@ -4833,14 +4950,17 @@
       <c r="M17" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="N17" s="2">
+      <c r="N17" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="O17" s="2">
         <v>1224</v>
       </c>
-      <c r="O17" s="1">
+      <c r="P17" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:15">
+    <row r="18" spans="1:16">
       <c r="A18" s="1" t="s">
         <v>209</v>
       </c>
@@ -4878,14 +4998,17 @@
       <c r="M18" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="N18" s="1">
+      <c r="N18" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="O18" s="1">
         <v>1225</v>
       </c>
-      <c r="O18" s="1">
+      <c r="P18" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:15">
+    <row r="19" spans="1:16">
       <c r="A19" s="1" t="s">
         <v>254</v>
       </c>
@@ -4923,14 +5046,17 @@
       <c r="M19" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="N19" s="1">
+      <c r="N19" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="O19" s="1">
         <v>1226</v>
       </c>
-      <c r="O19" s="1">
+      <c r="P19" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:15">
+    <row r="20" spans="1:16">
       <c r="A20" s="1" t="s">
         <v>255</v>
       </c>
@@ -4966,14 +5092,17 @@
       <c r="M20" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="N20" s="1">
+      <c r="N20" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="O20" s="1">
         <v>1223</v>
       </c>
-      <c r="O20" s="1">
+      <c r="P20" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:15">
+    <row r="21" spans="1:16">
       <c r="A21" s="1" t="s">
         <v>256</v>
       </c>
@@ -5009,14 +5138,17 @@
       <c r="M21" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="N21" s="1">
+      <c r="N21" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="O21" s="1">
         <v>1229</v>
       </c>
-      <c r="O21" s="1">
+      <c r="P21" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:15">
+    <row r="22" spans="1:16">
       <c r="A22" s="1" t="s">
         <v>257</v>
       </c>
@@ -5052,14 +5184,17 @@
       <c r="M22" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="N22" s="1">
+      <c r="N22" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="O22" s="1">
         <v>1228</v>
       </c>
-      <c r="O22" s="1">
+      <c r="P22" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:15">
+    <row r="23" spans="1:16">
       <c r="A23" s="1" t="s">
         <v>258</v>
       </c>
@@ -5095,10 +5230,13 @@
       <c r="M23" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="N23" s="1">
+      <c r="N23" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="O23" s="1">
         <v>1227</v>
       </c>
-      <c r="O23" s="1">
+      <c r="P23" s="1">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added data and removed site group duplicates.
</commit_message>
<xml_diff>
--- a/backend/internal/seed/seed_data/mst_dummy_data.xlsx
+++ b/backend/internal/seed/seed_data/mst_dummy_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Uni\Intern SM\Stock Opname App [SOSMIT]\SOSMIT\backend\internal\seed\seed_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B741DB89-E599-4721-B60B-0ECBCC8C075E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7E3DF17-8783-4E10-9600-5D4378BAF31A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10540" firstSheet="1" activeTab="5" xr2:uid="{AF28B77B-5B1D-47C2-ADE5-ADF50DA09BCF}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10540" activeTab="3" xr2:uid="{AF28B77B-5B1D-47C2-ADE5-ADF50DA09BCF}"/>
   </bookViews>
   <sheets>
     <sheet name="Region" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="558" uniqueCount="285">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="556" uniqueCount="300">
   <si>
     <t>id</t>
   </si>
@@ -868,9 +868,6 @@
     <t>RADITYA</t>
   </si>
   <si>
-    <t>DIKA</t>
-  </si>
-  <si>
     <t>AREA MANAGER</t>
   </si>
   <si>
@@ -896,6 +893,54 @@
   </si>
   <si>
     <t>Tas, Tali tas, Adaptor, Kabel USB</t>
+  </si>
+  <si>
+    <t>XXZHJ225436587</t>
+  </si>
+  <si>
+    <t>XXZHJ231525344</t>
+  </si>
+  <si>
+    <t>XXZWS48F95H39</t>
+  </si>
+  <si>
+    <t>XXZHJ23DFV3445</t>
+  </si>
+  <si>
+    <t>In Inventory</t>
+  </si>
+  <si>
+    <t>Down</t>
+  </si>
+  <si>
+    <t>SMPR00000009</t>
+  </si>
+  <si>
+    <t>SMPR00000010</t>
+  </si>
+  <si>
+    <t>SMPR00000011</t>
+  </si>
+  <si>
+    <t>SMPR00000012</t>
+  </si>
+  <si>
+    <t>DENY</t>
+  </si>
+  <si>
+    <t>SUMARGA</t>
+  </si>
+  <si>
+    <t>DENSU</t>
+  </si>
+  <si>
+    <t>DIPA</t>
+  </si>
+  <si>
+    <t>SHEILA</t>
+  </si>
+  <si>
+    <t>PARA</t>
   </si>
 </sst>
 </file>
@@ -948,7 +993,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -971,24 +1016,13 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1007,9 +1041,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="2" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -1348,8 +1379,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9239C4D5-8E93-45CD-8BEC-3AD8E34539C8}">
   <dimension ref="A1:B79"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -1996,10 +2027,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F51990CE-FF2C-48E9-82E1-2E87B3A6C16A}">
-  <dimension ref="A1:C82"/>
+  <dimension ref="A1:C26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -2078,10 +2109,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C7" s="4">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -2089,10 +2120,10 @@
         <v>7</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C8" s="4">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -2100,10 +2131,10 @@
         <v>8</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="C9" s="4">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -2111,10 +2142,10 @@
         <v>9</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C10" s="4">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -2122,10 +2153,10 @@
         <v>10</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C11" s="4">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -2133,10 +2164,10 @@
         <v>11</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C12" s="4">
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -2144,10 +2175,10 @@
         <v>12</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="C13" s="4">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -2155,10 +2186,10 @@
         <v>13</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>57</v>
+        <v>68</v>
       </c>
       <c r="C14" s="4">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -2166,10 +2197,10 @@
         <v>14</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>58</v>
+        <v>69</v>
       </c>
       <c r="C15" s="4">
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -2177,10 +2208,10 @@
         <v>15</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="C16" s="4">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -2188,10 +2219,10 @@
         <v>16</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>62</v>
+        <v>71</v>
       </c>
       <c r="C17" s="4">
-        <v>12</v>
+        <v>22</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -2199,10 +2230,10 @@
         <v>17</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>60</v>
+        <v>72</v>
       </c>
       <c r="C18" s="4">
-        <v>12</v>
+        <v>25</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -2210,10 +2241,10 @@
         <v>18</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="C19" s="4">
-        <v>12</v>
+        <v>25</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -2221,10 +2252,10 @@
         <v>19</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
       <c r="C20" s="4">
-        <v>13</v>
+        <v>35</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -2232,10 +2263,10 @@
         <v>20</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>67</v>
+        <v>75</v>
       </c>
       <c r="C21" s="4">
-        <v>13</v>
+        <v>39</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -2243,10 +2274,10 @@
         <v>21</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>61</v>
+        <v>76</v>
       </c>
       <c r="C22" s="4">
-        <v>13</v>
+        <v>6</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -2254,10 +2285,10 @@
         <v>22</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>60</v>
+        <v>11</v>
       </c>
       <c r="C23" s="4">
-        <v>13</v>
+        <v>6</v>
       </c>
     </row>
     <row r="24" spans="1:3">
@@ -2265,10 +2296,10 @@
         <v>23</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>65</v>
+        <v>77</v>
       </c>
       <c r="C24" s="4">
-        <v>13</v>
+        <v>36</v>
       </c>
     </row>
     <row r="25" spans="1:3">
@@ -2276,7 +2307,7 @@
         <v>24</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>68</v>
+        <v>78</v>
       </c>
       <c r="C25" s="4">
         <v>13</v>
@@ -2287,626 +2318,10 @@
         <v>25</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>69</v>
+        <v>79</v>
       </c>
       <c r="C26" s="4">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3">
-      <c r="A27" s="4">
-        <v>26</v>
-      </c>
-      <c r="B27" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="C27" s="4">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3">
-      <c r="A28" s="4">
-        <v>27</v>
-      </c>
-      <c r="B28" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="C28" s="4">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3">
-      <c r="A29" s="4">
         <v>28</v>
-      </c>
-      <c r="B29" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="C29" s="4">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3">
-      <c r="A30" s="4">
-        <v>29</v>
-      </c>
-      <c r="B30" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="C30" s="4">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3">
-      <c r="A31" s="4">
-        <v>30</v>
-      </c>
-      <c r="B31" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="C31" s="4">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3">
-      <c r="A32" s="4">
-        <v>31</v>
-      </c>
-      <c r="B32" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="C32" s="4">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3">
-      <c r="A33" s="4">
-        <v>32</v>
-      </c>
-      <c r="B33" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="C33" s="4">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3">
-      <c r="A34" s="4">
-        <v>33</v>
-      </c>
-      <c r="B34" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="C34" s="4">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3">
-      <c r="A35" s="4">
-        <v>34</v>
-      </c>
-      <c r="B35" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="C35" s="4">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3">
-      <c r="A36" s="4">
-        <v>35</v>
-      </c>
-      <c r="B36" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="C36" s="4">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3">
-      <c r="A37" s="4">
-        <v>36</v>
-      </c>
-      <c r="B37" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="C37" s="4">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3">
-      <c r="A38" s="4">
-        <v>37</v>
-      </c>
-      <c r="B38" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="C38" s="4">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3">
-      <c r="A39" s="4">
-        <v>38</v>
-      </c>
-      <c r="B39" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="C39" s="4">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3">
-      <c r="A40" s="4">
-        <v>39</v>
-      </c>
-      <c r="B40" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="C40" s="4">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3">
-      <c r="A41" s="4">
-        <v>40</v>
-      </c>
-      <c r="B41" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="C41" s="4">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3">
-      <c r="A42" s="4">
-        <v>41</v>
-      </c>
-      <c r="B42" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="C42" s="4">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3">
-      <c r="A43" s="4">
-        <v>42</v>
-      </c>
-      <c r="B43" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="C43" s="4">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3">
-      <c r="A44" s="4">
-        <v>43</v>
-      </c>
-      <c r="B44" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="C44" s="4">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3">
-      <c r="A45" s="4">
-        <v>44</v>
-      </c>
-      <c r="B45" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="C45" s="4">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3">
-      <c r="A46" s="4">
-        <v>45</v>
-      </c>
-      <c r="B46" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="C46" s="4">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3">
-      <c r="A47" s="4">
-        <v>46</v>
-      </c>
-      <c r="B47" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="C47" s="4">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3">
-      <c r="A48" s="4">
-        <v>47</v>
-      </c>
-      <c r="B48" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="C48" s="4">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3">
-      <c r="A49" s="4">
-        <v>48</v>
-      </c>
-      <c r="B49" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="C49" s="4">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3">
-      <c r="A50" s="4">
-        <v>49</v>
-      </c>
-      <c r="B50" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="C50" s="4">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3">
-      <c r="A51" s="4">
-        <v>50</v>
-      </c>
-      <c r="B51" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="C51" s="4">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3">
-      <c r="A52" s="4">
-        <v>51</v>
-      </c>
-      <c r="B52" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="C52" s="4">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3">
-      <c r="A53" s="4">
-        <v>52</v>
-      </c>
-      <c r="B53" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="C53" s="4">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3">
-      <c r="A54" s="4">
-        <v>53</v>
-      </c>
-      <c r="B54" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="C54" s="4">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3">
-      <c r="A55" s="4">
-        <v>54</v>
-      </c>
-      <c r="B55" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="C55" s="4">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3">
-      <c r="A56" s="4">
-        <v>55</v>
-      </c>
-      <c r="B56" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="C56" s="4">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3">
-      <c r="A57" s="4">
-        <v>56</v>
-      </c>
-      <c r="B57" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="C57" s="4">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3">
-      <c r="A58" s="4">
-        <v>57</v>
-      </c>
-      <c r="B58" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="C58" s="4">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3">
-      <c r="A59" s="4">
-        <v>58</v>
-      </c>
-      <c r="B59" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="C59" s="4">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3">
-      <c r="A60" s="4">
-        <v>59</v>
-      </c>
-      <c r="B60" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="C60" s="4">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3">
-      <c r="A61" s="4">
-        <v>60</v>
-      </c>
-      <c r="B61" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="C61" s="4">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3">
-      <c r="A62" s="4">
-        <v>61</v>
-      </c>
-      <c r="B62" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="C62" s="4">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3">
-      <c r="A63" s="4">
-        <v>62</v>
-      </c>
-      <c r="B63" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="C63" s="4">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3">
-      <c r="A64" s="4">
-        <v>63</v>
-      </c>
-      <c r="B64" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="C64" s="4">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3">
-      <c r="A65" s="4">
-        <v>64</v>
-      </c>
-      <c r="B65" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="C65" s="4">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3">
-      <c r="A66" s="4">
-        <v>65</v>
-      </c>
-      <c r="B66" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C66" s="4">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3">
-      <c r="A67" s="4">
-        <v>66</v>
-      </c>
-      <c r="B67" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="C67" s="4">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3">
-      <c r="A68" s="4">
-        <v>67</v>
-      </c>
-      <c r="B68" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="C68" s="4">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3">
-      <c r="A69" s="4">
-        <v>68</v>
-      </c>
-      <c r="B69" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="C69" s="4">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3">
-      <c r="A70" s="4">
-        <v>69</v>
-      </c>
-      <c r="B70" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="C70" s="4">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3">
-      <c r="A71" s="4">
-        <v>70</v>
-      </c>
-      <c r="B71" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="C71" s="4">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3">
-      <c r="A72" s="4">
-        <v>71</v>
-      </c>
-      <c r="B72" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="C72" s="4">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3">
-      <c r="A73" s="4">
-        <v>72</v>
-      </c>
-      <c r="B73" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="C73" s="4">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3">
-      <c r="A74" s="4">
-        <v>73</v>
-      </c>
-      <c r="B74" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="C74" s="4">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3">
-      <c r="A75" s="4">
-        <v>74</v>
-      </c>
-      <c r="B75" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="C75" s="4">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3">
-      <c r="A76" s="4">
-        <v>75</v>
-      </c>
-      <c r="B76" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="C76" s="4">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3">
-      <c r="A77" s="4">
-        <v>76</v>
-      </c>
-      <c r="B77" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="C77" s="4">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3">
-      <c r="A78" s="4">
-        <v>77</v>
-      </c>
-      <c r="B78" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="C78" s="4">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3">
-      <c r="A79" s="4">
-        <v>78</v>
-      </c>
-      <c r="B79" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="C79" s="4">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3">
-      <c r="A80" s="4">
-        <v>79</v>
-      </c>
-      <c r="B80" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="C80" s="4">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3">
-      <c r="A81" s="4">
-        <v>80</v>
-      </c>
-      <c r="B81" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="C81" s="4">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3">
-      <c r="A82" s="4">
-        <v>81</v>
-      </c>
-      <c r="B82" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="C82" s="4">
-        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -2918,8 +2333,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E6AD482-693C-4526-A8EF-051504D339CF}">
   <dimension ref="A1:D51"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C49" sqref="C49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -3067,7 +2482,7 @@
       </c>
       <c r="D10" s="1">
         <f ca="1">RANDBETWEEN(1223,1232)</f>
-        <v>1223</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -3082,7 +2497,7 @@
       </c>
       <c r="D11" s="1">
         <f t="shared" ref="D11:D51" ca="1" si="0">RANDBETWEEN(1223,1232)</f>
-        <v>1227</v>
+        <v>1223</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -3097,7 +2512,7 @@
       </c>
       <c r="D12" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1224</v>
+        <v>1231</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -3112,7 +2527,7 @@
       </c>
       <c r="D13" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1228</v>
+        <v>1223</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -3127,7 +2542,7 @@
       </c>
       <c r="D14" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1225</v>
+        <v>1231</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -3142,7 +2557,7 @@
       </c>
       <c r="D15" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1228</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -3157,7 +2572,7 @@
       </c>
       <c r="D16" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1232</v>
+        <v>1231</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -3172,12 +2587,12 @@
       </c>
       <c r="D17" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1232</v>
+        <v>1231</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="4">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B18" s="5" t="s">
         <v>98</v>
@@ -3192,7 +2607,7 @@
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="4">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B19" s="5" t="s">
         <v>99</v>
@@ -3202,12 +2617,12 @@
       </c>
       <c r="D19" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1224</v>
+        <v>1230</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="4">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B20" s="5" t="s">
         <v>100</v>
@@ -3217,12 +2632,12 @@
       </c>
       <c r="D20" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1229</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="4">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B21" s="5" t="s">
         <v>101</v>
@@ -3237,43 +2652,43 @@
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="4">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B22" s="5" t="s">
         <v>102</v>
       </c>
       <c r="C22" s="4">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D22" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1232</v>
+        <v>1230</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="4">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B23" s="5" t="s">
         <v>103</v>
       </c>
       <c r="C23" s="4">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D23" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1227</v>
+        <v>1231</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="4">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B24" s="5" t="s">
         <v>104</v>
       </c>
       <c r="C24" s="4">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D24" s="1">
         <f t="shared" ca="1" si="0"/>
@@ -3282,58 +2697,58 @@
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="4">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B25" s="5" t="s">
         <v>105</v>
       </c>
       <c r="C25" s="4">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D25" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1225</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="26" spans="1:4">
       <c r="A26" s="4">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B26" s="5" t="s">
         <v>106</v>
       </c>
       <c r="C26" s="4">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D26" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1225</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="27" spans="1:4">
       <c r="A27" s="4">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="B27" s="5" t="s">
         <v>107</v>
       </c>
       <c r="C27" s="4">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D27" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1226</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="28" spans="1:4">
       <c r="A28" s="4">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="B28" s="5" t="s">
         <v>108</v>
       </c>
       <c r="C28" s="4">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D28" s="1">
         <f t="shared" ca="1" si="0"/>
@@ -3342,13 +2757,13 @@
     </row>
     <row r="29" spans="1:4">
       <c r="A29" s="4">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="B29" s="5" t="s">
         <v>109</v>
       </c>
       <c r="C29" s="4">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D29" s="1">
         <f t="shared" ca="1" si="0"/>
@@ -3357,13 +2772,13 @@
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="4">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="B30" s="5" t="s">
         <v>110</v>
       </c>
       <c r="C30" s="4">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D30" s="1">
         <f t="shared" ca="1" si="0"/>
@@ -3372,43 +2787,43 @@
     </row>
     <row r="31" spans="1:4">
       <c r="A31" s="4">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="B31" s="5" t="s">
         <v>111</v>
       </c>
       <c r="C31" s="4">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D31" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1224</v>
+        <v>1223</v>
       </c>
     </row>
     <row r="32" spans="1:4">
       <c r="A32" s="4">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B32" s="5" t="s">
         <v>112</v>
       </c>
       <c r="C32" s="4">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D32" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1227</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="33" spans="1:4">
       <c r="A33" s="4">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="B33" s="5" t="s">
         <v>113</v>
       </c>
       <c r="C33" s="4">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D33" s="1">
         <f t="shared" ca="1" si="0"/>
@@ -3417,172 +2832,172 @@
     </row>
     <row r="34" spans="1:4">
       <c r="A34" s="4">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="B34" s="5" t="s">
         <v>114</v>
       </c>
       <c r="C34" s="4">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D34" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1225</v>
+        <v>1231</v>
       </c>
     </row>
     <row r="35" spans="1:4">
       <c r="A35" s="4">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="B35" s="5" t="s">
         <v>115</v>
       </c>
       <c r="C35" s="4">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D35" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1224</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="36" spans="1:4">
       <c r="A36" s="4">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="B36" s="5" t="s">
         <v>116</v>
       </c>
       <c r="C36" s="4">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D36" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1226</v>
+        <v>1230</v>
       </c>
     </row>
     <row r="37" spans="1:4">
       <c r="A37" s="4">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="B37" s="5" t="s">
         <v>117</v>
       </c>
       <c r="C37" s="4">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D37" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1226</v>
+        <v>1232</v>
       </c>
     </row>
     <row r="38" spans="1:4">
       <c r="A38" s="4">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="B38" s="5" t="s">
         <v>118</v>
       </c>
       <c r="C38" s="4">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D38" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1230</v>
+        <v>1231</v>
       </c>
     </row>
     <row r="39" spans="1:4">
       <c r="A39" s="4">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="B39" s="5" t="s">
         <v>119</v>
       </c>
       <c r="C39" s="4">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D39" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1231</v>
+        <v>1229</v>
       </c>
     </row>
     <row r="40" spans="1:4">
       <c r="A40" s="4">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="B40" s="5" t="s">
         <v>120</v>
       </c>
       <c r="C40" s="4">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D40" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1232</v>
+        <v>1224</v>
       </c>
     </row>
     <row r="41" spans="1:4">
       <c r="A41" s="4">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="B41" s="5" t="s">
         <v>121</v>
       </c>
       <c r="C41" s="4">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D41" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1224</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="42" spans="1:4">
       <c r="A42" s="4">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="B42" s="5" t="s">
         <v>122</v>
       </c>
       <c r="C42" s="4">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D42" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1225</v>
+        <v>1229</v>
       </c>
     </row>
     <row r="43" spans="1:4">
       <c r="A43" s="4">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="B43" s="5" t="s">
         <v>123</v>
       </c>
       <c r="C43" s="4">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D43" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1232</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="44" spans="1:4">
       <c r="A44" s="4">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="B44" s="5" t="s">
         <v>124</v>
       </c>
       <c r="C44" s="4">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D44" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1227</v>
+        <v>1232</v>
       </c>
     </row>
     <row r="45" spans="1:4">
       <c r="A45" s="4">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="B45" s="5" t="s">
         <v>125</v>
@@ -3592,12 +3007,12 @@
       </c>
       <c r="D45" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1231</v>
+        <v>1224</v>
       </c>
     </row>
     <row r="46" spans="1:4">
       <c r="A46" s="4">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="B46" s="5" t="s">
         <v>126</v>
@@ -3607,12 +3022,12 @@
       </c>
       <c r="D46" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1230</v>
+        <v>1232</v>
       </c>
     </row>
     <row r="47" spans="1:4">
       <c r="A47" s="4">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="B47" s="5" t="s">
         <v>127</v>
@@ -3622,12 +3037,12 @@
       </c>
       <c r="D47" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1223</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="48" spans="1:4">
       <c r="A48" s="4">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="B48" s="5" t="s">
         <v>128</v>
@@ -3637,12 +3052,12 @@
       </c>
       <c r="D48" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1229</v>
+        <v>1223</v>
       </c>
     </row>
     <row r="49" spans="1:4">
       <c r="A49" s="4">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="B49" s="5" t="s">
         <v>129</v>
@@ -3652,18 +3067,18 @@
       </c>
       <c r="D49" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1232</v>
+        <v>1230</v>
       </c>
     </row>
     <row r="50" spans="1:4">
       <c r="A50" s="4">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="B50" s="5" t="s">
         <v>130</v>
       </c>
       <c r="C50" s="4">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="D50" s="1">
         <f t="shared" ca="1" si="0"/>
@@ -3672,17 +3087,17 @@
     </row>
     <row r="51" spans="1:4">
       <c r="A51" s="4">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="B51" s="5" t="s">
         <v>131</v>
       </c>
       <c r="C51" s="4">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="D51" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1228</v>
+        <v>1232</v>
       </c>
     </row>
   </sheetData>
@@ -3692,10 +3107,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6E05CD4-7C76-4891-A9C7-AB36831BB0B8}">
-  <dimension ref="A1:H14"/>
+  <dimension ref="A1:H16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -3989,7 +3404,7 @@
         <v>138</v>
       </c>
       <c r="G11" s="8">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="H11" s="8">
         <v>110</v>
@@ -4041,42 +3456,96 @@
         <v>173</v>
       </c>
       <c r="G13" s="8">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="H13" s="8">
         <v>110</v>
       </c>
     </row>
     <row r="14" spans="1:8">
-      <c r="A14" s="10">
+      <c r="A14" s="8">
         <v>1235</v>
       </c>
-      <c r="B14" s="11" t="s">
+      <c r="B14" s="3" t="s">
         <v>274</v>
       </c>
-      <c r="C14" s="12" t="s">
+      <c r="C14" s="9" t="s">
         <v>273</v>
       </c>
-      <c r="D14" s="11" t="s">
+      <c r="D14" s="3" t="s">
         <v>274</v>
       </c>
-      <c r="E14" s="11" t="s">
+      <c r="E14" s="3" t="s">
+        <v>297</v>
+      </c>
+      <c r="F14" s="8" t="s">
         <v>275</v>
       </c>
-      <c r="F14" s="10" t="s">
-        <v>276</v>
-      </c>
-      <c r="G14" s="10">
-        <v>1</v>
-      </c>
-      <c r="H14" s="10">
+      <c r="G14" s="8">
+        <v>1</v>
+      </c>
+      <c r="H14" s="8">
         <v>230</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" s="8">
+        <v>1236</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>273</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>295</v>
+      </c>
+      <c r="F15" s="8" t="s">
+        <v>275</v>
+      </c>
+      <c r="G15" s="8">
+        <v>14</v>
+      </c>
+      <c r="H15" s="8">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" s="8">
+        <v>1237</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>298</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>273</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>298</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>299</v>
+      </c>
+      <c r="F16" s="8" t="s">
+        <v>275</v>
+      </c>
+      <c r="G16" s="8">
+        <v>25</v>
+      </c>
+      <c r="H16" s="8">
+        <v>110</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" xr:uid="{326C7255-3775-42C0-8CED-A0F3BD8EC552}"/>
     <hyperlink ref="C14" r:id="rId2" xr:uid="{3075A95B-B014-4146-9A02-CE8105DDA61C}"/>
+    <hyperlink ref="C15" r:id="rId3" xr:uid="{AFA86EE8-5F45-4116-A3FB-D1EBD86D2849}"/>
+    <hyperlink ref="C16" r:id="rId4" xr:uid="{4D1991A4-676E-4D81-B282-274D9EC0BE3E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4151,16 +3620,17 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{491D14EC-1CB1-4681-930A-4B9B4015FC83}">
-  <dimension ref="A1:P23"/>
+  <dimension ref="A1:P27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="N21" sqref="N21"/>
+    <sheetView topLeftCell="H12" workbookViewId="0">
+      <selection activeCell="P28" sqref="P28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="14.08984375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.90625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.26953125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19.08984375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="22.54296875" bestFit="1" customWidth="1"/>
@@ -4215,7 +3685,7 @@
         <v>248</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="O1" s="1" t="s">
         <v>217</v>
@@ -4261,13 +3731,13 @@
         <v>250</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="O2" s="2">
         <v>1223</v>
       </c>
       <c r="P2" s="1">
-        <v>30</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:16">
@@ -4307,7 +3777,7 @@
         <v>250</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="O3" s="1">
         <v>1224</v>
@@ -4353,7 +3823,7 @@
         <v>250</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="O4" s="2">
         <v>1225</v>
@@ -4399,7 +3869,7 @@
         <v>250</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="O5" s="1">
         <v>1225</v>
@@ -4445,7 +3915,7 @@
         <v>250</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="O6" s="1">
         <v>1227</v>
@@ -4491,7 +3961,7 @@
         <v>250</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="O7" s="1">
         <v>1226</v>
@@ -4537,13 +4007,13 @@
         <v>250</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="O8" s="2">
         <v>1223</v>
       </c>
       <c r="P8" s="1">
-        <v>30</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:16">
@@ -4583,13 +4053,13 @@
         <v>250</v>
       </c>
       <c r="N9" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="O9" s="1">
         <v>1223</v>
       </c>
       <c r="P9" s="1">
-        <v>30</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:16">
@@ -4629,13 +4099,13 @@
         <v>250</v>
       </c>
       <c r="N10" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="O10" s="2">
         <v>1226</v>
       </c>
       <c r="P10" s="1">
-        <v>30</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:16">
@@ -4675,13 +4145,13 @@
         <v>250</v>
       </c>
       <c r="N11" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="O11" s="1">
         <v>1226</v>
       </c>
       <c r="P11" s="1">
-        <v>30</v>
+        <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:16">
@@ -4721,13 +4191,13 @@
         <v>250</v>
       </c>
       <c r="N12" s="1" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="O12" s="2">
         <v>1226</v>
       </c>
       <c r="P12" s="1">
-        <v>30</v>
+        <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:16">
@@ -4767,7 +4237,7 @@
         <v>250</v>
       </c>
       <c r="N13" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="O13" s="2">
         <v>1229</v>
@@ -4813,7 +4283,7 @@
         <v>250</v>
       </c>
       <c r="N14" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="O14" s="1">
         <v>1230</v>
@@ -4859,7 +4329,7 @@
         <v>250</v>
       </c>
       <c r="N15" s="1" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="O15" s="2">
         <v>1231</v>
@@ -4905,7 +4375,7 @@
         <v>250</v>
       </c>
       <c r="N16" s="1" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="O16" s="1">
         <v>1231</v>
@@ -4951,7 +4421,7 @@
         <v>250</v>
       </c>
       <c r="N17" s="1" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="O17" s="2">
         <v>1224</v>
@@ -4999,7 +4469,7 @@
         <v>250</v>
       </c>
       <c r="N18" s="1" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="O18" s="1">
         <v>1225</v>
@@ -5047,7 +4517,7 @@
         <v>250</v>
       </c>
       <c r="N19" s="1" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="O19" s="1">
         <v>1226</v>
@@ -5093,7 +4563,7 @@
         <v>250</v>
       </c>
       <c r="N20" s="1" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="O20" s="1">
         <v>1223</v>
@@ -5139,7 +4609,7 @@
         <v>250</v>
       </c>
       <c r="N21" s="1" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="O21" s="1">
         <v>1229</v>
@@ -5185,7 +4655,7 @@
         <v>250</v>
       </c>
       <c r="N22" s="1" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="O22" s="1">
         <v>1228</v>
@@ -5231,13 +4701,197 @@
         <v>250</v>
       </c>
       <c r="N23" s="1" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="O23" s="1">
         <v>1227</v>
       </c>
       <c r="P23" s="1">
         <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16">
+      <c r="A24" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="J24" s="1">
+        <v>1</v>
+      </c>
+      <c r="K24" s="1"/>
+      <c r="L24" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="M24" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="N24" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="O24" s="1">
+        <v>1227</v>
+      </c>
+      <c r="P24" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16">
+      <c r="A25" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="I25" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="J25" s="1">
+        <v>1</v>
+      </c>
+      <c r="K25" s="1"/>
+      <c r="L25" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="M25" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="N25" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="O25" s="1">
+        <v>1227</v>
+      </c>
+      <c r="P25" s="1">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16">
+      <c r="A26" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="I26" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="J26" s="1">
+        <v>1</v>
+      </c>
+      <c r="K26" s="1"/>
+      <c r="L26" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="M26" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="N26" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="O26" s="1">
+        <v>1227</v>
+      </c>
+      <c r="P26" s="1">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16">
+      <c r="A27" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="I27" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="J27" s="1">
+        <v>1</v>
+      </c>
+      <c r="K27" s="1"/>
+      <c r="L27" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="M27" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="N27" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="O27" s="1">
+        <v>1227</v>
+      </c>
+      <c r="P27" s="1">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added user name info at settings modal and changed a user's info
</commit_message>
<xml_diff>
--- a/backend/internal/seed/seed_data/mst_dummy_data.xlsx
+++ b/backend/internal/seed/seed_data/mst_dummy_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Uni\Intern SM\Stock Opname App [SOSMIT]\SOSMIT\backend\internal\seed\seed_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7E3DF17-8783-4E10-9600-5D4378BAF31A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{127AE3A5-4E24-4224-AE69-DE4C7F2EB2E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10540" activeTab="3" xr2:uid="{AF28B77B-5B1D-47C2-ADE5-ADF50DA09BCF}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="556" uniqueCount="300">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="556" uniqueCount="299">
   <si>
     <t>id</t>
   </si>
@@ -925,15 +925,6 @@
     <t>SMPR00000012</t>
   </si>
   <si>
-    <t>DENY</t>
-  </si>
-  <si>
-    <t>SUMARGA</t>
-  </si>
-  <si>
-    <t>DENSU</t>
-  </si>
-  <si>
     <t>DIPA</t>
   </si>
   <si>
@@ -941,6 +932,12 @@
   </si>
   <si>
     <t>PARA</t>
+  </si>
+  <si>
+    <t>DION</t>
+  </si>
+  <si>
+    <t>WIYOYO</t>
   </si>
 </sst>
 </file>
@@ -2482,7 +2479,7 @@
       </c>
       <c r="D10" s="1">
         <f ca="1">RANDBETWEEN(1223,1232)</f>
-        <v>1228</v>
+        <v>1224</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -2497,7 +2494,7 @@
       </c>
       <c r="D11" s="1">
         <f t="shared" ref="D11:D51" ca="1" si="0">RANDBETWEEN(1223,1232)</f>
-        <v>1223</v>
+        <v>1225</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -2512,7 +2509,7 @@
       </c>
       <c r="D12" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1231</v>
+        <v>1230</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -2527,7 +2524,7 @@
       </c>
       <c r="D13" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1223</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -2542,7 +2539,7 @@
       </c>
       <c r="D14" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1231</v>
+        <v>1224</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -2557,7 +2554,7 @@
       </c>
       <c r="D15" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1227</v>
+        <v>1231</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -2587,7 +2584,7 @@
       </c>
       <c r="D17" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1231</v>
+        <v>1223</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -2602,7 +2599,7 @@
       </c>
       <c r="D18" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1226</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -2617,7 +2614,7 @@
       </c>
       <c r="D19" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1230</v>
+        <v>1223</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -2632,7 +2629,7 @@
       </c>
       <c r="D20" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1227</v>
+        <v>1226</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -2647,7 +2644,7 @@
       </c>
       <c r="D21" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1228</v>
+        <v>1226</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -2662,7 +2659,7 @@
       </c>
       <c r="D22" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1230</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -2677,7 +2674,7 @@
       </c>
       <c r="D23" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1231</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -2692,7 +2689,7 @@
       </c>
       <c r="D24" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1231</v>
+        <v>1230</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -2722,7 +2719,7 @@
       </c>
       <c r="D26" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1228</v>
+        <v>1229</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -2752,7 +2749,7 @@
       </c>
       <c r="D28" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1231</v>
+        <v>1230</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -2767,7 +2764,7 @@
       </c>
       <c r="D29" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1229</v>
+        <v>1232</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -2782,7 +2779,7 @@
       </c>
       <c r="D30" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1223</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -2797,7 +2794,7 @@
       </c>
       <c r="D31" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1223</v>
+        <v>1230</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -2812,7 +2809,7 @@
       </c>
       <c r="D32" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1228</v>
+        <v>1225</v>
       </c>
     </row>
     <row r="33" spans="1:4">
@@ -2827,7 +2824,7 @@
       </c>
       <c r="D33" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1232</v>
+        <v>1226</v>
       </c>
     </row>
     <row r="34" spans="1:4">
@@ -2842,7 +2839,7 @@
       </c>
       <c r="D34" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1231</v>
+        <v>1224</v>
       </c>
     </row>
     <row r="35" spans="1:4">
@@ -2857,7 +2854,7 @@
       </c>
       <c r="D35" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1228</v>
+        <v>1229</v>
       </c>
     </row>
     <row r="36" spans="1:4">
@@ -2872,7 +2869,7 @@
       </c>
       <c r="D36" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1230</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="37" spans="1:4">
@@ -2887,7 +2884,7 @@
       </c>
       <c r="D37" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1232</v>
+        <v>1226</v>
       </c>
     </row>
     <row r="38" spans="1:4">
@@ -2902,7 +2899,7 @@
       </c>
       <c r="D38" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1231</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="39" spans="1:4">
@@ -2917,7 +2914,7 @@
       </c>
       <c r="D39" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1229</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="40" spans="1:4">
@@ -2947,7 +2944,7 @@
       </c>
       <c r="D41" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1227</v>
+        <v>1229</v>
       </c>
     </row>
     <row r="42" spans="1:4">
@@ -2962,7 +2959,7 @@
       </c>
       <c r="D42" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1229</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="43" spans="1:4">
@@ -2977,7 +2974,7 @@
       </c>
       <c r="D43" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1227</v>
+        <v>1232</v>
       </c>
     </row>
     <row r="44" spans="1:4">
@@ -2992,7 +2989,7 @@
       </c>
       <c r="D44" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1232</v>
+        <v>1226</v>
       </c>
     </row>
     <row r="45" spans="1:4">
@@ -3007,7 +3004,7 @@
       </c>
       <c r="D45" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1224</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="46" spans="1:4">
@@ -3037,7 +3034,7 @@
       </c>
       <c r="D47" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1227</v>
+        <v>1230</v>
       </c>
     </row>
     <row r="48" spans="1:4">
@@ -3052,7 +3049,7 @@
       </c>
       <c r="D48" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1223</v>
+        <v>1231</v>
       </c>
     </row>
     <row r="49" spans="1:4">
@@ -3067,7 +3064,7 @@
       </c>
       <c r="D49" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1230</v>
+        <v>1226</v>
       </c>
     </row>
     <row r="50" spans="1:4">
@@ -3082,7 +3079,7 @@
       </c>
       <c r="D50" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1229</v>
+        <v>1226</v>
       </c>
     </row>
     <row r="51" spans="1:4">
@@ -3097,7 +3094,7 @@
       </c>
       <c r="D51" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1232</v>
+        <v>1228</v>
       </c>
     </row>
   </sheetData>
@@ -3110,7 +3107,7 @@
   <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -3476,7 +3473,7 @@
         <v>274</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="F14" s="8" t="s">
         <v>275</v>
@@ -3493,16 +3490,16 @@
         <v>1236</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="C15" s="9" t="s">
         <v>273</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>294</v>
+        <v>297</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>295</v>
+        <v>298</v>
       </c>
       <c r="F15" s="8" t="s">
         <v>275</v>
@@ -3519,16 +3516,16 @@
         <v>1237</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="C16" s="9" t="s">
         <v>273</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="F16" s="8" t="s">
         <v>275</v>

</xml_diff>

<commit_message>
add asset equipments CSV seed data and update dummy data file
</commit_message>
<xml_diff>
--- a/backend/internal/seed/seed_data/mst_dummy_data.xlsx
+++ b/backend/internal/seed/seed_data/mst_dummy_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Uni\Intern SM\Stock Opname App [SOSMIT]\SOSMIT\backend\internal\seed\seed_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{127AE3A5-4E24-4224-AE69-DE4C7F2EB2E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC49B665-48DA-45CF-9567-CB7C17C71B54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10540" activeTab="3" xr2:uid="{AF28B77B-5B1D-47C2-ADE5-ADF50DA09BCF}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10540" activeTab="6" xr2:uid="{AF28B77B-5B1D-47C2-ADE5-ADF50DA09BCF}"/>
   </bookViews>
   <sheets>
     <sheet name="Region" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,11 @@
     <sheet name="User" sheetId="4" r:id="rId4"/>
     <sheet name="Cost Center" sheetId="6" r:id="rId5"/>
     <sheet name="Asset" sheetId="5" r:id="rId6"/>
+    <sheet name="Asset Equipment" sheetId="7" r:id="rId7"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'Asset Equipment'!$A$1:$A$7</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -41,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="556" uniqueCount="299">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="570" uniqueCount="306">
   <si>
     <t>id</t>
   </si>
@@ -938,6 +942,27 @@
   </si>
   <si>
     <t>WIYOYO</t>
+  </si>
+  <si>
+    <t>equipments</t>
+  </si>
+  <si>
+    <t>Unit, Kabel power</t>
+  </si>
+  <si>
+    <t>Unit, Tas, Kabel power, Adaptor</t>
+  </si>
+  <si>
+    <t>Unit, Kabel power, Kabel VGA, Kabel HDMI</t>
+  </si>
+  <si>
+    <t>Unit, Kabel power, Kabel UPS</t>
+  </si>
+  <si>
+    <t>Unit, Simcard, Handstrap, Adaptor, Kabel USB</t>
+  </si>
+  <si>
+    <t>Unit, Tas, Tali tas, Adaptor, Kabel USB</t>
   </si>
 </sst>
 </file>
@@ -2479,7 +2504,7 @@
       </c>
       <c r="D10" s="1">
         <f ca="1">RANDBETWEEN(1223,1232)</f>
-        <v>1224</v>
+        <v>1230</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -2494,7 +2519,7 @@
       </c>
       <c r="D11" s="1">
         <f t="shared" ref="D11:D51" ca="1" si="0">RANDBETWEEN(1223,1232)</f>
-        <v>1225</v>
+        <v>1230</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -2524,7 +2549,7 @@
       </c>
       <c r="D13" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1228</v>
+        <v>1232</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -2554,7 +2579,7 @@
       </c>
       <c r="D15" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1231</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -2569,7 +2594,7 @@
       </c>
       <c r="D16" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1231</v>
+        <v>1232</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -2584,7 +2609,7 @@
       </c>
       <c r="D17" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1223</v>
+        <v>1225</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -2599,7 +2624,7 @@
       </c>
       <c r="D18" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1227</v>
+        <v>1226</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -2614,7 +2639,7 @@
       </c>
       <c r="D19" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1223</v>
+        <v>1230</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -2629,7 +2654,7 @@
       </c>
       <c r="D20" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1226</v>
+        <v>1229</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -2644,7 +2669,7 @@
       </c>
       <c r="D21" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1226</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -2659,7 +2684,7 @@
       </c>
       <c r="D22" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1228</v>
+        <v>1226</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -2689,7 +2714,7 @@
       </c>
       <c r="D24" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1230</v>
+        <v>1223</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -2704,7 +2729,7 @@
       </c>
       <c r="D25" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1228</v>
+        <v>1224</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -2764,7 +2789,7 @@
       </c>
       <c r="D29" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1232</v>
+        <v>1226</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -2779,7 +2804,7 @@
       </c>
       <c r="D30" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1228</v>
+        <v>1231</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -2794,7 +2819,7 @@
       </c>
       <c r="D31" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1230</v>
+        <v>1229</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -2809,7 +2834,7 @@
       </c>
       <c r="D32" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1225</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="33" spans="1:4">
@@ -2824,7 +2849,7 @@
       </c>
       <c r="D33" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1226</v>
+        <v>1224</v>
       </c>
     </row>
     <row r="34" spans="1:4">
@@ -2839,7 +2864,7 @@
       </c>
       <c r="D34" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1224</v>
+        <v>1225</v>
       </c>
     </row>
     <row r="35" spans="1:4">
@@ -2854,7 +2879,7 @@
       </c>
       <c r="D35" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1229</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="36" spans="1:4">
@@ -2869,7 +2894,7 @@
       </c>
       <c r="D36" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1228</v>
+        <v>1231</v>
       </c>
     </row>
     <row r="37" spans="1:4">
@@ -2884,7 +2909,7 @@
       </c>
       <c r="D37" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1226</v>
+        <v>1229</v>
       </c>
     </row>
     <row r="38" spans="1:4">
@@ -2899,7 +2924,7 @@
       </c>
       <c r="D38" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1227</v>
+        <v>1232</v>
       </c>
     </row>
     <row r="39" spans="1:4">
@@ -2914,7 +2939,7 @@
       </c>
       <c r="D39" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1228</v>
+        <v>1224</v>
       </c>
     </row>
     <row r="40" spans="1:4">
@@ -2929,7 +2954,7 @@
       </c>
       <c r="D40" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1224</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="41" spans="1:4">
@@ -2944,7 +2969,7 @@
       </c>
       <c r="D41" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1229</v>
+        <v>1230</v>
       </c>
     </row>
     <row r="42" spans="1:4">
@@ -2959,7 +2984,7 @@
       </c>
       <c r="D42" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1228</v>
+        <v>1223</v>
       </c>
     </row>
     <row r="43" spans="1:4">
@@ -2974,7 +2999,7 @@
       </c>
       <c r="D43" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1232</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="44" spans="1:4">
@@ -2989,7 +3014,7 @@
       </c>
       <c r="D44" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1226</v>
+        <v>1230</v>
       </c>
     </row>
     <row r="45" spans="1:4">
@@ -3004,7 +3029,7 @@
       </c>
       <c r="D45" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1228</v>
+        <v>1232</v>
       </c>
     </row>
     <row r="46" spans="1:4">
@@ -3019,7 +3044,7 @@
       </c>
       <c r="D46" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1232</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="47" spans="1:4">
@@ -3034,7 +3059,7 @@
       </c>
       <c r="D47" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1230</v>
+        <v>1231</v>
       </c>
     </row>
     <row r="48" spans="1:4">
@@ -3049,7 +3074,7 @@
       </c>
       <c r="D48" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1231</v>
+        <v>1223</v>
       </c>
     </row>
     <row r="49" spans="1:4">
@@ -3064,7 +3089,7 @@
       </c>
       <c r="D49" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1226</v>
+        <v>1231</v>
       </c>
     </row>
     <row r="50" spans="1:4">
@@ -3079,7 +3104,7 @@
       </c>
       <c r="D50" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1226</v>
+        <v>1232</v>
       </c>
     </row>
     <row r="51" spans="1:4">
@@ -3094,7 +3119,7 @@
       </c>
       <c r="D51" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1228</v>
+        <v>1229</v>
       </c>
     </row>
   </sheetData>
@@ -3106,7 +3131,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6E05CD4-7C76-4891-A9C7-AB36831BB0B8}">
   <dimension ref="A1:H16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
@@ -3619,8 +3644,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{491D14EC-1CB1-4681-930A-4B9B4015FC83}">
   <dimension ref="A1:P27"/>
   <sheetViews>
-    <sheetView topLeftCell="H12" workbookViewId="0">
-      <selection activeCell="P28" sqref="P28"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="N1" sqref="N1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -4895,4 +4920,80 @@
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28F0C749-0F7B-4353-B0A5-2957163B7B34}">
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="1" max="1" width="23.36328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.08984375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>305</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:A7" xr:uid="{28F0C749-0F7B-4353-B0A5-2957163B7B34}"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
update asset CSV seed data to include additional equipment details and modify dummy data file
</commit_message>
<xml_diff>
--- a/backend/internal/seed/seed_data/mst_dummy_data.xlsx
+++ b/backend/internal/seed/seed_data/mst_dummy_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Uni\Intern SM\Stock Opname App [SOSMIT]\SOSMIT\backend\internal\seed\seed_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC49B665-48DA-45CF-9567-CB7C17C71B54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4706CACC-5B4A-4130-8372-043C73C9BD14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10540" activeTab="6" xr2:uid="{AF28B77B-5B1D-47C2-ADE5-ADF50DA09BCF}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10540" activeTab="5" xr2:uid="{AF28B77B-5B1D-47C2-ADE5-ADF50DA09BCF}"/>
   </bookViews>
   <sheets>
     <sheet name="Region" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="570" uniqueCount="306">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="570" uniqueCount="317">
   <si>
     <t>id</t>
   </si>
@@ -875,30 +875,6 @@
     <t>AREA MANAGER</t>
   </si>
   <si>
-    <t>equipment</t>
-  </si>
-  <si>
-    <t>Kabel power, Adaptor</t>
-  </si>
-  <si>
-    <t>Tas</t>
-  </si>
-  <si>
-    <t>Kabel power</t>
-  </si>
-  <si>
-    <t>Kabel power, Kabel VGA</t>
-  </si>
-  <si>
-    <t>Simcard, Handstrap, Adaptor, Kabel USB</t>
-  </si>
-  <si>
-    <t>Simcard, Adaptor, Kabel USB</t>
-  </si>
-  <si>
-    <t>Tas, Tali tas, Adaptor, Kabel USB</t>
-  </si>
-  <si>
     <t>XXZHJ225436587</t>
   </si>
   <si>
@@ -962,7 +938,64 @@
     <t>Unit, Simcard, Handstrap, Adaptor, Kabel USB</t>
   </si>
   <si>
-    <t>Unit, Tas, Tali tas, Adaptor, Kabel USB</t>
+    <t>Unit, Tas</t>
+  </si>
+  <si>
+    <t>Unit, Kabel power, Keyboard, Mouse</t>
+  </si>
+  <si>
+    <t>Unit, Kabel power, Keyboard</t>
+  </si>
+  <si>
+    <t>Unit, Kabel power, Adaptor (s/n: ADQ9175G32)</t>
+  </si>
+  <si>
+    <t>Unit, Tas, Tali tas, Adaptor (s/n: ADQ917645D), Kabel USB</t>
+  </si>
+  <si>
+    <t>Unit, Tas, Tali tas, Adaptor (s/n: ADQ9176222), Kabel USB</t>
+  </si>
+  <si>
+    <t>Unit, Tas, Tali tas, Adaptor (s/n: ADQ917345D), Kabel USB</t>
+  </si>
+  <si>
+    <t>Unit, Tas, Tali tas, Adaptor (s/n: ADQ2FR645D), Kabel USB</t>
+  </si>
+  <si>
+    <t>Unit, Tas, Tali tas, Adaptor (s/n: ADQ9175KJT), Kabel USB</t>
+  </si>
+  <si>
+    <t>Unit, Tas, Tali tas, Adaptor (s/n: ADQ917SF54), Kabel USB</t>
+  </si>
+  <si>
+    <t>Unit, Tas, Tali tas, Adaptor (s/n: ADQ91764G6), Kabel USB</t>
+  </si>
+  <si>
+    <t>Unit, Tas, Tali tas, Adaptor (s/n: ADQ9174444), Kabel USB</t>
+  </si>
+  <si>
+    <t>Unit, Tas, Tali tas, Adaptor (s/n: ADQ13F45D), Kabel USB</t>
+  </si>
+  <si>
+    <t>Unit, Tas, Tali tas, Adaptor (s/n: ADQ91778KL), Kabel USB</t>
+  </si>
+  <si>
+    <t>Unit, Tas, Tali tas, Adaptor (s/n: ADQ91721ER), Kabel USB</t>
+  </si>
+  <si>
+    <t>Unit, Tas, Tali tas, Adaptor (s/n: ADY97O645D), Kabel USB</t>
+  </si>
+  <si>
+    <t>Unit, Simcard, Handstrap, Adaptor (s/n: ADQ917YY54), Kabel USB</t>
+  </si>
+  <si>
+    <t>Unit, Simcard, Handstrap, Adaptor (s/n: ADQ9172P1O), Kabel USB</t>
+  </si>
+  <si>
+    <t>Unit, Simcard, Adaptor (s/n: ADQ902DFG4), Kabel USB</t>
+  </si>
+  <si>
+    <t>Unit, Tas, Tali tas, Adaptor, Kabel USB, Bracket</t>
   </si>
 </sst>
 </file>
@@ -2355,8 +2388,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E6AD482-693C-4526-A8EF-051504D339CF}">
   <dimension ref="A1:D51"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C49" sqref="C49"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -2504,7 +2537,7 @@
       </c>
       <c r="D10" s="1">
         <f ca="1">RANDBETWEEN(1223,1232)</f>
-        <v>1230</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -2534,7 +2567,7 @@
       </c>
       <c r="D12" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1230</v>
+        <v>1232</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -2564,7 +2597,7 @@
       </c>
       <c r="D14" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1224</v>
+        <v>1223</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -2579,7 +2612,7 @@
       </c>
       <c r="D15" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1227</v>
+        <v>1230</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -2609,7 +2642,7 @@
       </c>
       <c r="D17" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1225</v>
+        <v>1230</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -2624,7 +2657,7 @@
       </c>
       <c r="D18" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1226</v>
+        <v>1225</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -2639,7 +2672,7 @@
       </c>
       <c r="D19" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1230</v>
+        <v>1223</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -2669,7 +2702,7 @@
       </c>
       <c r="D21" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1227</v>
+        <v>1223</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -2684,7 +2717,7 @@
       </c>
       <c r="D22" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1226</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -2699,7 +2732,7 @@
       </c>
       <c r="D23" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1228</v>
+        <v>1232</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -2714,7 +2747,7 @@
       </c>
       <c r="D24" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1223</v>
+        <v>1229</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -2729,7 +2762,7 @@
       </c>
       <c r="D25" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1224</v>
+        <v>1223</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -2744,7 +2777,7 @@
       </c>
       <c r="D26" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1229</v>
+        <v>1225</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -2759,7 +2792,7 @@
       </c>
       <c r="D27" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1228</v>
+        <v>1226</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -2774,7 +2807,7 @@
       </c>
       <c r="D28" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1230</v>
+        <v>1231</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -2789,7 +2822,7 @@
       </c>
       <c r="D29" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1226</v>
+        <v>1224</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -2804,7 +2837,7 @@
       </c>
       <c r="D30" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1231</v>
+        <v>1223</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -2819,7 +2852,7 @@
       </c>
       <c r="D31" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1229</v>
+        <v>1231</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -2834,7 +2867,7 @@
       </c>
       <c r="D32" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1228</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="33" spans="1:4">
@@ -2849,7 +2882,7 @@
       </c>
       <c r="D33" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1224</v>
+        <v>1230</v>
       </c>
     </row>
     <row r="34" spans="1:4">
@@ -2864,7 +2897,7 @@
       </c>
       <c r="D34" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1225</v>
+        <v>1230</v>
       </c>
     </row>
     <row r="35" spans="1:4">
@@ -2879,7 +2912,7 @@
       </c>
       <c r="D35" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1227</v>
+        <v>1229</v>
       </c>
     </row>
     <row r="36" spans="1:4">
@@ -2894,7 +2927,7 @@
       </c>
       <c r="D36" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1231</v>
+        <v>1226</v>
       </c>
     </row>
     <row r="37" spans="1:4">
@@ -2924,7 +2957,7 @@
       </c>
       <c r="D38" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1232</v>
+        <v>1225</v>
       </c>
     </row>
     <row r="39" spans="1:4">
@@ -2939,7 +2972,7 @@
       </c>
       <c r="D39" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1224</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="40" spans="1:4">
@@ -2969,7 +3002,7 @@
       </c>
       <c r="D41" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1230</v>
+        <v>1223</v>
       </c>
     </row>
     <row r="42" spans="1:4">
@@ -2984,7 +3017,7 @@
       </c>
       <c r="D42" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1223</v>
+        <v>1230</v>
       </c>
     </row>
     <row r="43" spans="1:4">
@@ -2999,7 +3032,7 @@
       </c>
       <c r="D43" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1228</v>
+        <v>1230</v>
       </c>
     </row>
     <row r="44" spans="1:4">
@@ -3014,7 +3047,7 @@
       </c>
       <c r="D44" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1230</v>
+        <v>1232</v>
       </c>
     </row>
     <row r="45" spans="1:4">
@@ -3029,7 +3062,7 @@
       </c>
       <c r="D45" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1232</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="46" spans="1:4">
@@ -3044,7 +3077,7 @@
       </c>
       <c r="D46" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1228</v>
+        <v>1231</v>
       </c>
     </row>
     <row r="47" spans="1:4">
@@ -3059,7 +3092,7 @@
       </c>
       <c r="D47" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1231</v>
+        <v>1223</v>
       </c>
     </row>
     <row r="48" spans="1:4">
@@ -3074,7 +3107,7 @@
       </c>
       <c r="D48" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1223</v>
+        <v>1231</v>
       </c>
     </row>
     <row r="49" spans="1:4">
@@ -3089,7 +3122,7 @@
       </c>
       <c r="D49" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1231</v>
+        <v>1223</v>
       </c>
     </row>
     <row r="50" spans="1:4">
@@ -3104,7 +3137,7 @@
       </c>
       <c r="D50" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1232</v>
+        <v>1225</v>
       </c>
     </row>
     <row r="51" spans="1:4">
@@ -3119,7 +3152,7 @@
       </c>
       <c r="D51" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1229</v>
+        <v>1226</v>
       </c>
     </row>
   </sheetData>
@@ -3498,7 +3531,7 @@
         <v>274</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>294</v>
+        <v>286</v>
       </c>
       <c r="F14" s="8" t="s">
         <v>275</v>
@@ -3515,16 +3548,16 @@
         <v>1236</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>297</v>
+        <v>289</v>
       </c>
       <c r="C15" s="9" t="s">
         <v>273</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>297</v>
+        <v>289</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>298</v>
+        <v>290</v>
       </c>
       <c r="F15" s="8" t="s">
         <v>275</v>
@@ -3541,16 +3574,16 @@
         <v>1237</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>295</v>
+        <v>287</v>
       </c>
       <c r="C16" s="9" t="s">
         <v>273</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>295</v>
+        <v>287</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>296</v>
+        <v>288</v>
       </c>
       <c r="F16" s="8" t="s">
         <v>275</v>
@@ -3644,8 +3677,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{491D14EC-1CB1-4681-930A-4B9B4015FC83}">
   <dimension ref="A1:P27"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="N1" sqref="N1"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -3707,7 +3740,7 @@
         <v>248</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>276</v>
+        <v>291</v>
       </c>
       <c r="O1" s="1" t="s">
         <v>217</v>
@@ -3753,7 +3786,7 @@
         <v>250</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>277</v>
+        <v>298</v>
       </c>
       <c r="O2" s="2">
         <v>1223</v>
@@ -3799,7 +3832,7 @@
         <v>250</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>278</v>
+        <v>297</v>
       </c>
       <c r="O3" s="1">
         <v>1224</v>
@@ -3845,7 +3878,7 @@
         <v>250</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>278</v>
+        <v>297</v>
       </c>
       <c r="O4" s="2">
         <v>1225</v>
@@ -3891,7 +3924,7 @@
         <v>250</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>278</v>
+        <v>297</v>
       </c>
       <c r="O5" s="1">
         <v>1225</v>
@@ -3937,7 +3970,7 @@
         <v>250</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>278</v>
+        <v>297</v>
       </c>
       <c r="O6" s="1">
         <v>1227</v>
@@ -3983,7 +4016,7 @@
         <v>250</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>278</v>
+        <v>297</v>
       </c>
       <c r="O7" s="1">
         <v>1226</v>
@@ -4029,7 +4062,7 @@
         <v>250</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>279</v>
+        <v>292</v>
       </c>
       <c r="O8" s="2">
         <v>1223</v>
@@ -4075,7 +4108,7 @@
         <v>250</v>
       </c>
       <c r="N9" s="1" t="s">
-        <v>279</v>
+        <v>292</v>
       </c>
       <c r="O9" s="1">
         <v>1223</v>
@@ -4121,7 +4154,7 @@
         <v>250</v>
       </c>
       <c r="N10" s="1" t="s">
-        <v>277</v>
+        <v>300</v>
       </c>
       <c r="O10" s="2">
         <v>1226</v>
@@ -4167,7 +4200,7 @@
         <v>250</v>
       </c>
       <c r="N11" s="1" t="s">
-        <v>279</v>
+        <v>292</v>
       </c>
       <c r="O11" s="1">
         <v>1226</v>
@@ -4213,7 +4246,7 @@
         <v>250</v>
       </c>
       <c r="N12" s="1" t="s">
-        <v>280</v>
+        <v>299</v>
       </c>
       <c r="O12" s="2">
         <v>1226</v>
@@ -4259,7 +4292,7 @@
         <v>250</v>
       </c>
       <c r="N13" s="1" t="s">
-        <v>281</v>
+        <v>313</v>
       </c>
       <c r="O13" s="2">
         <v>1229</v>
@@ -4305,7 +4338,7 @@
         <v>250</v>
       </c>
       <c r="N14" s="1" t="s">
-        <v>281</v>
+        <v>314</v>
       </c>
       <c r="O14" s="1">
         <v>1230</v>
@@ -4351,7 +4384,7 @@
         <v>250</v>
       </c>
       <c r="N15" s="1" t="s">
-        <v>282</v>
+        <v>315</v>
       </c>
       <c r="O15" s="2">
         <v>1231</v>
@@ -4397,7 +4430,7 @@
         <v>250</v>
       </c>
       <c r="N16" s="1" t="s">
-        <v>283</v>
+        <v>301</v>
       </c>
       <c r="O16" s="1">
         <v>1231</v>
@@ -4443,7 +4476,7 @@
         <v>250</v>
       </c>
       <c r="N17" s="1" t="s">
-        <v>283</v>
+        <v>302</v>
       </c>
       <c r="O17" s="2">
         <v>1224</v>
@@ -4491,7 +4524,7 @@
         <v>250</v>
       </c>
       <c r="N18" s="1" t="s">
-        <v>283</v>
+        <v>303</v>
       </c>
       <c r="O18" s="1">
         <v>1225</v>
@@ -4539,7 +4572,7 @@
         <v>250</v>
       </c>
       <c r="N19" s="1" t="s">
-        <v>283</v>
+        <v>304</v>
       </c>
       <c r="O19" s="1">
         <v>1226</v>
@@ -4585,7 +4618,7 @@
         <v>250</v>
       </c>
       <c r="N20" s="1" t="s">
-        <v>283</v>
+        <v>305</v>
       </c>
       <c r="O20" s="1">
         <v>1223</v>
@@ -4631,7 +4664,7 @@
         <v>250</v>
       </c>
       <c r="N21" s="1" t="s">
-        <v>283</v>
+        <v>306</v>
       </c>
       <c r="O21" s="1">
         <v>1229</v>
@@ -4677,7 +4710,7 @@
         <v>250</v>
       </c>
       <c r="N22" s="1" t="s">
-        <v>283</v>
+        <v>307</v>
       </c>
       <c r="O22" s="1">
         <v>1228</v>
@@ -4723,7 +4756,7 @@
         <v>250</v>
       </c>
       <c r="N23" s="1" t="s">
-        <v>283</v>
+        <v>308</v>
       </c>
       <c r="O23" s="1">
         <v>1227</v>
@@ -4734,13 +4767,13 @@
     </row>
     <row r="24" spans="1:16">
       <c r="A24" s="1" t="s">
-        <v>290</v>
+        <v>282</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>284</v>
+        <v>276</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>288</v>
+        <v>280</v>
       </c>
       <c r="D24" s="1"/>
       <c r="E24" s="1" t="s">
@@ -4769,7 +4802,7 @@
         <v>250</v>
       </c>
       <c r="N24" s="1" t="s">
-        <v>283</v>
+        <v>309</v>
       </c>
       <c r="O24" s="1">
         <v>1227</v>
@@ -4780,13 +4813,13 @@
     </row>
     <row r="25" spans="1:16">
       <c r="A25" s="1" t="s">
-        <v>291</v>
+        <v>283</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>285</v>
+        <v>277</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>289</v>
+        <v>281</v>
       </c>
       <c r="D25" s="1"/>
       <c r="E25" s="1" t="s">
@@ -4815,7 +4848,7 @@
         <v>250</v>
       </c>
       <c r="N25" s="1" t="s">
-        <v>283</v>
+        <v>310</v>
       </c>
       <c r="O25" s="1">
         <v>1227</v>
@@ -4826,13 +4859,13 @@
     </row>
     <row r="26" spans="1:16">
       <c r="A26" s="1" t="s">
-        <v>292</v>
+        <v>284</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>286</v>
+        <v>278</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>289</v>
+        <v>281</v>
       </c>
       <c r="D26" s="1"/>
       <c r="E26" s="1" t="s">
@@ -4861,7 +4894,7 @@
         <v>250</v>
       </c>
       <c r="N26" s="1" t="s">
-        <v>283</v>
+        <v>311</v>
       </c>
       <c r="O26" s="1">
         <v>1227</v>
@@ -4872,13 +4905,13 @@
     </row>
     <row r="27" spans="1:16">
       <c r="A27" s="1" t="s">
-        <v>293</v>
+        <v>285</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>287</v>
+        <v>279</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>288</v>
+        <v>280</v>
       </c>
       <c r="D27" s="1"/>
       <c r="E27" s="1" t="s">
@@ -4907,7 +4940,7 @@
         <v>250</v>
       </c>
       <c r="N27" s="1" t="s">
-        <v>283</v>
+        <v>312</v>
       </c>
       <c r="O27" s="1">
         <v>1227</v>
@@ -4926,8 +4959,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28F0C749-0F7B-4353-B0A5-2957163B7B34}">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -4941,7 +4974,7 @@
         <v>214</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>299</v>
+        <v>291</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -4949,7 +4982,7 @@
         <v>179</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -4957,7 +4990,7 @@
         <v>183</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>301</v>
+        <v>293</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -4965,7 +4998,7 @@
         <v>191</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>302</v>
+        <v>294</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -4973,7 +5006,7 @@
         <v>195</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>303</v>
+        <v>295</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -4981,7 +5014,7 @@
         <v>199</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>304</v>
+        <v>296</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -4989,7 +5022,7 @@
         <v>206</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>305</v>
+        <v>316</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update asset CSV data and modify dummy Excel data
</commit_message>
<xml_diff>
--- a/backend/internal/seed/seed_data/mst_dummy_data.xlsx
+++ b/backend/internal/seed/seed_data/mst_dummy_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Uni\Intern SM\Stock Opname App [SOSMIT]\SOSMIT\backend\internal\seed\seed_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2A47D41-0F8F-421E-A3C9-D0EB24531F01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96BADE25-8163-4591-8B59-8D50074CB802}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10540" firstSheet="1" activeTab="4" xr2:uid="{AF28B77B-5B1D-47C2-ADE5-ADF50DA09BCF}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10540" firstSheet="1" activeTab="6" xr2:uid="{AF28B77B-5B1D-47C2-ADE5-ADF50DA09BCF}"/>
   </bookViews>
   <sheets>
     <sheet name="Region" sheetId="1" r:id="rId1"/>
@@ -2622,7 +2622,7 @@
       </c>
       <c r="D10" s="1">
         <f ca="1">RANDBETWEEN(1223,1232)</f>
-        <v>1225</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -2637,7 +2637,7 @@
       </c>
       <c r="D11" s="1">
         <f t="shared" ref="D11:D51" ca="1" si="0">RANDBETWEEN(1223,1232)</f>
-        <v>1228</v>
+        <v>1231</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -2667,7 +2667,7 @@
       </c>
       <c r="D13" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1228</v>
+        <v>1223</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -2682,7 +2682,7 @@
       </c>
       <c r="D14" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1223</v>
+        <v>1232</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -2697,7 +2697,7 @@
       </c>
       <c r="D15" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1230</v>
+        <v>1232</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -2712,7 +2712,7 @@
       </c>
       <c r="D16" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1228</v>
+        <v>1225</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -2727,7 +2727,7 @@
       </c>
       <c r="D17" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1223</v>
+        <v>1230</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -2742,7 +2742,7 @@
       </c>
       <c r="D18" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1226</v>
+        <v>1225</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -2757,7 +2757,7 @@
       </c>
       <c r="D19" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1227</v>
+        <v>1224</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -2772,7 +2772,7 @@
       </c>
       <c r="D20" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1224</v>
+        <v>1230</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -2787,7 +2787,7 @@
       </c>
       <c r="D21" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1225</v>
+        <v>1226</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -2802,7 +2802,7 @@
       </c>
       <c r="D22" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1226</v>
+        <v>1232</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -2817,7 +2817,7 @@
       </c>
       <c r="D23" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1225</v>
+        <v>1229</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -2832,7 +2832,7 @@
       </c>
       <c r="D24" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1224</v>
+        <v>1231</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -2847,7 +2847,7 @@
       </c>
       <c r="D25" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1225</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -2862,7 +2862,7 @@
       </c>
       <c r="D26" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1227</v>
+        <v>1224</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -2877,7 +2877,7 @@
       </c>
       <c r="D27" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1231</v>
+        <v>1232</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -2892,7 +2892,7 @@
       </c>
       <c r="D28" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1227</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -2907,7 +2907,7 @@
       </c>
       <c r="D29" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1225</v>
+        <v>1230</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -2922,7 +2922,7 @@
       </c>
       <c r="D30" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1225</v>
+        <v>1230</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -2937,7 +2937,7 @@
       </c>
       <c r="D31" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1226</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -2967,7 +2967,7 @@
       </c>
       <c r="D33" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1223</v>
+        <v>1225</v>
       </c>
     </row>
     <row r="34" spans="1:4">
@@ -2982,7 +2982,7 @@
       </c>
       <c r="D34" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1226</v>
+        <v>1225</v>
       </c>
     </row>
     <row r="35" spans="1:4">
@@ -2997,7 +2997,7 @@
       </c>
       <c r="D35" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1226</v>
+        <v>1225</v>
       </c>
     </row>
     <row r="36" spans="1:4">
@@ -3012,7 +3012,7 @@
       </c>
       <c r="D36" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1231</v>
+        <v>1223</v>
       </c>
     </row>
     <row r="37" spans="1:4">
@@ -3027,7 +3027,7 @@
       </c>
       <c r="D37" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1231</v>
+        <v>1232</v>
       </c>
     </row>
     <row r="38" spans="1:4">
@@ -3042,7 +3042,7 @@
       </c>
       <c r="D38" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1228</v>
+        <v>1226</v>
       </c>
     </row>
     <row r="39" spans="1:4">
@@ -3057,7 +3057,7 @@
       </c>
       <c r="D39" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1224</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="40" spans="1:4">
@@ -3072,7 +3072,7 @@
       </c>
       <c r="D40" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1224</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="41" spans="1:4">
@@ -3087,7 +3087,7 @@
       </c>
       <c r="D41" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1223</v>
+        <v>1226</v>
       </c>
     </row>
     <row r="42" spans="1:4">
@@ -3102,7 +3102,7 @@
       </c>
       <c r="D42" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1228</v>
+        <v>1231</v>
       </c>
     </row>
     <row r="43" spans="1:4">
@@ -3132,7 +3132,7 @@
       </c>
       <c r="D44" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1226</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="45" spans="1:4">
@@ -3147,7 +3147,7 @@
       </c>
       <c r="D45" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1226</v>
+        <v>1224</v>
       </c>
     </row>
     <row r="46" spans="1:4">
@@ -3177,7 +3177,7 @@
       </c>
       <c r="D47" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1223</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="48" spans="1:4">
@@ -3192,7 +3192,7 @@
       </c>
       <c r="D48" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1232</v>
+        <v>1230</v>
       </c>
     </row>
     <row r="49" spans="1:4">
@@ -3207,7 +3207,7 @@
       </c>
       <c r="D49" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1225</v>
+        <v>1232</v>
       </c>
     </row>
     <row r="50" spans="1:4">
@@ -3237,7 +3237,7 @@
       </c>
       <c r="D51" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1226</v>
+        <v>1224</v>
       </c>
     </row>
   </sheetData>
@@ -3850,7 +3850,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6E05CD4-7C76-4891-A9C7-AB36831BB0B8}">
   <dimension ref="A1:J16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
@@ -4461,8 +4461,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{491D14EC-1CB1-4681-930A-4B9B4015FC83}">
   <dimension ref="A1:P35"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="N9" sqref="N9"/>
+    <sheetView tabSelected="1" topLeftCell="E17" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="P38" sqref="P38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -4577,7 +4577,7 @@
         <v>1223</v>
       </c>
       <c r="P2" s="1">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:16">
@@ -4853,7 +4853,7 @@
         <v>1223</v>
       </c>
       <c r="P8" s="1">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:16">
@@ -4899,7 +4899,7 @@
         <v>1223</v>
       </c>
       <c r="P9" s="1">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:16">
@@ -4945,7 +4945,7 @@
         <v>1226</v>
       </c>
       <c r="P10" s="1">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:16">
@@ -4991,7 +4991,7 @@
         <v>1226</v>
       </c>
       <c r="P11" s="1">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:16">
@@ -5037,7 +5037,7 @@
         <v>1226</v>
       </c>
       <c r="P12" s="1">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="13" spans="1:16">
@@ -5639,7 +5639,7 @@
         <v>1227</v>
       </c>
       <c r="P25" s="1">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="26" spans="1:16">
@@ -5685,7 +5685,7 @@
         <v>1227</v>
       </c>
       <c r="P26" s="1">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="27" spans="1:16">
@@ -5731,7 +5731,7 @@
         <v>1227</v>
       </c>
       <c r="P27" s="1">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="28" spans="1:16">

</xml_diff>

<commit_message>
update User model to handle nullable fields, a.k.a. Vacant user
- Updated User table to allow nullable site_id and cost_center_id.
- Modified User model to use sql.Null types for nullable fields.
- Enhanced user serialization to handle nullable fields in API responses.
- Updated frontend User model to reflect nullable siteID and costCenterID.
- Adjusted asset CSV data to ensure consistency with new User model.
- Added asset_equipment.csv for mapping product varieties to equipment.
- Improved user search functionality in OpnameAsset component.
- Updated validation logic in OpnameAsset component to handle vacant users.
- Refactored titleCase utility function to handle undefined input.
</commit_message>
<xml_diff>
--- a/backend/internal/seed/seed_data/mst_dummy_data.xlsx
+++ b/backend/internal/seed/seed_data/mst_dummy_data.xlsx
@@ -8,22 +8,23 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Uni\Intern SM\Stock Opname App [SOSMIT]\SOSMIT\backend\internal\seed\seed_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96BADE25-8163-4591-8B59-8D50074CB802}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{579FB297-837E-4FC8-A485-4C4A379805CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10540" firstSheet="1" activeTab="6" xr2:uid="{AF28B77B-5B1D-47C2-ADE5-ADF50DA09BCF}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10540" firstSheet="2" activeTab="8" xr2:uid="{AF28B77B-5B1D-47C2-ADE5-ADF50DA09BCF}"/>
   </bookViews>
   <sheets>
     <sheet name="Region" sheetId="1" r:id="rId1"/>
     <sheet name="Site Group" sheetId="2" r:id="rId2"/>
     <sheet name="Site" sheetId="3" r:id="rId3"/>
     <sheet name="SubSite" sheetId="8" r:id="rId4"/>
-    <sheet name="User" sheetId="4" r:id="rId5"/>
-    <sheet name="Cost Center" sheetId="6" r:id="rId6"/>
-    <sheet name="Asset" sheetId="5" r:id="rId7"/>
-    <sheet name="Asset Equipment" sheetId="7" r:id="rId8"/>
+    <sheet name="ApprovalPath" sheetId="9" r:id="rId5"/>
+    <sheet name="User" sheetId="4" r:id="rId6"/>
+    <sheet name="Cost Center" sheetId="6" r:id="rId7"/>
+    <sheet name="Asset" sheetId="5" r:id="rId8"/>
+    <sheet name="Asset Equipment" sheetId="7" r:id="rId9"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">'Asset Equipment'!$A$1:$A$7</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">'Asset Equipment'!$A$1:$A$7</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -46,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="745" uniqueCount="345">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="739" uniqueCount="348">
   <si>
     <t>id</t>
   </si>
@@ -918,81 +919,6 @@
     <t>equipments</t>
   </si>
   <si>
-    <t>Unit, Kabel power</t>
-  </si>
-  <si>
-    <t>Unit, Tas, Kabel power, Adaptor</t>
-  </si>
-  <si>
-    <t>Unit, Kabel power, Kabel VGA, Kabel HDMI</t>
-  </si>
-  <si>
-    <t>Unit, Kabel power, Kabel UPS</t>
-  </si>
-  <si>
-    <t>Unit, Simcard, Handstrap, Adaptor, Kabel USB</t>
-  </si>
-  <si>
-    <t>Unit, Tas</t>
-  </si>
-  <si>
-    <t>Unit, Kabel power, Keyboard, Mouse</t>
-  </si>
-  <si>
-    <t>Unit, Kabel power, Keyboard</t>
-  </si>
-  <si>
-    <t>Unit, Kabel power, Adaptor (s/n: ADQ9175G32)</t>
-  </si>
-  <si>
-    <t>Unit, Tas, Tali tas, Adaptor (s/n: ADQ917645D), Kabel USB</t>
-  </si>
-  <si>
-    <t>Unit, Tas, Tali tas, Adaptor (s/n: ADQ9176222), Kabel USB</t>
-  </si>
-  <si>
-    <t>Unit, Tas, Tali tas, Adaptor (s/n: ADQ917345D), Kabel USB</t>
-  </si>
-  <si>
-    <t>Unit, Tas, Tali tas, Adaptor (s/n: ADQ2FR645D), Kabel USB</t>
-  </si>
-  <si>
-    <t>Unit, Tas, Tali tas, Adaptor (s/n: ADQ9175KJT), Kabel USB</t>
-  </si>
-  <si>
-    <t>Unit, Tas, Tali tas, Adaptor (s/n: ADQ917SF54), Kabel USB</t>
-  </si>
-  <si>
-    <t>Unit, Tas, Tali tas, Adaptor (s/n: ADQ91764G6), Kabel USB</t>
-  </si>
-  <si>
-    <t>Unit, Tas, Tali tas, Adaptor (s/n: ADQ9174444), Kabel USB</t>
-  </si>
-  <si>
-    <t>Unit, Tas, Tali tas, Adaptor (s/n: ADQ13F45D), Kabel USB</t>
-  </si>
-  <si>
-    <t>Unit, Tas, Tali tas, Adaptor (s/n: ADQ91778KL), Kabel USB</t>
-  </si>
-  <si>
-    <t>Unit, Tas, Tali tas, Adaptor (s/n: ADQ91721ER), Kabel USB</t>
-  </si>
-  <si>
-    <t>Unit, Tas, Tali tas, Adaptor (s/n: ADY97O645D), Kabel USB</t>
-  </si>
-  <si>
-    <t>Unit, Simcard, Handstrap, Adaptor (s/n: ADQ917YY54), Kabel USB</t>
-  </si>
-  <si>
-    <t>Unit, Simcard, Handstrap, Adaptor (s/n: ADQ9172P1O), Kabel USB</t>
-  </si>
-  <si>
-    <t>Unit, Simcard, Adaptor (s/n: ADQ902DFG4), Kabel USB</t>
-  </si>
-  <si>
-    <t>Unit, Tas, Tali tas, Adaptor, Kabel USB, Bracket</t>
-  </si>
-  <si>
     <t>Meeting Point Retail Denpasar</t>
   </si>
   <si>
@@ -1062,25 +988,109 @@
     <t>division</t>
   </si>
   <si>
-    <t>IT</t>
-  </si>
-  <si>
     <t>Sales</t>
   </si>
   <si>
-    <t>Administration</t>
-  </si>
-  <si>
     <t>Management</t>
   </si>
   <si>
-    <t>Support</t>
-  </si>
-  <si>
-    <t>TMC</t>
-  </si>
-  <si>
-    <t>Regional Operations</t>
+    <t>sequence</t>
+  </si>
+  <si>
+    <t>IT Services Manager</t>
+  </si>
+  <si>
+    <t>L1 Support</t>
+  </si>
+  <si>
+    <t>Area Manager</t>
+  </si>
+  <si>
+    <t>VACANT</t>
+  </si>
+  <si>
+    <t>IT Services</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HEAD </t>
+  </si>
+  <si>
+    <t>Finance &amp; Accounting Manager</t>
+  </si>
+  <si>
+    <t>Kabel power, Keyboard, Mouse</t>
+  </si>
+  <si>
+    <t>Tas</t>
+  </si>
+  <si>
+    <t>Kabel power</t>
+  </si>
+  <si>
+    <t>Kabel power, Adaptor (s/n: ADQ9175G32)</t>
+  </si>
+  <si>
+    <t>Kabel power, Keyboard</t>
+  </si>
+  <si>
+    <t>Simcard, Handstrap, Adaptor (s/n: ADQ917YY54), Kabel USB</t>
+  </si>
+  <si>
+    <t>Simcard, Handstrap, Adaptor (s/n: ADQ9172P1O), Kabel USB</t>
+  </si>
+  <si>
+    <t>Simcard, Adaptor (s/n: ADQ902DFG4), Kabel USB</t>
+  </si>
+  <si>
+    <t>Tas, Tali tas, Adaptor (s/n: ADQ917645D), Kabel USB</t>
+  </si>
+  <si>
+    <t>Tas, Tali tas, Adaptor (s/n: ADQ9176222), Kabel USB</t>
+  </si>
+  <si>
+    <t>Tas, Tali tas, Adaptor (s/n: ADQ917345D), Kabel USB</t>
+  </si>
+  <si>
+    <t>Tas, Tali tas, Adaptor (s/n: ADQ2FR645D), Kabel USB</t>
+  </si>
+  <si>
+    <t>Tas, Tali tas, Adaptor (s/n: ADQ9175KJT), Kabel USB</t>
+  </si>
+  <si>
+    <t>Tas, Tali tas, Adaptor (s/n: ADQ917SF54), Kabel USB</t>
+  </si>
+  <si>
+    <t>Tas, Tali tas, Adaptor (s/n: ADQ91764G6), Kabel USB</t>
+  </si>
+  <si>
+    <t>Tas, Tali tas, Adaptor (s/n: ADQ9174444), Kabel USB</t>
+  </si>
+  <si>
+    <t>Tas, Tali tas, Adaptor (s/n: ADQ13F45D), Kabel USB</t>
+  </si>
+  <si>
+    <t>Tas, Tali tas, Adaptor (s/n: ADQ91778KL), Kabel USB</t>
+  </si>
+  <si>
+    <t>Tas, Tali tas, Adaptor (s/n: ADQ91721ER), Kabel USB</t>
+  </si>
+  <si>
+    <t>Tas, Tali tas, Adaptor (s/n: ADY97O645D), Kabel USB</t>
+  </si>
+  <si>
+    <t>Tas, Kabel power, Adaptor</t>
+  </si>
+  <si>
+    <t>Kabel power, Kabel VGA, Kabel HDMI</t>
+  </si>
+  <si>
+    <t>Kabel power, Kabel UPS</t>
+  </si>
+  <si>
+    <t>Simcard, Handstrap, Adaptor, Kabel USB</t>
+  </si>
+  <si>
+    <t>Tas, Tali tas, Adaptor, Kabel USB, Bracket</t>
   </si>
 </sst>
 </file>
@@ -1133,7 +1143,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -1156,13 +1166,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1181,6 +1202,7 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -2473,7 +2495,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E6AD482-693C-4526-A8EF-051504D339CF}">
   <dimension ref="A1:D51"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A15" workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
@@ -2492,10 +2514,10 @@
         <v>80</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>332</v>
+        <v>307</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>333</v>
+        <v>308</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -2622,7 +2644,7 @@
       </c>
       <c r="D10" s="1">
         <f ca="1">RANDBETWEEN(1223,1232)</f>
-        <v>1228</v>
+        <v>1226</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -2637,7 +2659,7 @@
       </c>
       <c r="D11" s="1">
         <f t="shared" ref="D11:D51" ca="1" si="0">RANDBETWEEN(1223,1232)</f>
-        <v>1231</v>
+        <v>1226</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -2652,7 +2674,7 @@
       </c>
       <c r="D12" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1227</v>
+        <v>1226</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -2667,7 +2689,7 @@
       </c>
       <c r="D13" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1223</v>
+        <v>1224</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -2697,7 +2719,7 @@
       </c>
       <c r="D15" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1232</v>
+        <v>1223</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -2712,7 +2734,7 @@
       </c>
       <c r="D16" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1225</v>
+        <v>1230</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -2727,7 +2749,7 @@
       </c>
       <c r="D17" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1230</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -2742,7 +2764,7 @@
       </c>
       <c r="D18" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1225</v>
+        <v>1231</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -2757,7 +2779,7 @@
       </c>
       <c r="D19" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1224</v>
+        <v>1232</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -2772,7 +2794,7 @@
       </c>
       <c r="D20" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1230</v>
+        <v>1223</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -2787,7 +2809,7 @@
       </c>
       <c r="D21" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1226</v>
+        <v>1230</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -2802,7 +2824,7 @@
       </c>
       <c r="D22" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1232</v>
+        <v>1224</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -2817,7 +2839,7 @@
       </c>
       <c r="D23" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1229</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -2832,7 +2854,7 @@
       </c>
       <c r="D24" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1231</v>
+        <v>1229</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -2847,7 +2869,7 @@
       </c>
       <c r="D25" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1227</v>
+        <v>1230</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -2892,7 +2914,7 @@
       </c>
       <c r="D28" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1228</v>
+        <v>1231</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -2922,7 +2944,7 @@
       </c>
       <c r="D30" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1230</v>
+        <v>1224</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -2937,7 +2959,7 @@
       </c>
       <c r="D31" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1227</v>
+        <v>1231</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -2952,7 +2974,7 @@
       </c>
       <c r="D32" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1230</v>
+        <v>1232</v>
       </c>
     </row>
     <row r="33" spans="1:4">
@@ -2982,7 +3004,7 @@
       </c>
       <c r="D34" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1225</v>
+        <v>1226</v>
       </c>
     </row>
     <row r="35" spans="1:4">
@@ -3012,7 +3034,7 @@
       </c>
       <c r="D36" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1223</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="37" spans="1:4">
@@ -3027,7 +3049,7 @@
       </c>
       <c r="D37" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1232</v>
+        <v>1229</v>
       </c>
     </row>
     <row r="38" spans="1:4">
@@ -3042,7 +3064,7 @@
       </c>
       <c r="D38" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1226</v>
+        <v>1225</v>
       </c>
     </row>
     <row r="39" spans="1:4">
@@ -3057,7 +3079,7 @@
       </c>
       <c r="D39" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1227</v>
+        <v>1225</v>
       </c>
     </row>
     <row r="40" spans="1:4">
@@ -3072,7 +3094,7 @@
       </c>
       <c r="D40" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1228</v>
+        <v>1226</v>
       </c>
     </row>
     <row r="41" spans="1:4">
@@ -3087,7 +3109,7 @@
       </c>
       <c r="D41" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1226</v>
+        <v>1223</v>
       </c>
     </row>
     <row r="42" spans="1:4">
@@ -3102,7 +3124,7 @@
       </c>
       <c r="D42" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1231</v>
+        <v>1230</v>
       </c>
     </row>
     <row r="43" spans="1:4">
@@ -3117,7 +3139,7 @@
       </c>
       <c r="D43" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1223</v>
+        <v>1231</v>
       </c>
     </row>
     <row r="44" spans="1:4">
@@ -3132,7 +3154,7 @@
       </c>
       <c r="D44" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1228</v>
+        <v>1231</v>
       </c>
     </row>
     <row r="45" spans="1:4">
@@ -3147,7 +3169,7 @@
       </c>
       <c r="D45" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1224</v>
+        <v>1229</v>
       </c>
     </row>
     <row r="46" spans="1:4">
@@ -3162,7 +3184,7 @@
       </c>
       <c r="D46" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1226</v>
+        <v>1231</v>
       </c>
     </row>
     <row r="47" spans="1:4">
@@ -3177,7 +3199,7 @@
       </c>
       <c r="D47" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1227</v>
+        <v>1226</v>
       </c>
     </row>
     <row r="48" spans="1:4">
@@ -3192,7 +3214,7 @@
       </c>
       <c r="D48" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1230</v>
+        <v>1232</v>
       </c>
     </row>
     <row r="49" spans="1:4">
@@ -3207,7 +3229,7 @@
       </c>
       <c r="D49" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1232</v>
+        <v>1224</v>
       </c>
     </row>
     <row r="50" spans="1:4">
@@ -3222,7 +3244,7 @@
       </c>
       <c r="D50" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1224</v>
+        <v>1230</v>
       </c>
     </row>
     <row r="51" spans="1:4">
@@ -3237,7 +3259,7 @@
       </c>
       <c r="D51" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1224</v>
+        <v>1229</v>
       </c>
     </row>
   </sheetData>
@@ -3263,7 +3285,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>334</v>
+        <v>309</v>
       </c>
       <c r="C1" s="5" t="s">
         <v>132</v>
@@ -3274,7 +3296,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>315</v>
+        <v>290</v>
       </c>
       <c r="C2" s="5">
         <v>1</v>
@@ -3285,7 +3307,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>316</v>
+        <v>291</v>
       </c>
       <c r="C3" s="5">
         <v>1</v>
@@ -3847,11 +3869,96 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6E05CD4-7C76-4891-A9C7-AB36831BB0B8}">
-  <dimension ref="A1:J16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9F1D321-262E-4B92-9ED1-453EAE798920}">
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="1" max="1" width="26" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.81640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>226</v>
+      </c>
+      <c r="B1" t="s">
+        <v>315</v>
+      </c>
+      <c r="C1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>318</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>317</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>316</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>322</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
+        <v>316</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6E05CD4-7C76-4891-A9C7-AB36831BB0B8}">
+  <dimension ref="A1:J18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -3887,10 +3994,10 @@
         <v>226</v>
       </c>
       <c r="G1" s="8" t="s">
-        <v>336</v>
+        <v>311</v>
       </c>
       <c r="H1" s="8" t="s">
-        <v>337</v>
+        <v>312</v>
       </c>
       <c r="I1" s="8" t="s">
         <v>132</v>
@@ -3900,125 +4007,103 @@
       </c>
     </row>
     <row r="2" spans="1:10">
-      <c r="A2" s="6">
+      <c r="A2" s="8">
+        <v>1</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>319</v>
+      </c>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="8"/>
+      <c r="J2" s="8"/>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" s="6">
         <v>1223</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B3" s="3" t="s">
         <v>135</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>271</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="F2" s="8" t="s">
-        <v>137</v>
-      </c>
-      <c r="G2" s="8" t="s">
-        <v>338</v>
-      </c>
-      <c r="H2" s="8" t="s">
-        <v>342</v>
-      </c>
-      <c r="I2" s="7">
-        <v>30</v>
-      </c>
-      <c r="J2" s="8">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10">
-      <c r="A3" s="8">
-        <v>1224</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>138</v>
       </c>
       <c r="C3" s="9" t="s">
         <v>271</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>339</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>343</v>
-      </c>
+        <v>136</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>320</v>
+      </c>
+      <c r="H3" s="8"/>
       <c r="I3" s="7">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="J3" s="8">
-        <v>410</v>
+        <v>110</v>
       </c>
     </row>
     <row r="4" spans="1:10">
-      <c r="A4" s="6">
-        <v>1225</v>
+      <c r="A4" s="8">
+        <v>1224</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="C4" s="9" t="s">
         <v>271</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>339</v>
-      </c>
+        <v>139</v>
+      </c>
+      <c r="G4" s="3"/>
       <c r="H4" s="3" t="s">
-        <v>343</v>
+        <v>313</v>
       </c>
       <c r="I4" s="7">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J4" s="8">
-        <v>240</v>
+        <v>410</v>
       </c>
     </row>
     <row r="5" spans="1:10">
-      <c r="A5" s="8">
-        <v>1226</v>
+      <c r="A5" s="6">
+        <v>1225</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="C5" s="9" t="s">
         <v>271</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>339</v>
-      </c>
+        <v>143</v>
+      </c>
+      <c r="G5" s="3"/>
       <c r="H5" s="3" t="s">
-        <v>343</v>
+        <v>313</v>
       </c>
       <c r="I5" s="7">
         <v>3</v>
@@ -4028,61 +4113,57 @@
       </c>
     </row>
     <row r="6" spans="1:10">
-      <c r="A6" s="6">
-        <v>1227</v>
+      <c r="A6" s="8">
+        <v>1226</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="C6" s="9" t="s">
         <v>271</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="G6" s="3" t="s">
-        <v>339</v>
-      </c>
+      <c r="G6" s="3"/>
       <c r="H6" s="3" t="s">
-        <v>343</v>
+        <v>313</v>
       </c>
       <c r="I6" s="7">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J6" s="8">
-        <v>230</v>
+        <v>240</v>
       </c>
     </row>
     <row r="7" spans="1:10">
-      <c r="A7" s="8">
-        <v>1228</v>
+      <c r="A7" s="6">
+        <v>1227</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="C7" s="9" t="s">
         <v>271</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="F7" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="G7" s="3" t="s">
-        <v>339</v>
-      </c>
+      <c r="G7" s="3"/>
       <c r="H7" s="3" t="s">
-        <v>343</v>
+        <v>313</v>
       </c>
       <c r="I7" s="7">
         <v>1</v>
@@ -4092,29 +4173,27 @@
       </c>
     </row>
     <row r="8" spans="1:10">
-      <c r="A8" s="6">
-        <v>1229</v>
+      <c r="A8" s="8">
+        <v>1228</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C8" s="9" t="s">
         <v>271</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="F8" s="8" t="s">
-        <v>156</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>339</v>
-      </c>
+        <v>154</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="G8" s="3"/>
       <c r="H8" s="3" t="s">
-        <v>343</v>
+        <v>313</v>
       </c>
       <c r="I8" s="7">
         <v>1</v>
@@ -4124,29 +4203,27 @@
       </c>
     </row>
     <row r="9" spans="1:10">
-      <c r="A9" s="8">
-        <v>1230</v>
+      <c r="A9" s="6">
+        <v>1229</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="C9" s="9" t="s">
         <v>271</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>161</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>339</v>
-      </c>
+        <v>158</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="G9" s="3"/>
       <c r="H9" s="3" t="s">
-        <v>343</v>
+        <v>313</v>
       </c>
       <c r="I9" s="7">
         <v>1</v>
@@ -4156,29 +4233,27 @@
       </c>
     </row>
     <row r="10" spans="1:10">
-      <c r="A10" s="6">
-        <v>1231</v>
+      <c r="A10" s="8">
+        <v>1230</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C10" s="9" t="s">
         <v>271</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>164</v>
-      </c>
-      <c r="F10" s="8" t="s">
-        <v>156</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>339</v>
-      </c>
+        <v>161</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="G10" s="3"/>
       <c r="H10" s="3" t="s">
-        <v>343</v>
+        <v>313</v>
       </c>
       <c r="I10" s="7">
         <v>1</v>
@@ -4188,209 +4263,232 @@
       </c>
     </row>
     <row r="11" spans="1:10">
-      <c r="A11" s="8">
-        <v>1232</v>
+      <c r="A11" s="6">
+        <v>1231</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="C11" s="9" t="s">
         <v>271</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>148</v>
+        <v>164</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>137</v>
-      </c>
-      <c r="G11" s="8" t="s">
-        <v>338</v>
-      </c>
-      <c r="H11" s="8" t="s">
-        <v>342</v>
-      </c>
-      <c r="I11" s="8">
-        <v>25</v>
+        <v>156</v>
+      </c>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3" t="s">
+        <v>313</v>
+      </c>
+      <c r="I11" s="7">
+        <v>1</v>
       </c>
       <c r="J11" s="8">
-        <v>110</v>
+        <v>230</v>
       </c>
     </row>
     <row r="12" spans="1:10">
       <c r="A12" s="8">
-        <v>1233</v>
+        <v>1232</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C12" s="9" t="s">
         <v>271</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>170</v>
+        <v>148</v>
       </c>
       <c r="F12" s="8" t="s">
-        <v>168</v>
+        <v>137</v>
       </c>
       <c r="G12" s="8" t="s">
-        <v>340</v>
-      </c>
-      <c r="H12" s="8" t="s">
-        <v>223</v>
-      </c>
+        <v>320</v>
+      </c>
+      <c r="H12" s="8"/>
       <c r="I12" s="8">
-        <v>4</v>
+        <v>25</v>
       </c>
       <c r="J12" s="8">
-        <v>350</v>
+        <v>110</v>
       </c>
     </row>
     <row r="13" spans="1:10">
       <c r="A13" s="8">
-        <v>1234</v>
-      </c>
-      <c r="B13" s="8" t="s">
-        <v>171</v>
+        <v>1233</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>167</v>
       </c>
       <c r="C13" s="9" t="s">
         <v>271</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>172</v>
-      </c>
-      <c r="G13" s="8" t="s">
-        <v>338</v>
-      </c>
+        <v>168</v>
+      </c>
+      <c r="G13" s="8"/>
       <c r="H13" s="8" t="s">
-        <v>342</v>
+        <v>223</v>
       </c>
       <c r="I13" s="8">
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="J13" s="8">
-        <v>110</v>
+        <v>350</v>
       </c>
     </row>
     <row r="14" spans="1:10">
       <c r="A14" s="8">
-        <v>1235</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>272</v>
+        <v>1234</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>171</v>
       </c>
       <c r="C14" s="9" t="s">
         <v>271</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>272</v>
+        <v>171</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>284</v>
+        <v>173</v>
       </c>
       <c r="F14" s="8" t="s">
-        <v>273</v>
+        <v>172</v>
       </c>
       <c r="G14" s="8" t="s">
-        <v>341</v>
-      </c>
-      <c r="H14" s="8" t="s">
-        <v>344</v>
-      </c>
+        <v>320</v>
+      </c>
+      <c r="H14" s="8"/>
       <c r="I14" s="8">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="J14" s="8">
-        <v>230</v>
+        <v>110</v>
       </c>
     </row>
     <row r="15" spans="1:10">
       <c r="A15" s="8">
-        <v>1236</v>
+        <v>1235</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>287</v>
+        <v>272</v>
       </c>
       <c r="C15" s="9" t="s">
         <v>271</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>287</v>
+        <v>272</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="F15" s="8" t="s">
         <v>273</v>
       </c>
-      <c r="G15" s="8" t="s">
-        <v>341</v>
-      </c>
+      <c r="G15" s="8"/>
       <c r="H15" s="8" t="s">
-        <v>344</v>
+        <v>314</v>
       </c>
       <c r="I15" s="8">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="J15" s="8">
-        <v>410</v>
+        <v>230</v>
       </c>
     </row>
     <row r="16" spans="1:10">
       <c r="A16" s="8">
-        <v>1237</v>
+        <v>1236</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>285</v>
+        <v>287</v>
       </c>
       <c r="C16" s="9" t="s">
         <v>271</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>285</v>
+        <v>287</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="F16" s="8" t="s">
         <v>273</v>
       </c>
-      <c r="G16" s="8" t="s">
-        <v>341</v>
-      </c>
+      <c r="G16" s="8"/>
       <c r="H16" s="8" t="s">
-        <v>344</v>
+        <v>314</v>
       </c>
       <c r="I16" s="8">
+        <v>14</v>
+      </c>
+      <c r="J16" s="8">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10">
+      <c r="A17" s="8">
+        <v>1237</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>285</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>271</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>285</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>286</v>
+      </c>
+      <c r="F17" s="8" t="s">
+        <v>321</v>
+      </c>
+      <c r="G17" s="8" t="s">
+        <v>314</v>
+      </c>
+      <c r="H17" s="8"/>
+      <c r="I17" s="8">
         <v>25</v>
       </c>
-      <c r="J16" s="8">
+      <c r="J17" s="8">
         <v>110</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10">
+      <c r="A18" s="10">
+        <v>1238</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{326C7255-3775-42C0-8CED-A0F3BD8EC552}"/>
-    <hyperlink ref="C14" r:id="rId2" xr:uid="{3075A95B-B014-4146-9A02-CE8105DDA61C}"/>
-    <hyperlink ref="C15" r:id="rId3" xr:uid="{AFA86EE8-5F45-4116-A3FB-D1EBD86D2849}"/>
-    <hyperlink ref="C16" r:id="rId4" xr:uid="{4D1991A4-676E-4D81-B282-274D9EC0BE3E}"/>
+    <hyperlink ref="C3" r:id="rId1" xr:uid="{326C7255-3775-42C0-8CED-A0F3BD8EC552}"/>
+    <hyperlink ref="C15" r:id="rId2" xr:uid="{3075A95B-B014-4146-9A02-CE8105DDA61C}"/>
+    <hyperlink ref="C16" r:id="rId3" xr:uid="{AFA86EE8-5F45-4116-A3FB-D1EBD86D2849}"/>
+    <hyperlink ref="C17" r:id="rId4" xr:uid="{4D1991A4-676E-4D81-B282-274D9EC0BE3E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7DF7A36-0BE1-4085-9FD3-20961A4A2C2E}">
   <dimension ref="A1:B6"/>
   <sheetViews>
@@ -4457,12 +4555,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{491D14EC-1CB1-4681-930A-4B9B4015FC83}">
   <dimension ref="A1:P35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E17" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="P38" sqref="P38"/>
+    <sheetView topLeftCell="G1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Q12" sqref="Q12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -4479,7 +4577,8 @@
     <col min="10" max="10" width="10.453125" customWidth="1"/>
     <col min="11" max="11" width="21" customWidth="1"/>
     <col min="12" max="12" width="14.54296875" customWidth="1"/>
-    <col min="13" max="14" width="16.54296875" customWidth="1"/>
+    <col min="13" max="13" width="20.6328125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="56.453125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="9.7265625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="10" customWidth="1"/>
   </cols>
@@ -4531,7 +4630,7 @@
         <v>216</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>335</v>
+        <v>310</v>
       </c>
     </row>
     <row r="2" spans="1:16">
@@ -4571,7 +4670,7 @@
         <v>248</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>296</v>
+        <v>323</v>
       </c>
       <c r="O2" s="2">
         <v>1223</v>
@@ -4617,7 +4716,7 @@
         <v>248</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>295</v>
+        <v>324</v>
       </c>
       <c r="O3" s="1">
         <v>1224</v>
@@ -4663,7 +4762,7 @@
         <v>248</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>295</v>
+        <v>324</v>
       </c>
       <c r="O4" s="2">
         <v>1225</v>
@@ -4709,7 +4808,7 @@
         <v>248</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>295</v>
+        <v>324</v>
       </c>
       <c r="O5" s="1">
         <v>1225</v>
@@ -4755,7 +4854,7 @@
         <v>248</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>295</v>
+        <v>324</v>
       </c>
       <c r="O6" s="1">
         <v>1227</v>
@@ -4801,7 +4900,7 @@
         <v>248</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>295</v>
+        <v>324</v>
       </c>
       <c r="O7" s="1">
         <v>1226</v>
@@ -4847,7 +4946,7 @@
         <v>248</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>290</v>
+        <v>325</v>
       </c>
       <c r="O8" s="2">
         <v>1223</v>
@@ -4893,7 +4992,7 @@
         <v>248</v>
       </c>
       <c r="N9" s="1" t="s">
-        <v>290</v>
+        <v>325</v>
       </c>
       <c r="O9" s="1">
         <v>1223</v>
@@ -4939,7 +5038,7 @@
         <v>248</v>
       </c>
       <c r="N10" s="1" t="s">
-        <v>298</v>
+        <v>326</v>
       </c>
       <c r="O10" s="2">
         <v>1226</v>
@@ -4985,7 +5084,7 @@
         <v>248</v>
       </c>
       <c r="N11" s="1" t="s">
-        <v>290</v>
+        <v>325</v>
       </c>
       <c r="O11" s="1">
         <v>1226</v>
@@ -5031,7 +5130,7 @@
         <v>248</v>
       </c>
       <c r="N12" s="1" t="s">
-        <v>297</v>
+        <v>327</v>
       </c>
       <c r="O12" s="2">
         <v>1226</v>
@@ -5077,7 +5176,7 @@
         <v>248</v>
       </c>
       <c r="N13" s="1" t="s">
-        <v>311</v>
+        <v>328</v>
       </c>
       <c r="O13" s="2">
         <v>1229</v>
@@ -5123,7 +5222,7 @@
         <v>248</v>
       </c>
       <c r="N14" s="1" t="s">
-        <v>312</v>
+        <v>329</v>
       </c>
       <c r="O14" s="1">
         <v>1230</v>
@@ -5169,7 +5268,7 @@
         <v>248</v>
       </c>
       <c r="N15" s="1" t="s">
-        <v>313</v>
+        <v>330</v>
       </c>
       <c r="O15" s="2">
         <v>1231</v>
@@ -5215,7 +5314,7 @@
         <v>248</v>
       </c>
       <c r="N16" s="1" t="s">
-        <v>299</v>
+        <v>331</v>
       </c>
       <c r="O16" s="1">
         <v>1231</v>
@@ -5261,7 +5360,7 @@
         <v>248</v>
       </c>
       <c r="N17" s="1" t="s">
-        <v>300</v>
+        <v>332</v>
       </c>
       <c r="O17" s="2">
         <v>1224</v>
@@ -5309,7 +5408,7 @@
         <v>248</v>
       </c>
       <c r="N18" s="1" t="s">
-        <v>301</v>
+        <v>333</v>
       </c>
       <c r="O18" s="1">
         <v>1225</v>
@@ -5357,7 +5456,7 @@
         <v>248</v>
       </c>
       <c r="N19" s="1" t="s">
-        <v>302</v>
+        <v>334</v>
       </c>
       <c r="O19" s="1">
         <v>1226</v>
@@ -5403,7 +5502,7 @@
         <v>248</v>
       </c>
       <c r="N20" s="1" t="s">
-        <v>303</v>
+        <v>335</v>
       </c>
       <c r="O20" s="1">
         <v>1223</v>
@@ -5449,7 +5548,7 @@
         <v>248</v>
       </c>
       <c r="N21" s="1" t="s">
-        <v>304</v>
+        <v>336</v>
       </c>
       <c r="O21" s="1">
         <v>1229</v>
@@ -5495,7 +5594,7 @@
         <v>248</v>
       </c>
       <c r="N22" s="1" t="s">
-        <v>305</v>
+        <v>337</v>
       </c>
       <c r="O22" s="1">
         <v>1228</v>
@@ -5541,7 +5640,7 @@
         <v>248</v>
       </c>
       <c r="N23" s="1" t="s">
-        <v>306</v>
+        <v>338</v>
       </c>
       <c r="O23" s="1">
         <v>1227</v>
@@ -5587,7 +5686,7 @@
         <v>248</v>
       </c>
       <c r="N24" s="1" t="s">
-        <v>307</v>
+        <v>339</v>
       </c>
       <c r="O24" s="1">
         <v>1227</v>
@@ -5633,7 +5732,7 @@
         <v>248</v>
       </c>
       <c r="N25" s="1" t="s">
-        <v>308</v>
+        <v>340</v>
       </c>
       <c r="O25" s="1">
         <v>1227</v>
@@ -5679,7 +5778,7 @@
         <v>248</v>
       </c>
       <c r="N26" s="1" t="s">
-        <v>309</v>
+        <v>341</v>
       </c>
       <c r="O26" s="1">
         <v>1227</v>
@@ -5725,7 +5824,7 @@
         <v>248</v>
       </c>
       <c r="N27" s="1" t="s">
-        <v>310</v>
+        <v>342</v>
       </c>
       <c r="O27" s="1">
         <v>1227</v>
@@ -5736,10 +5835,10 @@
     </row>
     <row r="28" spans="1:16">
       <c r="A28" s="1" t="s">
-        <v>317</v>
+        <v>292</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>324</v>
+        <v>299</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>175</v>
@@ -5771,7 +5870,7 @@
         <v>248</v>
       </c>
       <c r="N28" s="1" t="s">
-        <v>298</v>
+        <v>326</v>
       </c>
       <c r="O28" s="2">
         <v>1226</v>
@@ -5782,10 +5881,10 @@
     </row>
     <row r="29" spans="1:16">
       <c r="A29" s="1" t="s">
-        <v>318</v>
+        <v>293</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>325</v>
+        <v>300</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>175</v>
@@ -5817,7 +5916,7 @@
         <v>248</v>
       </c>
       <c r="N29" s="1" t="s">
-        <v>290</v>
+        <v>325</v>
       </c>
       <c r="O29" s="1">
         <v>1226</v>
@@ -5828,10 +5927,10 @@
     </row>
     <row r="30" spans="1:16">
       <c r="A30" s="1" t="s">
-        <v>319</v>
+        <v>294</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>326</v>
+        <v>301</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>175</v>
@@ -5863,7 +5962,7 @@
         <v>248</v>
       </c>
       <c r="N30" s="1" t="s">
-        <v>297</v>
+        <v>327</v>
       </c>
       <c r="O30" s="2">
         <v>1226</v>
@@ -5874,10 +5973,10 @@
     </row>
     <row r="31" spans="1:16">
       <c r="A31" s="1" t="s">
-        <v>320</v>
+        <v>295</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>327</v>
+        <v>302</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>175</v>
@@ -5909,10 +6008,10 @@
         <v>248</v>
       </c>
       <c r="N31" s="1" t="s">
-        <v>311</v>
+        <v>328</v>
       </c>
       <c r="O31" s="2">
-        <v>1229</v>
+        <v>1</v>
       </c>
       <c r="P31" s="1">
         <v>3</v>
@@ -5920,10 +6019,10 @@
     </row>
     <row r="32" spans="1:16">
       <c r="A32" s="1" t="s">
-        <v>321</v>
+        <v>296</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>328</v>
+        <v>303</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>279</v>
@@ -5955,10 +6054,10 @@
         <v>248</v>
       </c>
       <c r="N32" s="1" t="s">
-        <v>312</v>
+        <v>329</v>
       </c>
       <c r="O32" s="1">
-        <v>1230</v>
+        <v>1</v>
       </c>
       <c r="P32" s="1">
         <v>3</v>
@@ -5966,10 +6065,10 @@
     </row>
     <row r="33" spans="1:16">
       <c r="A33" s="1" t="s">
-        <v>322</v>
+        <v>297</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>329</v>
+        <v>304</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>279</v>
@@ -6001,10 +6100,10 @@
         <v>248</v>
       </c>
       <c r="N33" s="1" t="s">
-        <v>313</v>
+        <v>330</v>
       </c>
       <c r="O33" s="2">
-        <v>1231</v>
+        <v>1</v>
       </c>
       <c r="P33" s="1">
         <v>3</v>
@@ -6015,7 +6114,7 @@
         <v>283</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>330</v>
+        <v>305</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>175</v>
@@ -6047,10 +6146,10 @@
         <v>248</v>
       </c>
       <c r="N34" s="1" t="s">
-        <v>299</v>
+        <v>331</v>
       </c>
       <c r="O34" s="1">
-        <v>1231</v>
+        <v>1</v>
       </c>
       <c r="P34" s="1">
         <v>3</v>
@@ -6058,10 +6157,10 @@
     </row>
     <row r="35" spans="1:16">
       <c r="A35" s="1" t="s">
-        <v>323</v>
+        <v>298</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>331</v>
+        <v>306</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>175</v>
@@ -6093,10 +6192,10 @@
         <v>248</v>
       </c>
       <c r="N35" s="1" t="s">
-        <v>300</v>
+        <v>332</v>
       </c>
       <c r="O35" s="2">
-        <v>1224</v>
+        <v>1</v>
       </c>
       <c r="P35" s="1">
         <v>3</v>
@@ -6108,12 +6207,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28F0C749-0F7B-4353-B0A5-2957163B7B34}">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -6135,7 +6234,7 @@
         <v>178</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>296</v>
+        <v>323</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -6143,7 +6242,7 @@
         <v>182</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>291</v>
+        <v>343</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -6151,7 +6250,7 @@
         <v>190</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>292</v>
+        <v>344</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -6159,7 +6258,7 @@
         <v>194</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>293</v>
+        <v>345</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -6167,7 +6266,7 @@
         <v>198</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>294</v>
+        <v>346</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -6175,7 +6274,7 @@
         <v>205</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>314</v>
+        <v>347</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add total cost field to asset management
- Updated asset model to include total cost as a float64 field.
- Modified SQL functions to retrieve total cost for assets by tag and serial number.
- Adjusted asset seeding process to include total cost in the CSV and database.
- Enhanced API service to format and return total cost in the asset response.
- Updated frontend components to display total cost in asset details.
- Removed obsolete asset equipment CSV file and cleaned up asset equipment data.
- Added utility function to format total cost as Indonesian Rupiah.
</commit_message>
<xml_diff>
--- a/backend/internal/seed/seed_data/mst_dummy_data.xlsx
+++ b/backend/internal/seed/seed_data/mst_dummy_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Uni\Intern SM\Stock Opname App [SOSMIT]\SOSMIT\backend\internal\seed\seed_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{579FB297-837E-4FC8-A485-4C4A379805CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{487B53E3-F3D7-4F7F-9752-85D1185E81F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10540" firstSheet="2" activeTab="8" xr2:uid="{AF28B77B-5B1D-47C2-ADE5-ADF50DA09BCF}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10540" firstSheet="2" activeTab="7" xr2:uid="{AF28B77B-5B1D-47C2-ADE5-ADF50DA09BCF}"/>
   </bookViews>
   <sheets>
     <sheet name="Region" sheetId="1" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="739" uniqueCount="348">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="751" uniqueCount="355">
   <si>
     <t>id</t>
   </si>
@@ -865,9 +865,6 @@
     <t>samistheguns@gmail.com</t>
   </si>
   <si>
-    <t>RADITYA</t>
-  </si>
-  <si>
     <t>AREA MANAGER</t>
   </si>
   <si>
@@ -901,9 +898,6 @@
     <t>SMPR00000012</t>
   </si>
   <si>
-    <t>DIPA</t>
-  </si>
-  <si>
     <t>SHEILA</t>
   </si>
   <si>
@@ -1006,15 +1000,9 @@
     <t>Area Manager</t>
   </si>
   <si>
-    <t>VACANT</t>
-  </si>
-  <si>
     <t>IT Services</t>
   </si>
   <si>
-    <t xml:space="preserve">HEAD </t>
-  </si>
-  <si>
     <t>Finance &amp; Accounting Manager</t>
   </si>
   <si>
@@ -1091,6 +1079,39 @@
   </si>
   <si>
     <t>Tas, Tali tas, Adaptor, Kabel USB, Bracket</t>
+  </si>
+  <si>
+    <t>total_cost</t>
+  </si>
+  <si>
+    <t>RIO</t>
+  </si>
+  <si>
+    <t>DEWANTE</t>
+  </si>
+  <si>
+    <t>IT SERVICES MANAGER</t>
+  </si>
+  <si>
+    <t>FINANCE &amp; ACCOUNTING MANAGER</t>
+  </si>
+  <si>
+    <t>VINCENT</t>
+  </si>
+  <si>
+    <t>ROMPI</t>
+  </si>
+  <si>
+    <t>FINANCE OFFICER</t>
+  </si>
+  <si>
+    <t>ANDRE</t>
+  </si>
+  <si>
+    <t>TAHULANY</t>
+  </si>
+  <si>
+    <t>ACCOUNTING OFFICER</t>
   </si>
 </sst>
 </file>
@@ -1143,7 +1164,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -1166,24 +1187,13 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1202,7 +1212,8 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="2" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -2514,10 +2525,10 @@
         <v>80</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -2644,7 +2655,7 @@
       </c>
       <c r="D10" s="1">
         <f ca="1">RANDBETWEEN(1223,1232)</f>
-        <v>1226</v>
+        <v>1225</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -2659,7 +2670,7 @@
       </c>
       <c r="D11" s="1">
         <f t="shared" ref="D11:D51" ca="1" si="0">RANDBETWEEN(1223,1232)</f>
-        <v>1226</v>
+        <v>1223</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -2674,7 +2685,7 @@
       </c>
       <c r="D12" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1226</v>
+        <v>1225</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -2689,7 +2700,7 @@
       </c>
       <c r="D13" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1224</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -2704,7 +2715,7 @@
       </c>
       <c r="D14" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1232</v>
+        <v>1230</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -2719,7 +2730,7 @@
       </c>
       <c r="D15" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1223</v>
+        <v>1226</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -2734,7 +2745,7 @@
       </c>
       <c r="D16" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1230</v>
+        <v>1229</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -2749,7 +2760,7 @@
       </c>
       <c r="D17" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1228</v>
+        <v>1226</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -2764,7 +2775,7 @@
       </c>
       <c r="D18" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1231</v>
+        <v>1223</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -2779,7 +2790,7 @@
       </c>
       <c r="D19" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1232</v>
+        <v>1225</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -2794,7 +2805,7 @@
       </c>
       <c r="D20" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1223</v>
+        <v>1226</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -2824,7 +2835,7 @@
       </c>
       <c r="D22" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1224</v>
+        <v>1225</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -2839,7 +2850,7 @@
       </c>
       <c r="D23" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1227</v>
+        <v>1231</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -2854,7 +2865,7 @@
       </c>
       <c r="D24" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1229</v>
+        <v>1230</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -2884,7 +2895,7 @@
       </c>
       <c r="D26" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1224</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -2899,7 +2910,7 @@
       </c>
       <c r="D27" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1232</v>
+        <v>1225</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -2914,7 +2925,7 @@
       </c>
       <c r="D28" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1231</v>
+        <v>1229</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -2929,7 +2940,7 @@
       </c>
       <c r="D29" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1230</v>
+        <v>1223</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -2944,7 +2955,7 @@
       </c>
       <c r="D30" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1224</v>
+        <v>1225</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -2959,7 +2970,7 @@
       </c>
       <c r="D31" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1231</v>
+        <v>1226</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -2974,7 +2985,7 @@
       </c>
       <c r="D32" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1232</v>
+        <v>1224</v>
       </c>
     </row>
     <row r="33" spans="1:4">
@@ -3004,7 +3015,7 @@
       </c>
       <c r="D34" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1226</v>
+        <v>1229</v>
       </c>
     </row>
     <row r="35" spans="1:4">
@@ -3019,7 +3030,7 @@
       </c>
       <c r="D35" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1225</v>
+        <v>1231</v>
       </c>
     </row>
     <row r="36" spans="1:4">
@@ -3034,7 +3045,7 @@
       </c>
       <c r="D36" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1228</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="37" spans="1:4">
@@ -3049,7 +3060,7 @@
       </c>
       <c r="D37" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1229</v>
+        <v>1231</v>
       </c>
     </row>
     <row r="38" spans="1:4">
@@ -3064,7 +3075,7 @@
       </c>
       <c r="D38" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1225</v>
+        <v>1229</v>
       </c>
     </row>
     <row r="39" spans="1:4">
@@ -3079,7 +3090,7 @@
       </c>
       <c r="D39" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1225</v>
+        <v>1229</v>
       </c>
     </row>
     <row r="40" spans="1:4">
@@ -3094,7 +3105,7 @@
       </c>
       <c r="D40" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1226</v>
+        <v>1230</v>
       </c>
     </row>
     <row r="41" spans="1:4">
@@ -3109,7 +3120,7 @@
       </c>
       <c r="D41" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1223</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="42" spans="1:4">
@@ -3124,7 +3135,7 @@
       </c>
       <c r="D42" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1230</v>
+        <v>1231</v>
       </c>
     </row>
     <row r="43" spans="1:4">
@@ -3139,7 +3150,7 @@
       </c>
       <c r="D43" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1231</v>
+        <v>1232</v>
       </c>
     </row>
     <row r="44" spans="1:4">
@@ -3154,7 +3165,7 @@
       </c>
       <c r="D44" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1231</v>
+        <v>1224</v>
       </c>
     </row>
     <row r="45" spans="1:4">
@@ -3169,7 +3180,7 @@
       </c>
       <c r="D45" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1229</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="46" spans="1:4">
@@ -3199,7 +3210,7 @@
       </c>
       <c r="D47" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1226</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="48" spans="1:4">
@@ -3214,7 +3225,7 @@
       </c>
       <c r="D48" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1232</v>
+        <v>1226</v>
       </c>
     </row>
     <row r="49" spans="1:4">
@@ -3229,7 +3240,7 @@
       </c>
       <c r="D49" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1224</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="50" spans="1:4">
@@ -3259,7 +3270,7 @@
       </c>
       <c r="D51" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1229</v>
+        <v>1228</v>
       </c>
     </row>
   </sheetData>
@@ -3285,7 +3296,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="C1" s="5" t="s">
         <v>132</v>
@@ -3296,7 +3307,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="C2" s="5">
         <v>1</v>
@@ -3307,7 +3318,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="C3" s="5">
         <v>1</v>
@@ -3873,7 +3884,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -3883,68 +3894,68 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="B2" s="1">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="1" t="s">
         <v>315</v>
       </c>
-      <c r="C1" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" t="s">
+      <c r="B3" s="1">
+        <v>2</v>
+      </c>
+      <c r="C3" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="B4" s="1">
+        <v>3</v>
+      </c>
+      <c r="C4" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="1" t="s">
         <v>318</v>
       </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" t="s">
-        <v>317</v>
-      </c>
-      <c r="B3">
+      <c r="B5" s="1">
+        <v>1</v>
+      </c>
+      <c r="C5" s="1">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="B6" s="1">
         <v>2</v>
       </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" t="s">
-        <v>316</v>
-      </c>
-      <c r="B4">
-        <v>3</v>
-      </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" t="s">
-        <v>322</v>
-      </c>
-      <c r="B5">
-        <v>1</v>
-      </c>
-      <c r="C5">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" t="s">
-        <v>316</v>
-      </c>
-      <c r="B6">
-        <v>2</v>
-      </c>
-      <c r="C6">
+      <c r="C6" s="1">
         <v>25</v>
       </c>
     </row>
@@ -3958,7 +3969,7 @@
   <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -3994,10 +4005,10 @@
         <v>226</v>
       </c>
       <c r="G1" s="8" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="H1" s="8" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="I1" s="8" t="s">
         <v>132</v>
@@ -4007,163 +4018,177 @@
       </c>
     </row>
     <row r="2" spans="1:10">
-      <c r="A2" s="8">
-        <v>1</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>319</v>
-      </c>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
+      <c r="A2" s="6">
+        <v>1223</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>271</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>317</v>
+      </c>
       <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
-      <c r="J2" s="8"/>
+      <c r="I2" s="7">
+        <v>25</v>
+      </c>
+      <c r="J2" s="8">
+        <v>110</v>
+      </c>
     </row>
     <row r="3" spans="1:10">
-      <c r="A3" s="6">
-        <v>1223</v>
+      <c r="A3" s="8">
+        <v>1224</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="C3" s="9" t="s">
         <v>271</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="F3" s="8" t="s">
-        <v>137</v>
-      </c>
-      <c r="G3" s="8" t="s">
-        <v>320</v>
-      </c>
-      <c r="H3" s="8"/>
+        <v>141</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3" t="s">
+        <v>311</v>
+      </c>
       <c r="I3" s="7">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="J3" s="8">
-        <v>110</v>
+        <v>410</v>
       </c>
     </row>
     <row r="4" spans="1:10">
-      <c r="A4" s="8">
-        <v>1224</v>
+      <c r="A4" s="6">
+        <v>1225</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="C4" s="9" t="s">
         <v>271</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="G4" s="3"/>
       <c r="H4" s="3" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="I4" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J4" s="8">
-        <v>410</v>
+        <v>230</v>
       </c>
     </row>
     <row r="5" spans="1:10">
-      <c r="A5" s="6">
-        <v>1225</v>
+      <c r="A5" s="8">
+        <v>1226</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="C5" s="9" t="s">
         <v>271</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="G5" s="3"/>
       <c r="H5" s="3" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="I5" s="7">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J5" s="8">
-        <v>240</v>
+        <v>230</v>
       </c>
     </row>
     <row r="6" spans="1:10">
-      <c r="A6" s="8">
-        <v>1226</v>
+      <c r="A6" s="6">
+        <v>1227</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="C6" s="9" t="s">
         <v>271</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>139</v>
       </c>
       <c r="G6" s="3"/>
       <c r="H6" s="3" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="I6" s="7">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J6" s="8">
-        <v>240</v>
+        <v>230</v>
       </c>
     </row>
     <row r="7" spans="1:10">
-      <c r="A7" s="6">
-        <v>1227</v>
+      <c r="A7" s="8">
+        <v>1228</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="C7" s="9" t="s">
         <v>271</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="F7" s="3" t="s">
         <v>139</v>
       </c>
       <c r="G7" s="3"/>
       <c r="H7" s="3" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="I7" s="7">
         <v>1</v>
@@ -4173,27 +4198,27 @@
       </c>
     </row>
     <row r="8" spans="1:10">
-      <c r="A8" s="8">
-        <v>1228</v>
+      <c r="A8" s="6">
+        <v>1229</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="C8" s="9" t="s">
         <v>271</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>139</v>
+        <v>158</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>156</v>
       </c>
       <c r="G8" s="3"/>
       <c r="H8" s="3" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="I8" s="7">
         <v>1</v>
@@ -4203,27 +4228,27 @@
       </c>
     </row>
     <row r="9" spans="1:10">
-      <c r="A9" s="6">
-        <v>1229</v>
+      <c r="A9" s="8">
+        <v>1230</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="C9" s="9" t="s">
         <v>271</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="F9" s="8" t="s">
-        <v>156</v>
+        <v>161</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>143</v>
       </c>
       <c r="G9" s="3"/>
       <c r="H9" s="3" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="I9" s="7">
         <v>1</v>
@@ -4233,27 +4258,27 @@
       </c>
     </row>
     <row r="10" spans="1:10">
-      <c r="A10" s="8">
-        <v>1230</v>
+      <c r="A10" s="6">
+        <v>1231</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="C10" s="9" t="s">
         <v>271</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>161</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>143</v>
+        <v>164</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>156</v>
       </c>
       <c r="G10" s="3"/>
       <c r="H10" s="3" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="I10" s="7">
         <v>1</v>
@@ -4263,226 +4288,253 @@
       </c>
     </row>
     <row r="11" spans="1:10">
-      <c r="A11" s="6">
-        <v>1231</v>
+      <c r="A11" s="8">
+        <v>1232</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="C11" s="9" t="s">
         <v>271</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>164</v>
+        <v>148</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>156</v>
-      </c>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3" t="s">
-        <v>313</v>
-      </c>
-      <c r="I11" s="7">
-        <v>1</v>
+        <v>137</v>
+      </c>
+      <c r="G11" s="8" t="s">
+        <v>317</v>
+      </c>
+      <c r="H11" s="8"/>
+      <c r="I11" s="8">
+        <v>25</v>
       </c>
       <c r="J11" s="8">
-        <v>230</v>
+        <v>110</v>
       </c>
     </row>
     <row r="12" spans="1:10">
       <c r="A12" s="8">
-        <v>1232</v>
+        <v>1233</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="C12" s="9" t="s">
         <v>271</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>148</v>
+        <v>170</v>
       </c>
       <c r="F12" s="8" t="s">
-        <v>137</v>
-      </c>
-      <c r="G12" s="8" t="s">
-        <v>320</v>
-      </c>
-      <c r="H12" s="8"/>
+        <v>168</v>
+      </c>
+      <c r="G12" s="8"/>
+      <c r="H12" s="8" t="s">
+        <v>223</v>
+      </c>
       <c r="I12" s="8">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="J12" s="8">
-        <v>110</v>
+        <v>350</v>
       </c>
     </row>
     <row r="13" spans="1:10">
       <c r="A13" s="8">
-        <v>1233</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>167</v>
+        <v>1234</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>171</v>
       </c>
       <c r="C13" s="9" t="s">
         <v>271</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>168</v>
-      </c>
-      <c r="G13" s="8"/>
-      <c r="H13" s="8" t="s">
-        <v>223</v>
-      </c>
+        <v>172</v>
+      </c>
+      <c r="G13" s="8" t="s">
+        <v>317</v>
+      </c>
+      <c r="H13" s="8"/>
       <c r="I13" s="8">
-        <v>4</v>
+        <v>25</v>
       </c>
       <c r="J13" s="8">
-        <v>350</v>
+        <v>110</v>
       </c>
     </row>
     <row r="14" spans="1:10">
       <c r="A14" s="8">
-        <v>1234</v>
-      </c>
-      <c r="B14" s="8" t="s">
-        <v>171</v>
+        <v>1235</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>285</v>
       </c>
       <c r="C14" s="9" t="s">
         <v>271</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>171</v>
+        <v>285</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>173</v>
+        <v>286</v>
       </c>
       <c r="F14" s="8" t="s">
-        <v>172</v>
-      </c>
-      <c r="G14" s="8" t="s">
-        <v>320</v>
-      </c>
-      <c r="H14" s="8"/>
+        <v>272</v>
+      </c>
+      <c r="G14" s="8"/>
+      <c r="H14" s="8" t="s">
+        <v>312</v>
+      </c>
       <c r="I14" s="8">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="J14" s="8">
-        <v>110</v>
+        <v>230</v>
       </c>
     </row>
     <row r="15" spans="1:10">
       <c r="A15" s="8">
-        <v>1235</v>
+        <v>1236</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>272</v>
+        <v>283</v>
       </c>
       <c r="C15" s="9" t="s">
         <v>271</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>272</v>
+        <v>283</v>
       </c>
       <c r="E15" s="3" t="s">
         <v>284</v>
       </c>
       <c r="F15" s="8" t="s">
-        <v>273</v>
-      </c>
-      <c r="G15" s="8"/>
-      <c r="H15" s="8" t="s">
-        <v>314</v>
-      </c>
+        <v>348</v>
+      </c>
+      <c r="G15" s="8" t="s">
+        <v>222</v>
+      </c>
+      <c r="H15" s="8"/>
       <c r="I15" s="8">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="J15" s="8">
-        <v>230</v>
+        <v>240</v>
       </c>
     </row>
     <row r="16" spans="1:10">
       <c r="A16" s="8">
-        <v>1236</v>
+        <v>1237</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>287</v>
+        <v>345</v>
       </c>
       <c r="C16" s="9" t="s">
         <v>271</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>287</v>
+        <v>345</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>288</v>
+        <v>346</v>
       </c>
       <c r="F16" s="8" t="s">
-        <v>273</v>
-      </c>
-      <c r="G16" s="8"/>
-      <c r="H16" s="8" t="s">
-        <v>314</v>
-      </c>
+        <v>347</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>317</v>
+      </c>
+      <c r="H16" s="1"/>
       <c r="I16" s="8">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="J16" s="8">
-        <v>410</v>
+        <v>110</v>
       </c>
     </row>
     <row r="17" spans="1:10">
       <c r="A17" s="8">
-        <v>1237</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>285</v>
+        <v>1238</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>349</v>
       </c>
       <c r="C17" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="D17" s="3" t="s">
-        <v>285</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="F17" s="8" t="s">
-        <v>321</v>
-      </c>
-      <c r="G17" s="8" t="s">
-        <v>314</v>
-      </c>
-      <c r="H17" s="8"/>
-      <c r="I17" s="8">
+      <c r="D17" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1">
         <v>25</v>
       </c>
-      <c r="J17" s="8">
-        <v>110</v>
+      <c r="J17" s="1">
+        <v>240</v>
       </c>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="10">
-        <v>1238</v>
+      <c r="A18" s="8">
+        <v>1239</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>352</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>271</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>352</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>354</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1">
+        <v>25</v>
+      </c>
+      <c r="J18" s="1">
+        <v>240</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C3" r:id="rId1" xr:uid="{326C7255-3775-42C0-8CED-A0F3BD8EC552}"/>
-    <hyperlink ref="C15" r:id="rId2" xr:uid="{3075A95B-B014-4146-9A02-CE8105DDA61C}"/>
-    <hyperlink ref="C16" r:id="rId3" xr:uid="{AFA86EE8-5F45-4116-A3FB-D1EBD86D2849}"/>
-    <hyperlink ref="C17" r:id="rId4" xr:uid="{4D1991A4-676E-4D81-B282-274D9EC0BE3E}"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{326C7255-3775-42C0-8CED-A0F3BD8EC552}"/>
+    <hyperlink ref="C14" r:id="rId2" xr:uid="{AFA86EE8-5F45-4116-A3FB-D1EBD86D2849}"/>
+    <hyperlink ref="C15" r:id="rId3" xr:uid="{4D1991A4-676E-4D81-B282-274D9EC0BE3E}"/>
+    <hyperlink ref="C16" r:id="rId4" xr:uid="{B250B158-7109-45B2-8042-FFB5BD004E4D}"/>
+    <hyperlink ref="C18" r:id="rId5" xr:uid="{1CEC1CF0-724D-466E-A15B-83EAF93FDCD2}"/>
+    <hyperlink ref="C17" r:id="rId6" xr:uid="{840A625E-CCBB-45E7-916E-F857D68B824B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4557,10 +4609,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{491D14EC-1CB1-4681-930A-4B9B4015FC83}">
-  <dimension ref="A1:P35"/>
+  <dimension ref="A1:Q35"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Q12" sqref="Q12"/>
+    <sheetView tabSelected="1" topLeftCell="I11" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="P18" sqref="P18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -4579,11 +4631,12 @@
     <col min="12" max="12" width="14.54296875" customWidth="1"/>
     <col min="13" max="13" width="20.6328125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="56.453125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.7265625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="10" customWidth="1"/>
+    <col min="15" max="15" width="18.08984375" style="11" customWidth="1"/>
+    <col min="16" max="16" width="9.7265625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:17">
       <c r="A1" s="1" t="s">
         <v>210</v>
       </c>
@@ -4624,16 +4677,19 @@
         <v>246</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>289</v>
-      </c>
-      <c r="O1" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="O1" s="10" t="s">
+        <v>344</v>
+      </c>
+      <c r="P1" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="P1" s="1" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16">
+      <c r="Q1" s="1" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17">
       <c r="A2" s="1" t="s">
         <v>174</v>
       </c>
@@ -4670,16 +4726,19 @@
         <v>248</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>323</v>
-      </c>
-      <c r="O2" s="2">
+        <v>319</v>
+      </c>
+      <c r="O2" s="10">
+        <v>7000000</v>
+      </c>
+      <c r="P2" s="2">
         <v>1223</v>
       </c>
-      <c r="P2" s="1">
+      <c r="Q2" s="1">
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:16">
+    <row r="3" spans="1:17">
       <c r="A3" s="1" t="s">
         <v>181</v>
       </c>
@@ -4716,16 +4775,19 @@
         <v>248</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>324</v>
-      </c>
-      <c r="O3" s="1">
-        <v>1224</v>
+        <v>320</v>
+      </c>
+      <c r="O3" s="10">
+        <v>16000000</v>
       </c>
       <c r="P3" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16">
+        <v>1228</v>
+      </c>
+      <c r="Q3" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17">
       <c r="A4" s="1" t="s">
         <v>184</v>
       </c>
@@ -4762,16 +4824,19 @@
         <v>248</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>324</v>
-      </c>
-      <c r="O4" s="2">
+        <v>320</v>
+      </c>
+      <c r="O4" s="10">
+        <v>14500000</v>
+      </c>
+      <c r="P4" s="2">
         <v>1225</v>
       </c>
-      <c r="P4" s="1">
+      <c r="Q4" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:16">
+    <row r="5" spans="1:17">
       <c r="A5" s="1" t="s">
         <v>249</v>
       </c>
@@ -4808,16 +4873,19 @@
         <v>248</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>324</v>
-      </c>
-      <c r="O5" s="1">
+        <v>320</v>
+      </c>
+      <c r="O5" s="10">
+        <v>14500000</v>
+      </c>
+      <c r="P5" s="1">
         <v>1225</v>
       </c>
-      <c r="P5" s="1">
+      <c r="Q5" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:16">
+    <row r="6" spans="1:17">
       <c r="A6" s="1" t="s">
         <v>263</v>
       </c>
@@ -4854,16 +4922,19 @@
         <v>248</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>324</v>
-      </c>
-      <c r="O6" s="1">
-        <v>1227</v>
+        <v>320</v>
+      </c>
+      <c r="O6" s="10">
+        <v>14500000</v>
       </c>
       <c r="P6" s="1">
+        <v>1228</v>
+      </c>
+      <c r="Q6" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:16">
+    <row r="7" spans="1:17">
       <c r="A7" s="1" t="s">
         <v>187</v>
       </c>
@@ -4900,16 +4971,19 @@
         <v>248</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>324</v>
-      </c>
-      <c r="O7" s="1">
+        <v>320</v>
+      </c>
+      <c r="O7" s="10">
+        <v>14500000</v>
+      </c>
+      <c r="P7" s="1">
         <v>1226</v>
       </c>
-      <c r="P7" s="1">
+      <c r="Q7" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:16">
+    <row r="8" spans="1:17">
       <c r="A8" s="1" t="s">
         <v>188</v>
       </c>
@@ -4946,16 +5020,19 @@
         <v>248</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>325</v>
-      </c>
-      <c r="O8" s="2">
-        <v>1223</v>
-      </c>
-      <c r="P8" s="1">
+        <v>321</v>
+      </c>
+      <c r="O8" s="10">
+        <v>3000000</v>
+      </c>
+      <c r="P8" s="2">
+        <v>1232</v>
+      </c>
+      <c r="Q8" s="1">
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:16">
+    <row r="9" spans="1:17">
       <c r="A9" s="1" t="s">
         <v>192</v>
       </c>
@@ -4992,16 +5069,19 @@
         <v>248</v>
       </c>
       <c r="N9" s="1" t="s">
-        <v>325</v>
-      </c>
-      <c r="O9" s="1">
-        <v>1223</v>
+        <v>321</v>
+      </c>
+      <c r="O9" s="10">
+        <v>5500000</v>
       </c>
       <c r="P9" s="1">
+        <v>1238</v>
+      </c>
+      <c r="Q9" s="1">
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:16">
+    <row r="10" spans="1:17">
       <c r="A10" s="1" t="s">
         <v>257</v>
       </c>
@@ -5038,16 +5118,19 @@
         <v>248</v>
       </c>
       <c r="N10" s="1" t="s">
-        <v>326</v>
-      </c>
-      <c r="O10" s="2">
-        <v>1226</v>
-      </c>
-      <c r="P10" s="1">
+        <v>322</v>
+      </c>
+      <c r="O10" s="10">
+        <v>3000000</v>
+      </c>
+      <c r="P10" s="2">
+        <v>1239</v>
+      </c>
+      <c r="Q10" s="1">
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:16">
+    <row r="11" spans="1:17">
       <c r="A11" s="1" t="s">
         <v>258</v>
       </c>
@@ -5084,16 +5167,19 @@
         <v>248</v>
       </c>
       <c r="N11" s="1" t="s">
-        <v>325</v>
-      </c>
-      <c r="O11" s="1">
-        <v>1226</v>
+        <v>321</v>
+      </c>
+      <c r="O11" s="10">
+        <v>5500000</v>
       </c>
       <c r="P11" s="1">
+        <v>1223</v>
+      </c>
+      <c r="Q11" s="1">
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:16">
+    <row r="12" spans="1:17">
       <c r="A12" s="1" t="s">
         <v>259</v>
       </c>
@@ -5130,16 +5216,19 @@
         <v>248</v>
       </c>
       <c r="N12" s="1" t="s">
-        <v>327</v>
-      </c>
-      <c r="O12" s="2">
-        <v>1226</v>
-      </c>
-      <c r="P12" s="1">
+        <v>323</v>
+      </c>
+      <c r="O12" s="10">
+        <v>7000000</v>
+      </c>
+      <c r="P12" s="2">
+        <v>1232</v>
+      </c>
+      <c r="Q12" s="1">
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:16">
+    <row r="13" spans="1:17">
       <c r="A13" s="1" t="s">
         <v>197</v>
       </c>
@@ -5176,16 +5265,19 @@
         <v>248</v>
       </c>
       <c r="N13" s="1" t="s">
-        <v>328</v>
-      </c>
-      <c r="O13" s="2">
-        <v>1229</v>
-      </c>
-      <c r="P13" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16">
+        <v>324</v>
+      </c>
+      <c r="O13" s="10">
+        <v>6700000</v>
+      </c>
+      <c r="P13" s="2">
+        <v>1231</v>
+      </c>
+      <c r="Q13" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17">
       <c r="A14" s="1" t="s">
         <v>201</v>
       </c>
@@ -5222,16 +5314,19 @@
         <v>248</v>
       </c>
       <c r="N14" s="1" t="s">
-        <v>329</v>
-      </c>
-      <c r="O14" s="1">
-        <v>1230</v>
+        <v>325</v>
+      </c>
+      <c r="O14" s="10">
+        <v>6700000</v>
       </c>
       <c r="P14" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16">
+        <v>1228</v>
+      </c>
+      <c r="Q14" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17">
       <c r="A15" s="1" t="s">
         <v>202</v>
       </c>
@@ -5268,16 +5363,19 @@
         <v>248</v>
       </c>
       <c r="N15" s="1" t="s">
-        <v>330</v>
-      </c>
-      <c r="O15" s="2">
-        <v>1231</v>
-      </c>
-      <c r="P15" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16">
+        <v>326</v>
+      </c>
+      <c r="O15" s="10">
+        <v>4350000</v>
+      </c>
+      <c r="P15" s="2">
+        <v>1226</v>
+      </c>
+      <c r="Q15" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17">
       <c r="A16" s="1" t="s">
         <v>204</v>
       </c>
@@ -5314,16 +5412,19 @@
         <v>248</v>
       </c>
       <c r="N16" s="1" t="s">
-        <v>331</v>
-      </c>
-      <c r="O16" s="1">
-        <v>1231</v>
+        <v>327</v>
+      </c>
+      <c r="O16" s="10">
+        <v>6600000</v>
       </c>
       <c r="P16" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:16">
+        <v>1228</v>
+      </c>
+      <c r="Q16" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17">
       <c r="A17" s="1" t="s">
         <v>207</v>
       </c>
@@ -5360,16 +5461,19 @@
         <v>248</v>
       </c>
       <c r="N17" s="1" t="s">
-        <v>332</v>
-      </c>
-      <c r="O17" s="2">
-        <v>1224</v>
-      </c>
-      <c r="P17" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:16">
+        <v>328</v>
+      </c>
+      <c r="O17" s="10">
+        <v>6600000</v>
+      </c>
+      <c r="P17" s="2">
+        <v>1231</v>
+      </c>
+      <c r="Q17" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17">
       <c r="A18" s="1" t="s">
         <v>208</v>
       </c>
@@ -5408,16 +5512,19 @@
         <v>248</v>
       </c>
       <c r="N18" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="O18" s="1">
-        <v>1225</v>
+        <v>329</v>
+      </c>
+      <c r="O18" s="10">
+        <v>7400000</v>
       </c>
       <c r="P18" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:16">
+      <c r="Q18" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17">
       <c r="A19" s="1" t="s">
         <v>252</v>
       </c>
@@ -5456,16 +5563,19 @@
         <v>248</v>
       </c>
       <c r="N19" s="1" t="s">
-        <v>334</v>
-      </c>
-      <c r="O19" s="1">
-        <v>1226</v>
+        <v>330</v>
+      </c>
+      <c r="O19" s="10">
+        <v>7400000</v>
       </c>
       <c r="P19" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:16">
+      <c r="Q19" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17">
       <c r="A20" s="1" t="s">
         <v>253</v>
       </c>
@@ -5502,16 +5612,19 @@
         <v>248</v>
       </c>
       <c r="N20" s="1" t="s">
-        <v>335</v>
-      </c>
-      <c r="O20" s="1">
-        <v>1223</v>
+        <v>331</v>
+      </c>
+      <c r="O20" s="10">
+        <v>7400000</v>
       </c>
       <c r="P20" s="1">
+        <v>1230</v>
+      </c>
+      <c r="Q20" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:16">
+    <row r="21" spans="1:17">
       <c r="A21" s="1" t="s">
         <v>254</v>
       </c>
@@ -5548,16 +5661,19 @@
         <v>248</v>
       </c>
       <c r="N21" s="1" t="s">
-        <v>336</v>
-      </c>
-      <c r="O21" s="1">
-        <v>1229</v>
+        <v>332</v>
+      </c>
+      <c r="O21" s="10">
+        <v>7400000</v>
       </c>
       <c r="P21" s="1">
+        <v>1227</v>
+      </c>
+      <c r="Q21" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:16">
+    <row r="22" spans="1:17">
       <c r="A22" s="1" t="s">
         <v>255</v>
       </c>
@@ -5594,16 +5710,19 @@
         <v>248</v>
       </c>
       <c r="N22" s="1" t="s">
-        <v>337</v>
-      </c>
-      <c r="O22" s="1">
-        <v>1228</v>
+        <v>333</v>
+      </c>
+      <c r="O22" s="10">
+        <v>7400000</v>
       </c>
       <c r="P22" s="1">
+        <v>1227</v>
+      </c>
+      <c r="Q22" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:16">
+    <row r="23" spans="1:17">
       <c r="A23" s="1" t="s">
         <v>256</v>
       </c>
@@ -5640,24 +5759,27 @@
         <v>248</v>
       </c>
       <c r="N23" s="1" t="s">
-        <v>338</v>
-      </c>
-      <c r="O23" s="1">
-        <v>1227</v>
+        <v>334</v>
+      </c>
+      <c r="O23" s="10">
+        <v>7400000</v>
       </c>
       <c r="P23" s="1">
+        <v>1224</v>
+      </c>
+      <c r="Q23" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:16">
+    <row r="24" spans="1:17">
       <c r="A24" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D24" s="1"/>
       <c r="E24" s="1" t="s">
@@ -5686,24 +5808,27 @@
         <v>248</v>
       </c>
       <c r="N24" s="1" t="s">
-        <v>339</v>
-      </c>
-      <c r="O24" s="1">
-        <v>1227</v>
+        <v>335</v>
+      </c>
+      <c r="O24" s="10">
+        <v>7400000</v>
       </c>
       <c r="P24" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:16">
+        <v>1</v>
+      </c>
+      <c r="Q24" s="1">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17">
       <c r="A25" s="1" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D25" s="1"/>
       <c r="E25" s="1" t="s">
@@ -5732,24 +5857,27 @@
         <v>248</v>
       </c>
       <c r="N25" s="1" t="s">
-        <v>340</v>
-      </c>
-      <c r="O25" s="1">
-        <v>1227</v>
+        <v>336</v>
+      </c>
+      <c r="O25" s="10">
+        <v>7400000</v>
       </c>
       <c r="P25" s="1">
+        <v>1238</v>
+      </c>
+      <c r="Q25" s="1">
         <v>27</v>
       </c>
     </row>
-    <row r="26" spans="1:16">
+    <row r="26" spans="1:17">
       <c r="A26" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D26" s="1"/>
       <c r="E26" s="1" t="s">
@@ -5778,24 +5906,27 @@
         <v>248</v>
       </c>
       <c r="N26" s="1" t="s">
-        <v>341</v>
-      </c>
-      <c r="O26" s="1">
-        <v>1227</v>
+        <v>337</v>
+      </c>
+      <c r="O26" s="10">
+        <v>7400000</v>
       </c>
       <c r="P26" s="1">
+        <v>1236</v>
+      </c>
+      <c r="Q26" s="1">
         <v>27</v>
       </c>
     </row>
-    <row r="27" spans="1:16">
+    <row r="27" spans="1:17">
       <c r="A27" s="1" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B27" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="C27" s="1" t="s">
         <v>277</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>278</v>
       </c>
       <c r="D27" s="1"/>
       <c r="E27" s="1" t="s">
@@ -5824,21 +5955,24 @@
         <v>248</v>
       </c>
       <c r="N27" s="1" t="s">
-        <v>342</v>
-      </c>
-      <c r="O27" s="1">
-        <v>1227</v>
+        <v>338</v>
+      </c>
+      <c r="O27" s="10">
+        <v>7400000</v>
       </c>
       <c r="P27" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q27" s="1">
         <v>27</v>
       </c>
     </row>
-    <row r="28" spans="1:16">
+    <row r="28" spans="1:17">
       <c r="A28" s="1" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>175</v>
@@ -5870,21 +6004,24 @@
         <v>248</v>
       </c>
       <c r="N28" s="1" t="s">
-        <v>326</v>
-      </c>
-      <c r="O28" s="2">
-        <v>1226</v>
-      </c>
-      <c r="P28" s="1">
+        <v>322</v>
+      </c>
+      <c r="O28" s="10">
+        <v>3000000</v>
+      </c>
+      <c r="P28" s="2">
+        <v>1225</v>
+      </c>
+      <c r="Q28" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:16">
+    <row r="29" spans="1:17">
       <c r="A29" s="1" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>175</v>
@@ -5916,21 +6053,24 @@
         <v>248</v>
       </c>
       <c r="N29" s="1" t="s">
-        <v>325</v>
-      </c>
-      <c r="O29" s="1">
+        <v>321</v>
+      </c>
+      <c r="O29" s="10">
+        <v>5500000</v>
+      </c>
+      <c r="P29" s="1">
         <v>1226</v>
       </c>
-      <c r="P29" s="1">
+      <c r="Q29" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="30" spans="1:16">
+    <row r="30" spans="1:17">
       <c r="A30" s="1" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>175</v>
@@ -5962,21 +6102,24 @@
         <v>248</v>
       </c>
       <c r="N30" s="1" t="s">
-        <v>327</v>
-      </c>
-      <c r="O30" s="2">
-        <v>1226</v>
-      </c>
-      <c r="P30" s="1">
+        <v>323</v>
+      </c>
+      <c r="O30" s="10">
+        <v>7000000</v>
+      </c>
+      <c r="P30" s="2">
+        <v>1227</v>
+      </c>
+      <c r="Q30" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:16">
+    <row r="31" spans="1:17">
       <c r="A31" s="1" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>175</v>
@@ -6008,24 +6151,27 @@
         <v>248</v>
       </c>
       <c r="N31" s="1" t="s">
-        <v>328</v>
-      </c>
-      <c r="O31" s="2">
-        <v>1</v>
-      </c>
-      <c r="P31" s="1">
+        <v>324</v>
+      </c>
+      <c r="O31" s="10">
+        <v>6700000</v>
+      </c>
+      <c r="P31" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q31" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="32" spans="1:16">
+    <row r="32" spans="1:17">
       <c r="A32" s="1" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D32" s="1"/>
       <c r="E32" s="1" t="s">
@@ -6054,24 +6200,27 @@
         <v>248</v>
       </c>
       <c r="N32" s="1" t="s">
-        <v>329</v>
-      </c>
-      <c r="O32" s="1">
-        <v>1</v>
+        <v>325</v>
+      </c>
+      <c r="O32" s="10">
+        <v>6700000</v>
       </c>
       <c r="P32" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q32" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="1:16">
+    <row r="33" spans="1:17">
       <c r="A33" s="1" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D33" s="1"/>
       <c r="E33" s="1" t="s">
@@ -6100,21 +6249,24 @@
         <v>248</v>
       </c>
       <c r="N33" s="1" t="s">
-        <v>330</v>
-      </c>
-      <c r="O33" s="2">
-        <v>1</v>
-      </c>
-      <c r="P33" s="1">
+        <v>326</v>
+      </c>
+      <c r="O33" s="10">
+        <v>4350000</v>
+      </c>
+      <c r="P33" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q33" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="34" spans="1:16">
+    <row r="34" spans="1:17">
       <c r="A34" s="1" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>175</v>
@@ -6146,21 +6298,24 @@
         <v>248</v>
       </c>
       <c r="N34" s="1" t="s">
-        <v>331</v>
-      </c>
-      <c r="O34" s="1">
-        <v>1</v>
+        <v>327</v>
+      </c>
+      <c r="O34" s="10">
+        <v>6600000</v>
       </c>
       <c r="P34" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q34" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="35" spans="1:16">
+    <row r="35" spans="1:17">
       <c r="A35" s="1" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>175</v>
@@ -6192,12 +6347,15 @@
         <v>248</v>
       </c>
       <c r="N35" s="1" t="s">
-        <v>332</v>
-      </c>
-      <c r="O35" s="2">
-        <v>1</v>
-      </c>
-      <c r="P35" s="1">
+        <v>328</v>
+      </c>
+      <c r="O35" s="10">
+        <v>6600000</v>
+      </c>
+      <c r="P35" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q35" s="1">
         <v>3</v>
       </c>
     </row>
@@ -6211,7 +6369,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28F0C749-0F7B-4353-B0A5-2957163B7B34}">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
@@ -6226,7 +6384,7 @@
         <v>213</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -6234,7 +6392,7 @@
         <v>178</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -6242,7 +6400,7 @@
         <v>182</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -6250,7 +6408,7 @@
         <v>190</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -6258,7 +6416,7 @@
         <v>194</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -6266,7 +6424,7 @@
         <v>198</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -6274,7 +6432,7 @@
         <v>205</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: add Department table and update related seed data; enhance User and Asset tables with new fields
</commit_message>
<xml_diff>
--- a/backend/internal/seed/seed_data/mst_dummy_data.xlsx
+++ b/backend/internal/seed/seed_data/mst_dummy_data.xlsx
@@ -8,23 +8,25 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Uni\Intern SM\Stock Opname App [SOSMIT]\SOSMIT\backend\internal\seed\seed_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{487B53E3-F3D7-4F7F-9752-85D1185E81F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D6B55BB-C0C9-4A87-8800-3339D8C49859}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10540" firstSheet="2" activeTab="7" xr2:uid="{AF28B77B-5B1D-47C2-ADE5-ADF50DA09BCF}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10540" firstSheet="4" activeTab="8" xr2:uid="{AF28B77B-5B1D-47C2-ADE5-ADF50DA09BCF}"/>
   </bookViews>
   <sheets>
     <sheet name="Region" sheetId="1" r:id="rId1"/>
     <sheet name="Site Group" sheetId="2" r:id="rId2"/>
     <sheet name="Site" sheetId="3" r:id="rId3"/>
     <sheet name="SubSite" sheetId="8" r:id="rId4"/>
-    <sheet name="ApprovalPath" sheetId="9" r:id="rId5"/>
-    <sheet name="User" sheetId="4" r:id="rId6"/>
-    <sheet name="Cost Center" sheetId="6" r:id="rId7"/>
-    <sheet name="Asset" sheetId="5" r:id="rId8"/>
-    <sheet name="Asset Equipment" sheetId="7" r:id="rId9"/>
+    <sheet name="Department" sheetId="10" r:id="rId5"/>
+    <sheet name="ApprovalPath" sheetId="9" r:id="rId6"/>
+    <sheet name="User" sheetId="4" r:id="rId7"/>
+    <sheet name="Cost Center" sheetId="6" r:id="rId8"/>
+    <sheet name="Asset" sheetId="5" r:id="rId9"/>
+    <sheet name="Asset Equipment" sheetId="7" r:id="rId10"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">'Asset Equipment'!$A$1:$A$7</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">'Asset Equipment'!$A$1:$A$7</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Department!$B$1:$B$17</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -47,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="751" uniqueCount="355">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="735" uniqueCount="364">
   <si>
     <t>id</t>
   </si>
@@ -1112,6 +1114,33 @@
   </si>
   <si>
     <t>ACCOUNTING OFFICER</t>
+  </si>
+  <si>
+    <t>from</t>
+  </si>
+  <si>
+    <t>ou_code</t>
+  </si>
+  <si>
+    <t>HO</t>
+  </si>
+  <si>
+    <t>BL1</t>
+  </si>
+  <si>
+    <t>BL2</t>
+  </si>
+  <si>
+    <t>BL3</t>
+  </si>
+  <si>
+    <t>dept_id</t>
+  </si>
+  <si>
+    <t>dept_name</t>
+  </si>
+  <si>
+    <t>Area</t>
   </si>
 </sst>
 </file>
@@ -1193,7 +1222,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1214,6 +1243,13 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="2" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -2198,6 +2234,82 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28F0C749-0F7B-4353-B0A5-2957163B7B34}">
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="1" max="1" width="23.36328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.08984375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>343</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:A7" xr:uid="{28F0C749-0F7B-4353-B0A5-2957163B7B34}"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F51990CE-FF2C-48E9-82E1-2E87B3A6C16A}">
   <dimension ref="A1:C26"/>
@@ -2506,8 +2618,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E6AD482-693C-4526-A8EF-051504D339CF}">
   <dimension ref="A1:D51"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -2655,7 +2767,7 @@
       </c>
       <c r="D10" s="1">
         <f ca="1">RANDBETWEEN(1223,1232)</f>
-        <v>1225</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -2670,7 +2782,7 @@
       </c>
       <c r="D11" s="1">
         <f t="shared" ref="D11:D51" ca="1" si="0">RANDBETWEEN(1223,1232)</f>
-        <v>1223</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -2685,7 +2797,7 @@
       </c>
       <c r="D12" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1225</v>
+        <v>1224</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -2715,7 +2827,7 @@
       </c>
       <c r="D14" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1230</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -2730,7 +2842,7 @@
       </c>
       <c r="D15" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1226</v>
+        <v>1223</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -2745,7 +2857,7 @@
       </c>
       <c r="D16" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1229</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -2760,7 +2872,7 @@
       </c>
       <c r="D17" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1226</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -2775,7 +2887,7 @@
       </c>
       <c r="D18" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1223</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -2790,7 +2902,7 @@
       </c>
       <c r="D19" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1225</v>
+        <v>1230</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -2805,7 +2917,7 @@
       </c>
       <c r="D20" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1226</v>
+        <v>1230</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -2820,7 +2932,7 @@
       </c>
       <c r="D21" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1230</v>
+        <v>1225</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -2835,7 +2947,7 @@
       </c>
       <c r="D22" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1225</v>
+        <v>1226</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -2850,7 +2962,7 @@
       </c>
       <c r="D23" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1231</v>
+        <v>1225</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -2865,7 +2977,7 @@
       </c>
       <c r="D24" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1230</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -2880,7 +2992,7 @@
       </c>
       <c r="D25" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1230</v>
+        <v>1224</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -2895,7 +3007,7 @@
       </c>
       <c r="D26" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1228</v>
+        <v>1232</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -2910,7 +3022,7 @@
       </c>
       <c r="D27" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1225</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -2925,7 +3037,7 @@
       </c>
       <c r="D28" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1229</v>
+        <v>1225</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -2940,7 +3052,7 @@
       </c>
       <c r="D29" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1223</v>
+        <v>1225</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -2955,7 +3067,7 @@
       </c>
       <c r="D30" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1225</v>
+        <v>1229</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -2970,7 +3082,7 @@
       </c>
       <c r="D31" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1226</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -3000,7 +3112,7 @@
       </c>
       <c r="D33" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1225</v>
+        <v>1230</v>
       </c>
     </row>
     <row r="34" spans="1:4">
@@ -3015,7 +3127,7 @@
       </c>
       <c r="D34" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1229</v>
+        <v>1224</v>
       </c>
     </row>
     <row r="35" spans="1:4">
@@ -3030,7 +3142,7 @@
       </c>
       <c r="D35" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1231</v>
+        <v>1225</v>
       </c>
     </row>
     <row r="36" spans="1:4">
@@ -3045,7 +3157,7 @@
       </c>
       <c r="D36" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1227</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="37" spans="1:4">
@@ -3060,7 +3172,7 @@
       </c>
       <c r="D37" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1231</v>
+        <v>1230</v>
       </c>
     </row>
     <row r="38" spans="1:4">
@@ -3075,7 +3187,7 @@
       </c>
       <c r="D38" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1229</v>
+        <v>1223</v>
       </c>
     </row>
     <row r="39" spans="1:4">
@@ -3090,7 +3202,7 @@
       </c>
       <c r="D39" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1229</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="40" spans="1:4">
@@ -3105,7 +3217,7 @@
       </c>
       <c r="D40" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1230</v>
+        <v>1223</v>
       </c>
     </row>
     <row r="41" spans="1:4">
@@ -3120,7 +3232,7 @@
       </c>
       <c r="D41" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1228</v>
+        <v>1224</v>
       </c>
     </row>
     <row r="42" spans="1:4">
@@ -3135,7 +3247,7 @@
       </c>
       <c r="D42" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1231</v>
+        <v>1224</v>
       </c>
     </row>
     <row r="43" spans="1:4">
@@ -3150,7 +3262,7 @@
       </c>
       <c r="D43" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1232</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="44" spans="1:4">
@@ -3165,7 +3277,7 @@
       </c>
       <c r="D44" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1224</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="45" spans="1:4">
@@ -3195,7 +3307,7 @@
       </c>
       <c r="D46" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1231</v>
+        <v>1229</v>
       </c>
     </row>
     <row r="47" spans="1:4">
@@ -3210,7 +3322,7 @@
       </c>
       <c r="D47" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1227</v>
+        <v>1226</v>
       </c>
     </row>
     <row r="48" spans="1:4">
@@ -3225,7 +3337,7 @@
       </c>
       <c r="D48" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1226</v>
+        <v>1224</v>
       </c>
     </row>
     <row r="49" spans="1:4">
@@ -3240,7 +3352,7 @@
       </c>
       <c r="D49" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1227</v>
+        <v>1232</v>
       </c>
     </row>
     <row r="50" spans="1:4">
@@ -3255,7 +3367,7 @@
       </c>
       <c r="D50" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1230</v>
+        <v>1224</v>
       </c>
     </row>
     <row r="51" spans="1:4">
@@ -3270,7 +3382,7 @@
       </c>
       <c r="D51" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1228</v>
+        <v>1224</v>
       </c>
     </row>
   </sheetData>
@@ -3283,7 +3395,7 @@
   <dimension ref="A1:C53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -3325,554 +3437,254 @@
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="1">
-        <v>3</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="C4" s="4">
-        <v>1</v>
-      </c>
+      <c r="A4" s="14"/>
+      <c r="B4" s="15"/>
+      <c r="C4" s="16"/>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" s="1">
-        <v>4</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="C5" s="4">
-        <v>2</v>
-      </c>
+      <c r="A5" s="14"/>
+      <c r="B5" s="15"/>
+      <c r="C5" s="16"/>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6" s="1">
-        <v>5</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="C6" s="4">
-        <v>3</v>
-      </c>
+      <c r="A6" s="14"/>
+      <c r="B6" s="15"/>
+      <c r="C6" s="16"/>
     </row>
     <row r="7" spans="1:3">
-      <c r="A7" s="1">
-        <v>6</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="C7" s="4">
-        <v>4</v>
-      </c>
+      <c r="A7" s="14"/>
+      <c r="B7" s="15"/>
+      <c r="C7" s="16"/>
     </row>
     <row r="8" spans="1:3">
-      <c r="A8" s="1">
-        <v>7</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="C8" s="4">
-        <v>5</v>
-      </c>
+      <c r="A8" s="14"/>
+      <c r="B8" s="15"/>
+      <c r="C8" s="16"/>
     </row>
     <row r="9" spans="1:3">
-      <c r="A9" s="1">
-        <v>8</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="C9" s="4">
-        <v>6</v>
-      </c>
+      <c r="A9" s="14"/>
+      <c r="B9" s="15"/>
+      <c r="C9" s="16"/>
     </row>
     <row r="10" spans="1:3">
-      <c r="A10" s="1">
-        <v>9</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="C10" s="4">
-        <v>7</v>
-      </c>
+      <c r="A10" s="14"/>
+      <c r="B10" s="15"/>
+      <c r="C10" s="16"/>
     </row>
     <row r="11" spans="1:3">
-      <c r="A11" s="1">
-        <v>10</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="C11" s="4">
-        <v>8</v>
-      </c>
+      <c r="A11" s="14"/>
+      <c r="B11" s="15"/>
+      <c r="C11" s="16"/>
     </row>
     <row r="12" spans="1:3">
-      <c r="A12" s="1">
-        <v>11</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="C12" s="4">
-        <v>9</v>
-      </c>
+      <c r="A12" s="14"/>
+      <c r="B12" s="15"/>
+      <c r="C12" s="16"/>
     </row>
     <row r="13" spans="1:3">
-      <c r="A13" s="1">
-        <v>12</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="C13" s="4">
-        <v>10</v>
-      </c>
+      <c r="A13" s="14"/>
+      <c r="B13" s="15"/>
+      <c r="C13" s="16"/>
     </row>
     <row r="14" spans="1:3">
-      <c r="A14" s="1">
-        <v>13</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="C14" s="4">
-        <v>11</v>
-      </c>
+      <c r="A14" s="14"/>
+      <c r="B14" s="15"/>
+      <c r="C14" s="16"/>
     </row>
     <row r="15" spans="1:3">
-      <c r="A15" s="1">
-        <v>14</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="C15" s="4">
-        <v>12</v>
-      </c>
+      <c r="A15" s="14"/>
+      <c r="B15" s="15"/>
+      <c r="C15" s="16"/>
     </row>
     <row r="16" spans="1:3">
-      <c r="A16" s="1">
-        <v>15</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="C16" s="4">
-        <v>13</v>
-      </c>
+      <c r="A16" s="14"/>
+      <c r="B16" s="15"/>
+      <c r="C16" s="16"/>
     </row>
     <row r="17" spans="1:3">
-      <c r="A17" s="1">
-        <v>16</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="C17" s="4">
-        <v>14</v>
-      </c>
+      <c r="A17" s="14"/>
+      <c r="B17" s="15"/>
+      <c r="C17" s="16"/>
     </row>
     <row r="18" spans="1:3">
-      <c r="A18" s="1">
-        <v>17</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="C18" s="4">
-        <v>15</v>
-      </c>
+      <c r="A18" s="14"/>
+      <c r="B18" s="15"/>
+      <c r="C18" s="16"/>
     </row>
     <row r="19" spans="1:3">
-      <c r="A19" s="1">
-        <v>18</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="C19" s="4">
-        <v>16</v>
-      </c>
+      <c r="A19" s="14"/>
+      <c r="B19" s="15"/>
+      <c r="C19" s="16"/>
     </row>
     <row r="20" spans="1:3">
-      <c r="A20" s="1">
-        <v>19</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="C20" s="4">
-        <v>17</v>
-      </c>
+      <c r="A20" s="14"/>
+      <c r="B20" s="15"/>
+      <c r="C20" s="16"/>
     </row>
     <row r="21" spans="1:3">
-      <c r="A21" s="1">
-        <v>20</v>
-      </c>
-      <c r="B21" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="C21" s="4">
-        <v>18</v>
-      </c>
+      <c r="A21" s="14"/>
+      <c r="B21" s="15"/>
+      <c r="C21" s="16"/>
     </row>
     <row r="22" spans="1:3">
-      <c r="A22" s="1">
-        <v>21</v>
-      </c>
-      <c r="B22" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="C22" s="4">
-        <v>19</v>
-      </c>
+      <c r="A22" s="14"/>
+      <c r="B22" s="15"/>
+      <c r="C22" s="16"/>
     </row>
     <row r="23" spans="1:3">
-      <c r="A23" s="1">
-        <v>22</v>
-      </c>
-      <c r="B23" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="C23" s="4">
-        <v>20</v>
-      </c>
+      <c r="A23" s="14"/>
+      <c r="B23" s="15"/>
+      <c r="C23" s="16"/>
     </row>
     <row r="24" spans="1:3">
-      <c r="A24" s="1">
-        <v>23</v>
-      </c>
-      <c r="B24" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="C24" s="4">
-        <v>21</v>
-      </c>
+      <c r="A24" s="14"/>
+      <c r="B24" s="15"/>
+      <c r="C24" s="16"/>
     </row>
     <row r="25" spans="1:3">
-      <c r="A25" s="1">
-        <v>24</v>
-      </c>
-      <c r="B25" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="C25" s="4">
-        <v>22</v>
-      </c>
+      <c r="A25" s="14"/>
+      <c r="B25" s="15"/>
+      <c r="C25" s="16"/>
     </row>
     <row r="26" spans="1:3">
-      <c r="A26" s="1">
-        <v>25</v>
-      </c>
-      <c r="B26" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="C26" s="4">
-        <v>23</v>
-      </c>
+      <c r="A26" s="14"/>
+      <c r="B26" s="15"/>
+      <c r="C26" s="16"/>
     </row>
     <row r="27" spans="1:3">
-      <c r="A27" s="1">
-        <v>26</v>
-      </c>
-      <c r="B27" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="C27" s="4">
-        <v>24</v>
-      </c>
+      <c r="A27" s="14"/>
+      <c r="B27" s="15"/>
+      <c r="C27" s="16"/>
     </row>
     <row r="28" spans="1:3">
-      <c r="A28" s="1">
-        <v>27</v>
-      </c>
-      <c r="B28" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="C28" s="4">
-        <v>25</v>
-      </c>
+      <c r="A28" s="14"/>
+      <c r="B28" s="15"/>
+      <c r="C28" s="16"/>
     </row>
     <row r="29" spans="1:3">
-      <c r="A29" s="1">
-        <v>28</v>
-      </c>
-      <c r="B29" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="C29" s="4">
-        <v>26</v>
-      </c>
+      <c r="A29" s="14"/>
+      <c r="B29" s="15"/>
+      <c r="C29" s="16"/>
     </row>
     <row r="30" spans="1:3">
-      <c r="A30" s="1">
-        <v>29</v>
-      </c>
-      <c r="B30" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="C30" s="4">
-        <v>27</v>
-      </c>
+      <c r="A30" s="14"/>
+      <c r="B30" s="15"/>
+      <c r="C30" s="16"/>
     </row>
     <row r="31" spans="1:3">
-      <c r="A31" s="1">
-        <v>30</v>
-      </c>
-      <c r="B31" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="C31" s="4">
-        <v>28</v>
-      </c>
+      <c r="A31" s="14"/>
+      <c r="B31" s="15"/>
+      <c r="C31" s="16"/>
     </row>
     <row r="32" spans="1:3">
-      <c r="A32" s="1">
-        <v>31</v>
-      </c>
-      <c r="B32" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="C32" s="4">
-        <v>29</v>
-      </c>
+      <c r="A32" s="14"/>
+      <c r="B32" s="15"/>
+      <c r="C32" s="16"/>
     </row>
     <row r="33" spans="1:3">
-      <c r="A33" s="1">
-        <v>32</v>
-      </c>
-      <c r="B33" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="C33" s="4">
-        <v>30</v>
-      </c>
+      <c r="A33" s="14"/>
+      <c r="B33" s="15"/>
+      <c r="C33" s="16"/>
     </row>
     <row r="34" spans="1:3">
-      <c r="A34" s="1">
-        <v>33</v>
-      </c>
-      <c r="B34" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="C34" s="4">
-        <v>31</v>
-      </c>
+      <c r="A34" s="14"/>
+      <c r="B34" s="15"/>
+      <c r="C34" s="16"/>
     </row>
     <row r="35" spans="1:3">
-      <c r="A35" s="1">
-        <v>34</v>
-      </c>
-      <c r="B35" s="5" t="s">
-        <v>112</v>
-      </c>
-      <c r="C35" s="4">
-        <v>32</v>
-      </c>
+      <c r="A35" s="14"/>
+      <c r="B35" s="15"/>
+      <c r="C35" s="16"/>
     </row>
     <row r="36" spans="1:3">
-      <c r="A36" s="1">
-        <v>35</v>
-      </c>
-      <c r="B36" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="C36" s="4">
-        <v>33</v>
-      </c>
+      <c r="A36" s="14"/>
+      <c r="B36" s="15"/>
+      <c r="C36" s="16"/>
     </row>
     <row r="37" spans="1:3">
-      <c r="A37" s="1">
-        <v>36</v>
-      </c>
-      <c r="B37" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="C37" s="4">
-        <v>34</v>
-      </c>
+      <c r="A37" s="14"/>
+      <c r="B37" s="15"/>
+      <c r="C37" s="16"/>
     </row>
     <row r="38" spans="1:3">
-      <c r="A38" s="1">
-        <v>37</v>
-      </c>
-      <c r="B38" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="C38" s="4">
-        <v>35</v>
-      </c>
+      <c r="A38" s="14"/>
+      <c r="B38" s="15"/>
+      <c r="C38" s="16"/>
     </row>
     <row r="39" spans="1:3">
-      <c r="A39" s="1">
-        <v>38</v>
-      </c>
-      <c r="B39" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="C39" s="4">
-        <v>36</v>
-      </c>
+      <c r="A39" s="14"/>
+      <c r="B39" s="15"/>
+      <c r="C39" s="16"/>
     </row>
     <row r="40" spans="1:3">
-      <c r="A40" s="1">
-        <v>39</v>
-      </c>
-      <c r="B40" s="5" t="s">
-        <v>117</v>
-      </c>
-      <c r="C40" s="4">
-        <v>37</v>
-      </c>
+      <c r="A40" s="14"/>
+      <c r="B40" s="15"/>
+      <c r="C40" s="16"/>
     </row>
     <row r="41" spans="1:3">
-      <c r="A41" s="1">
-        <v>40</v>
-      </c>
-      <c r="B41" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="C41" s="4">
-        <v>38</v>
-      </c>
+      <c r="A41" s="14"/>
+      <c r="B41" s="15"/>
+      <c r="C41" s="16"/>
     </row>
     <row r="42" spans="1:3">
-      <c r="A42" s="1">
-        <v>41</v>
-      </c>
-      <c r="B42" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="C42" s="4">
-        <v>39</v>
-      </c>
+      <c r="A42" s="14"/>
+      <c r="B42" s="15"/>
+      <c r="C42" s="16"/>
     </row>
     <row r="43" spans="1:3">
-      <c r="A43" s="1">
-        <v>42</v>
-      </c>
-      <c r="B43" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="C43" s="4">
-        <v>40</v>
-      </c>
+      <c r="A43" s="14"/>
+      <c r="B43" s="15"/>
+      <c r="C43" s="16"/>
     </row>
     <row r="44" spans="1:3">
-      <c r="A44" s="1">
-        <v>43</v>
-      </c>
-      <c r="B44" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="C44" s="4">
-        <v>41</v>
-      </c>
+      <c r="A44" s="14"/>
+      <c r="B44" s="15"/>
+      <c r="C44" s="16"/>
     </row>
     <row r="45" spans="1:3">
-      <c r="A45" s="1">
-        <v>44</v>
-      </c>
-      <c r="B45" s="5" t="s">
-        <v>122</v>
-      </c>
-      <c r="C45" s="4">
-        <v>42</v>
-      </c>
+      <c r="A45" s="14"/>
+      <c r="B45" s="15"/>
+      <c r="C45" s="16"/>
     </row>
     <row r="46" spans="1:3">
-      <c r="A46" s="1">
-        <v>45</v>
-      </c>
-      <c r="B46" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="C46" s="4">
-        <v>43</v>
-      </c>
+      <c r="A46" s="14"/>
+      <c r="B46" s="15"/>
+      <c r="C46" s="16"/>
     </row>
     <row r="47" spans="1:3">
-      <c r="A47" s="1">
-        <v>46</v>
-      </c>
-      <c r="B47" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="C47" s="4">
-        <v>44</v>
-      </c>
+      <c r="A47" s="14"/>
+      <c r="B47" s="15"/>
+      <c r="C47" s="16"/>
     </row>
     <row r="48" spans="1:3">
-      <c r="A48" s="1">
-        <v>47</v>
-      </c>
-      <c r="B48" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="C48" s="4">
-        <v>45</v>
-      </c>
+      <c r="A48" s="14"/>
+      <c r="B48" s="15"/>
+      <c r="C48" s="16"/>
     </row>
     <row r="49" spans="1:3">
-      <c r="A49" s="1">
-        <v>48</v>
-      </c>
-      <c r="B49" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="C49" s="4">
-        <v>46</v>
-      </c>
+      <c r="A49" s="14"/>
+      <c r="B49" s="15"/>
+      <c r="C49" s="16"/>
     </row>
     <row r="50" spans="1:3">
-      <c r="A50" s="1">
-        <v>49</v>
-      </c>
-      <c r="B50" s="5" t="s">
-        <v>127</v>
-      </c>
-      <c r="C50" s="4">
-        <v>47</v>
-      </c>
+      <c r="A50" s="14"/>
+      <c r="B50" s="15"/>
+      <c r="C50" s="16"/>
     </row>
     <row r="51" spans="1:3">
-      <c r="A51" s="1">
-        <v>50</v>
-      </c>
-      <c r="B51" s="5" t="s">
-        <v>128</v>
-      </c>
-      <c r="C51" s="4">
-        <v>48</v>
-      </c>
+      <c r="A51" s="14"/>
+      <c r="B51" s="15"/>
+      <c r="C51" s="16"/>
     </row>
     <row r="52" spans="1:3">
-      <c r="A52" s="1">
-        <v>51</v>
-      </c>
-      <c r="B52" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="C52" s="4">
-        <v>49</v>
-      </c>
+      <c r="A52" s="14"/>
+      <c r="B52" s="15"/>
+      <c r="C52" s="16"/>
     </row>
     <row r="53" spans="1:3">
-      <c r="A53" s="1">
-        <v>52</v>
-      </c>
-      <c r="B53" s="5" t="s">
-        <v>130</v>
-      </c>
-      <c r="C53" s="4">
-        <v>50</v>
-      </c>
+      <c r="A53" s="14"/>
+      <c r="B53" s="15"/>
+      <c r="C53" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3880,20 +3692,63 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9F1D321-262E-4B92-9ED1-453EAE798920}">
-  <dimension ref="A1:C6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{569C5A1C-8B83-4300-B484-9F77666745FD}">
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="2" max="2" width="20.90625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>222</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9F1D321-262E-4B92-9ED1-453EAE798920}">
+  <dimension ref="A1:D8"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="26" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>226</v>
       </c>
@@ -3903,8 +3758,11 @@
       <c r="C1" s="1" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
+      <c r="D1" s="12" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" s="1" t="s">
         <v>316</v>
       </c>
@@ -3914,8 +3772,11 @@
       <c r="C2" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:3">
+      <c r="D2" s="1" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" s="1" t="s">
         <v>315</v>
       </c>
@@ -3925,8 +3786,11 @@
       <c r="C3" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:3">
+      <c r="D3" s="1" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" s="1" t="s">
         <v>314</v>
       </c>
@@ -3936,19 +3800,25 @@
       <c r="C4" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:3">
+      <c r="D4" s="1" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5" s="1" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="B5" s="1">
         <v>1</v>
       </c>
       <c r="C5" s="1">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
+        <v>1</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
       <c r="A6" s="1" t="s">
         <v>314</v>
       </c>
@@ -3956,20 +3826,52 @@
         <v>2</v>
       </c>
       <c r="C6" s="1">
+        <v>1</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="B7" s="1">
+        <v>1</v>
+      </c>
+      <c r="C7" s="1">
         <v>25</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="B8" s="1">
+        <v>2</v>
+      </c>
+      <c r="C8" s="1">
+        <v>25</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>357</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6E05CD4-7C76-4891-A9C7-AB36831BB0B8}">
-  <dimension ref="A1:J18"/>
+  <dimension ref="A1:K18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -3985,7 +3887,7 @@
     <col min="10" max="10" width="10.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:11">
       <c r="A1" s="8" t="s">
         <v>131</v>
       </c>
@@ -4016,8 +3918,11 @@
       <c r="J1" s="8" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="2" spans="1:10">
+      <c r="K1" s="13" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
       <c r="A2" s="6">
         <v>1223</v>
       </c>
@@ -4046,8 +3951,11 @@
       <c r="J2" s="8">
         <v>110</v>
       </c>
-    </row>
-    <row r="3" spans="1:10">
+      <c r="K2" s="1" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
       <c r="A3" s="8">
         <v>1224</v>
       </c>
@@ -4076,8 +3984,11 @@
       <c r="J3" s="8">
         <v>410</v>
       </c>
-    </row>
-    <row r="4" spans="1:10">
+      <c r="K3" s="1" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
       <c r="A4" s="6">
         <v>1225</v>
       </c>
@@ -4106,8 +4017,11 @@
       <c r="J4" s="8">
         <v>230</v>
       </c>
-    </row>
-    <row r="5" spans="1:10">
+      <c r="K4" s="1" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
       <c r="A5" s="8">
         <v>1226</v>
       </c>
@@ -4136,8 +4050,11 @@
       <c r="J5" s="8">
         <v>230</v>
       </c>
-    </row>
-    <row r="6" spans="1:10">
+      <c r="K5" s="1" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
       <c r="A6" s="6">
         <v>1227</v>
       </c>
@@ -4166,8 +4083,11 @@
       <c r="J6" s="8">
         <v>230</v>
       </c>
-    </row>
-    <row r="7" spans="1:10">
+      <c r="K6" s="1" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
       <c r="A7" s="8">
         <v>1228</v>
       </c>
@@ -4196,8 +4116,11 @@
       <c r="J7" s="8">
         <v>230</v>
       </c>
-    </row>
-    <row r="8" spans="1:10">
+      <c r="K7" s="1" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
       <c r="A8" s="6">
         <v>1229</v>
       </c>
@@ -4226,8 +4149,11 @@
       <c r="J8" s="8">
         <v>230</v>
       </c>
-    </row>
-    <row r="9" spans="1:10">
+      <c r="K8" s="1" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
       <c r="A9" s="8">
         <v>1230</v>
       </c>
@@ -4256,8 +4182,11 @@
       <c r="J9" s="8">
         <v>230</v>
       </c>
-    </row>
-    <row r="10" spans="1:10">
+      <c r="K9" s="1" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
       <c r="A10" s="6">
         <v>1231</v>
       </c>
@@ -4286,8 +4215,11 @@
       <c r="J10" s="8">
         <v>230</v>
       </c>
-    </row>
-    <row r="11" spans="1:10">
+      <c r="K10" s="1" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
       <c r="A11" s="8">
         <v>1232</v>
       </c>
@@ -4316,8 +4248,11 @@
       <c r="J11" s="8">
         <v>110</v>
       </c>
-    </row>
-    <row r="12" spans="1:10">
+      <c r="K11" s="1" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
       <c r="A12" s="8">
         <v>1233</v>
       </c>
@@ -4346,8 +4281,11 @@
       <c r="J12" s="8">
         <v>350</v>
       </c>
-    </row>
-    <row r="13" spans="1:10">
+      <c r="K12" s="1" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11">
       <c r="A13" s="8">
         <v>1234</v>
       </c>
@@ -4376,8 +4314,11 @@
       <c r="J13" s="8">
         <v>110</v>
       </c>
-    </row>
-    <row r="14" spans="1:10">
+      <c r="K13" s="1" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11">
       <c r="A14" s="8">
         <v>1235</v>
       </c>
@@ -4406,8 +4347,11 @@
       <c r="J14" s="8">
         <v>230</v>
       </c>
-    </row>
-    <row r="15" spans="1:10">
+      <c r="K14" s="1" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11">
       <c r="A15" s="8">
         <v>1236</v>
       </c>
@@ -4436,8 +4380,11 @@
       <c r="J15" s="8">
         <v>240</v>
       </c>
-    </row>
-    <row r="16" spans="1:10">
+      <c r="K15" s="1" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11">
       <c r="A16" s="8">
         <v>1237</v>
       </c>
@@ -4466,8 +4413,11 @@
       <c r="J16" s="8">
         <v>110</v>
       </c>
-    </row>
-    <row r="17" spans="1:10">
+      <c r="K16" s="1" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11">
       <c r="A17" s="8">
         <v>1238</v>
       </c>
@@ -4496,8 +4446,11 @@
       <c r="J17" s="1">
         <v>240</v>
       </c>
-    </row>
-    <row r="18" spans="1:10">
+      <c r="K17" s="1" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11">
       <c r="A18" s="8">
         <v>1239</v>
       </c>
@@ -4525,6 +4478,9 @@
       </c>
       <c r="J18" s="1">
         <v>240</v>
+      </c>
+      <c r="K18" s="1" t="s">
+        <v>357</v>
       </c>
     </row>
   </sheetData>
@@ -4540,7 +4496,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7DF7A36-0BE1-4085-9FD3-20961A4A2C2E}">
   <dimension ref="A1:B6"/>
   <sheetViews>
@@ -4607,12 +4563,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{491D14EC-1CB1-4681-930A-4B9B4015FC83}">
-  <dimension ref="A1:Q35"/>
+  <dimension ref="A1:S35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I11" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="P18" sqref="P18"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="R2" sqref="R2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -4636,7 +4592,7 @@
     <col min="17" max="17" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17">
+    <row r="1" spans="1:19">
       <c r="A1" s="1" t="s">
         <v>210</v>
       </c>
@@ -4688,8 +4644,14 @@
       <c r="Q1" s="1" t="s">
         <v>308</v>
       </c>
-    </row>
-    <row r="2" spans="1:17">
+      <c r="R1" s="12" t="s">
+        <v>361</v>
+      </c>
+      <c r="S1" s="12" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19">
       <c r="A2" s="1" t="s">
         <v>174</v>
       </c>
@@ -4734,11 +4696,15 @@
       <c r="P2" s="2">
         <v>1223</v>
       </c>
-      <c r="Q2" s="1">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17">
+      <c r="Q2" s="1"/>
+      <c r="R2" s="12">
+        <v>1</v>
+      </c>
+      <c r="S2" s="12">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19">
       <c r="A3" s="1" t="s">
         <v>181</v>
       </c>
@@ -4786,8 +4752,12 @@
       <c r="Q3" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:17">
+      <c r="R3" s="1"/>
+      <c r="S3" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19">
       <c r="A4" s="1" t="s">
         <v>184</v>
       </c>
@@ -4835,8 +4805,12 @@
       <c r="Q4" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:17">
+      <c r="R4" s="1"/>
+      <c r="S4" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19">
       <c r="A5" s="1" t="s">
         <v>249</v>
       </c>
@@ -4884,8 +4858,12 @@
       <c r="Q5" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:17">
+      <c r="R5" s="1"/>
+      <c r="S5" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19">
       <c r="A6" s="1" t="s">
         <v>263</v>
       </c>
@@ -4933,8 +4911,12 @@
       <c r="Q6" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="7" spans="1:17">
+      <c r="R6" s="1"/>
+      <c r="S6" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19">
       <c r="A7" s="1" t="s">
         <v>187</v>
       </c>
@@ -4982,8 +4964,12 @@
       <c r="Q7" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="8" spans="1:17">
+      <c r="R7" s="1"/>
+      <c r="S7" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19">
       <c r="A8" s="1" t="s">
         <v>188</v>
       </c>
@@ -5028,11 +5014,15 @@
       <c r="P8" s="2">
         <v>1232</v>
       </c>
-      <c r="Q8" s="1">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17">
+      <c r="Q8" s="1"/>
+      <c r="R8" s="12">
+        <v>1</v>
+      </c>
+      <c r="S8" s="12">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19">
       <c r="A9" s="1" t="s">
         <v>192</v>
       </c>
@@ -5077,11 +5067,15 @@
       <c r="P9" s="1">
         <v>1238</v>
       </c>
-      <c r="Q9" s="1">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17">
+      <c r="Q9" s="1"/>
+      <c r="R9" s="12">
+        <v>2</v>
+      </c>
+      <c r="S9" s="12">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19">
       <c r="A10" s="1" t="s">
         <v>257</v>
       </c>
@@ -5126,11 +5120,15 @@
       <c r="P10" s="2">
         <v>1239</v>
       </c>
-      <c r="Q10" s="1">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17">
+      <c r="Q10" s="1"/>
+      <c r="R10" s="12">
+        <v>2</v>
+      </c>
+      <c r="S10" s="12">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19">
       <c r="A11" s="1" t="s">
         <v>258</v>
       </c>
@@ -5175,11 +5173,15 @@
       <c r="P11" s="1">
         <v>1223</v>
       </c>
-      <c r="Q11" s="1">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17">
+      <c r="Q11" s="1"/>
+      <c r="R11" s="12">
+        <v>1</v>
+      </c>
+      <c r="S11" s="12">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19">
       <c r="A12" s="1" t="s">
         <v>259</v>
       </c>
@@ -5224,11 +5226,15 @@
       <c r="P12" s="2">
         <v>1232</v>
       </c>
-      <c r="Q12" s="1">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17">
+      <c r="Q12" s="1"/>
+      <c r="R12" s="12">
+        <v>1</v>
+      </c>
+      <c r="S12" s="12">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19">
       <c r="A13" s="1" t="s">
         <v>197</v>
       </c>
@@ -5276,8 +5282,12 @@
       <c r="Q13" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:17">
+      <c r="R13" s="1"/>
+      <c r="S13" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19">
       <c r="A14" s="1" t="s">
         <v>201</v>
       </c>
@@ -5325,8 +5335,12 @@
       <c r="Q14" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:17">
+      <c r="R14" s="1"/>
+      <c r="S14" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19">
       <c r="A15" s="1" t="s">
         <v>202</v>
       </c>
@@ -5374,8 +5388,12 @@
       <c r="Q15" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:17">
+      <c r="R15" s="1"/>
+      <c r="S15" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19">
       <c r="A16" s="1" t="s">
         <v>204</v>
       </c>
@@ -5423,8 +5441,12 @@
       <c r="Q16" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:17">
+      <c r="R16" s="1"/>
+      <c r="S16" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19">
       <c r="A17" s="1" t="s">
         <v>207</v>
       </c>
@@ -5472,8 +5494,12 @@
       <c r="Q17" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:17">
+      <c r="R17" s="1"/>
+      <c r="S17" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19">
       <c r="A18" s="1" t="s">
         <v>208</v>
       </c>
@@ -5523,8 +5549,12 @@
       <c r="Q18" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:17">
+      <c r="R18" s="1"/>
+      <c r="S18" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19">
       <c r="A19" s="1" t="s">
         <v>252</v>
       </c>
@@ -5574,8 +5604,12 @@
       <c r="Q19" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:17">
+      <c r="R19" s="1"/>
+      <c r="S19" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19">
       <c r="A20" s="1" t="s">
         <v>253</v>
       </c>
@@ -5623,8 +5657,12 @@
       <c r="Q20" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="21" spans="1:17">
+      <c r="R20" s="1"/>
+      <c r="S20" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19">
       <c r="A21" s="1" t="s">
         <v>254</v>
       </c>
@@ -5672,8 +5710,12 @@
       <c r="Q21" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="22" spans="1:17">
+      <c r="R21" s="1"/>
+      <c r="S21" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19">
       <c r="A22" s="1" t="s">
         <v>255</v>
       </c>
@@ -5721,8 +5763,12 @@
       <c r="Q22" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="23" spans="1:17">
+      <c r="R22" s="1"/>
+      <c r="S22" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19">
       <c r="A23" s="1" t="s">
         <v>256</v>
       </c>
@@ -5770,8 +5816,12 @@
       <c r="Q23" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="24" spans="1:17">
+      <c r="R23" s="1"/>
+      <c r="S23" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19">
       <c r="A24" s="1" t="s">
         <v>279</v>
       </c>
@@ -5816,11 +5866,15 @@
       <c r="P24" s="1">
         <v>1</v>
       </c>
-      <c r="Q24" s="1">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="25" spans="1:17">
+      <c r="Q24" s="1"/>
+      <c r="R24" s="12">
+        <v>1</v>
+      </c>
+      <c r="S24" s="12">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19">
       <c r="A25" s="1" t="s">
         <v>280</v>
       </c>
@@ -5865,11 +5919,15 @@
       <c r="P25" s="1">
         <v>1238</v>
       </c>
-      <c r="Q25" s="1">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="26" spans="1:17">
+      <c r="Q25" s="1"/>
+      <c r="R25" s="12">
+        <v>2</v>
+      </c>
+      <c r="S25" s="12">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19">
       <c r="A26" s="1" t="s">
         <v>281</v>
       </c>
@@ -5914,11 +5972,15 @@
       <c r="P26" s="1">
         <v>1236</v>
       </c>
-      <c r="Q26" s="1">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="27" spans="1:17">
+      <c r="Q26" s="1"/>
+      <c r="R26" s="12">
+        <v>2</v>
+      </c>
+      <c r="S26" s="12">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19">
       <c r="A27" s="1" t="s">
         <v>282</v>
       </c>
@@ -5963,11 +6025,15 @@
       <c r="P27" s="1">
         <v>1</v>
       </c>
-      <c r="Q27" s="1">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="28" spans="1:17">
+      <c r="Q27" s="1"/>
+      <c r="R27" s="12">
+        <v>1</v>
+      </c>
+      <c r="S27" s="12">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19">
       <c r="A28" s="1" t="s">
         <v>290</v>
       </c>
@@ -6012,11 +6078,13 @@
       <c r="P28" s="2">
         <v>1225</v>
       </c>
-      <c r="Q28" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="29" spans="1:17">
+      <c r="Q28" s="1"/>
+      <c r="R28" s="1"/>
+      <c r="S28" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19">
       <c r="A29" s="1" t="s">
         <v>291</v>
       </c>
@@ -6061,11 +6129,13 @@
       <c r="P29" s="1">
         <v>1226</v>
       </c>
-      <c r="Q29" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="30" spans="1:17">
+      <c r="Q29" s="1"/>
+      <c r="R29" s="1"/>
+      <c r="S29" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19">
       <c r="A30" s="1" t="s">
         <v>292</v>
       </c>
@@ -6110,11 +6180,13 @@
       <c r="P30" s="2">
         <v>1227</v>
       </c>
-      <c r="Q30" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="31" spans="1:17">
+      <c r="Q30" s="1"/>
+      <c r="R30" s="1"/>
+      <c r="S30" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19">
       <c r="A31" s="1" t="s">
         <v>293</v>
       </c>
@@ -6159,11 +6231,13 @@
       <c r="P31" s="2">
         <v>1</v>
       </c>
-      <c r="Q31" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="32" spans="1:17">
+      <c r="Q31" s="1"/>
+      <c r="R31" s="1"/>
+      <c r="S31" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:19">
       <c r="A32" s="1" t="s">
         <v>294</v>
       </c>
@@ -6208,11 +6282,13 @@
       <c r="P32" s="1">
         <v>1</v>
       </c>
-      <c r="Q32" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="33" spans="1:17">
+      <c r="Q32" s="1"/>
+      <c r="R32" s="1"/>
+      <c r="S32" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:19">
       <c r="A33" s="1" t="s">
         <v>295</v>
       </c>
@@ -6257,11 +6333,13 @@
       <c r="P33" s="2">
         <v>1</v>
       </c>
-      <c r="Q33" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="34" spans="1:17">
+      <c r="Q33" s="1"/>
+      <c r="R33" s="1"/>
+      <c r="S33" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:19">
       <c r="A34" s="1" t="s">
         <v>282</v>
       </c>
@@ -6306,11 +6384,13 @@
       <c r="P34" s="1">
         <v>1</v>
       </c>
-      <c r="Q34" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="35" spans="1:17">
+      <c r="Q34" s="1"/>
+      <c r="R34" s="1"/>
+      <c r="S34" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:19">
       <c r="A35" s="1" t="s">
         <v>296</v>
       </c>
@@ -6355,88 +6435,14 @@
       <c r="P35" s="2">
         <v>1</v>
       </c>
-      <c r="Q35" s="1">
-        <v>3</v>
+      <c r="Q35" s="1"/>
+      <c r="R35" s="1"/>
+      <c r="S35" s="12">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28F0C749-0F7B-4353-B0A5-2957163B7B34}">
-  <dimension ref="A1:B7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
-  <cols>
-    <col min="1" max="1" width="23.36328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="38.08984375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>343</v>
-      </c>
-    </row>
-  </sheetData>
-  <autoFilter ref="A1:A7" xr:uid="{28F0C749-0F7B-4353-B0A5-2957163B7B34}"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>